<commit_message>
changes to predictions, marginals
</commit_message>
<xml_diff>
--- a/csvs/collated-tt-election-results.xlsx
+++ b/csvs/collated-tt-election-results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophegittens/Desktop/my docs/U.W.I. YEAR 4/U.W.I. YEAR 4 - SEMESTER II/COMP 3610/Assignments/Election-Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophegittens/Desktop/my docs/U.W.I. YEAR 4/U.W.I. YEAR 4 - SEMESTER II/COMP 3610/Assignments/Election-Project/csvs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39EC8BDB-FDD5-874D-9D7F-ED23475BA844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55454404-E5A5-B54A-8CE2-ED8FCBF3F5E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00CD0EB4-DA0B-AB45-875C-9354388CE2C5}"/>
   </bookViews>
@@ -632,6 +632,7 @@
     <xf numFmtId="10" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -644,7 +645,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -984,7 +984,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="B19" sqref="B19"/>
+      <selection pane="topRight" activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1003,45 +1003,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
       <c r="R1"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
-      <c r="O2" s="36"/>
-      <c r="P2" s="36"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
       <c r="R2"/>
     </row>
     <row r="3" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -1064,30 +1064,30 @@
       <c r="F4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35" t="s">
+      <c r="H4" s="36"/>
+      <c r="I4" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35" t="s">
+      <c r="J4" s="36"/>
+      <c r="K4" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="35"/>
-      <c r="M4" s="37" t="s">
+      <c r="L4" s="36"/>
+      <c r="M4" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="N4" s="38"/>
-      <c r="O4" s="35" t="s">
+      <c r="N4" s="39"/>
+      <c r="O4" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="P4" s="35"/>
-      <c r="Q4" s="35" t="s">
+      <c r="P4" s="36"/>
+      <c r="Q4" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="R4" s="35"/>
+      <c r="R4" s="36"/>
     </row>
     <row r="5" spans="1:18" s="1" customFormat="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
@@ -1180,7 +1180,7 @@
       </c>
     </row>
     <row r="7" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="35" t="s">
         <v>56</v>
       </c>
       <c r="B7" s="19">
@@ -1235,7 +1235,7 @@
       </c>
     </row>
     <row r="8" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="35" t="s">
         <v>57</v>
       </c>
       <c r="B8" s="19">
@@ -1285,7 +1285,7 @@
       <c r="R8" s="10"/>
     </row>
     <row r="9" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="35" t="s">
         <v>58</v>
       </c>
       <c r="B9" s="19">
@@ -1335,7 +1335,7 @@
       <c r="R9" s="10"/>
     </row>
     <row r="10" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="35" t="s">
         <v>59</v>
       </c>
       <c r="B10" s="19">
@@ -1385,7 +1385,7 @@
       <c r="R10" s="10"/>
     </row>
     <row r="11" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="35" t="s">
         <v>60</v>
       </c>
       <c r="B11" s="19">
@@ -1435,7 +1435,7 @@
       <c r="R11" s="10"/>
     </row>
     <row r="12" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="35" t="s">
         <v>61</v>
       </c>
       <c r="B12" s="19">
@@ -1485,7 +1485,7 @@
       <c r="R12" s="10"/>
     </row>
     <row r="13" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="35" t="s">
         <v>62</v>
       </c>
       <c r="B13" s="19">
@@ -1535,7 +1535,7 @@
       <c r="R13" s="10"/>
     </row>
     <row r="14" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="35" t="s">
         <v>63</v>
       </c>
       <c r="B14" s="19">
@@ -1585,7 +1585,7 @@
       <c r="R14" s="10"/>
     </row>
     <row r="15" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="35" t="s">
         <v>64</v>
       </c>
       <c r="B15" s="19">
@@ -1635,7 +1635,7 @@
       <c r="R15" s="10"/>
     </row>
     <row r="16" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="35" t="s">
         <v>65</v>
       </c>
       <c r="B16" s="19">
@@ -1685,7 +1685,7 @@
       <c r="R16" s="10"/>
     </row>
     <row r="17" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="35" t="s">
         <v>66</v>
       </c>
       <c r="B17" s="19">
@@ -1740,7 +1740,7 @@
       </c>
     </row>
     <row r="18" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="35" t="s">
         <v>67</v>
       </c>
       <c r="B18" s="19">
@@ -1790,7 +1790,7 @@
       <c r="R18" s="10"/>
     </row>
     <row r="19" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="39" t="s">
+      <c r="A19" s="35" t="s">
         <v>68</v>
       </c>
       <c r="B19" s="19">
@@ -1840,7 +1840,7 @@
       <c r="R19" s="10"/>
     </row>
     <row r="20" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="39" t="s">
+      <c r="A20" s="35" t="s">
         <v>69</v>
       </c>
       <c r="B20" s="19">
@@ -1890,7 +1890,7 @@
       <c r="R20" s="10"/>
     </row>
     <row r="21" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="35" t="s">
         <v>70</v>
       </c>
       <c r="B21" s="19">
@@ -1940,7 +1940,7 @@
       <c r="R21" s="10"/>
     </row>
     <row r="22" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="35" t="s">
         <v>71</v>
       </c>
       <c r="B22" s="19">
@@ -1990,7 +1990,7 @@
       <c r="R22" s="10"/>
     </row>
     <row r="23" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="35" t="s">
         <v>72</v>
       </c>
       <c r="B23" s="19">
@@ -2040,7 +2040,7 @@
       <c r="R23" s="10"/>
     </row>
     <row r="24" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="39" t="s">
+      <c r="A24" s="35" t="s">
         <v>73</v>
       </c>
       <c r="B24" s="19">
@@ -2090,7 +2090,7 @@
       <c r="R24" s="10"/>
     </row>
     <row r="25" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="39" t="s">
+      <c r="A25" s="35" t="s">
         <v>74</v>
       </c>
       <c r="B25" s="19">
@@ -2140,7 +2140,7 @@
       <c r="R25" s="10"/>
     </row>
     <row r="26" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="39" t="s">
+      <c r="A26" s="35" t="s">
         <v>75</v>
       </c>
       <c r="B26" s="19">
@@ -2190,7 +2190,7 @@
       <c r="R26" s="10"/>
     </row>
     <row r="27" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="39" t="s">
+      <c r="A27" s="35" t="s">
         <v>76</v>
       </c>
       <c r="B27" s="19">
@@ -2240,7 +2240,7 @@
       <c r="R27" s="10"/>
     </row>
     <row r="28" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="39" t="s">
+      <c r="A28" s="35" t="s">
         <v>77</v>
       </c>
       <c r="B28" s="19">
@@ -2290,7 +2290,7 @@
       <c r="R28" s="10"/>
     </row>
     <row r="29" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="35" t="s">
         <v>78</v>
       </c>
       <c r="B29" s="19">
@@ -2340,7 +2340,7 @@
       <c r="R29" s="10"/>
     </row>
     <row r="30" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="35" t="s">
         <v>79</v>
       </c>
       <c r="B30" s="19">
@@ -2390,7 +2390,7 @@
       <c r="R30" s="10"/>
     </row>
     <row r="31" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="39" t="s">
+      <c r="A31" s="35" t="s">
         <v>80</v>
       </c>
       <c r="B31" s="19">
@@ -2440,7 +2440,7 @@
       <c r="R31" s="10"/>
     </row>
     <row r="32" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="39" t="s">
+      <c r="A32" s="35" t="s">
         <v>81</v>
       </c>
       <c r="B32" s="19">
@@ -2490,7 +2490,7 @@
       <c r="R32" s="10"/>
     </row>
     <row r="33" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="39" t="s">
+      <c r="A33" s="35" t="s">
         <v>82</v>
       </c>
       <c r="B33" s="19">
@@ -2540,7 +2540,7 @@
       <c r="R33" s="10"/>
     </row>
     <row r="34" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="39" t="s">
+      <c r="A34" s="35" t="s">
         <v>83</v>
       </c>
       <c r="B34" s="19">
@@ -2590,7 +2590,7 @@
       <c r="R34" s="10"/>
     </row>
     <row r="35" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="39" t="s">
+      <c r="A35" s="35" t="s">
         <v>84</v>
       </c>
       <c r="B35" s="19">
@@ -2645,7 +2645,7 @@
       </c>
     </row>
     <row r="36" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="39" t="s">
+      <c r="A36" s="35" t="s">
         <v>85</v>
       </c>
       <c r="B36" s="19">
@@ -2695,7 +2695,7 @@
       <c r="R36" s="10"/>
     </row>
     <row r="37" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="39" t="s">
+      <c r="A37" s="35" t="s">
         <v>86</v>
       </c>
       <c r="B37" s="19">
@@ -2745,7 +2745,7 @@
       <c r="R37" s="10"/>
     </row>
     <row r="38" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="39" t="s">
+      <c r="A38" s="35" t="s">
         <v>87</v>
       </c>
       <c r="B38" s="19">
@@ -2795,7 +2795,7 @@
       <c r="R38" s="10"/>
     </row>
     <row r="39" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="39" t="s">
+      <c r="A39" s="35" t="s">
         <v>88</v>
       </c>
       <c r="B39" s="19">
@@ -2845,7 +2845,7 @@
       <c r="R39" s="10"/>
     </row>
     <row r="40" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="39" t="s">
+      <c r="A40" s="35" t="s">
         <v>89</v>
       </c>
       <c r="B40" s="19">
@@ -2895,7 +2895,7 @@
       <c r="R40" s="10"/>
     </row>
     <row r="41" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="39" t="s">
+      <c r="A41" s="35" t="s">
         <v>90</v>
       </c>
       <c r="B41" s="19">
@@ -2945,7 +2945,7 @@
       <c r="R41" s="10"/>
     </row>
     <row r="42" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="35" t="s">
         <v>91</v>
       </c>
       <c r="B42" s="19">
@@ -2995,7 +2995,7 @@
       <c r="R42" s="10"/>
     </row>
     <row r="43" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="39" t="s">
+      <c r="A43" s="35" t="s">
         <v>92</v>
       </c>
       <c r="B43" s="19">
@@ -3045,7 +3045,7 @@
       <c r="R43" s="10"/>
     </row>
     <row r="44" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="39" t="s">
+      <c r="A44" s="35" t="s">
         <v>93</v>
       </c>
       <c r="B44" s="19">
@@ -3053,59 +3053,64 @@
       </c>
       <c r="C44" s="18">
         <f>SUM(E44,F44)</f>
-        <v>10880</v>
+        <v>15583</v>
       </c>
       <c r="D44" s="10">
         <f t="shared" si="5"/>
-        <v>0.56314699792960665</v>
+        <v>0.80657349896480335</v>
       </c>
       <c r="E44" s="22">
         <v>67</v>
       </c>
       <c r="F44" s="9">
         <f>SUM(G44,I44,K44,,M44,O44,Q44)</f>
-        <v>10813</v>
+        <v>15516</v>
       </c>
       <c r="G44" s="19">
         <v>5684</v>
       </c>
       <c r="H44" s="10">
         <f t="shared" si="6"/>
-        <v>0.52566355313049107</v>
-      </c>
-      <c r="I44" s="21"/>
-      <c r="J44" s="10"/>
+        <v>0.36633152874452179</v>
+      </c>
+      <c r="I44" s="21">
+        <v>4703</v>
+      </c>
+      <c r="J44" s="10">
+        <f>SUM(I44/B44)</f>
+        <v>0.2434265010351967</v>
+      </c>
       <c r="K44" s="21">
         <v>237</v>
       </c>
       <c r="L44" s="10">
         <f t="shared" si="3"/>
-        <v>2.1918061592527512E-2</v>
+        <v>1.5274555297757154E-2</v>
       </c>
       <c r="M44" s="21">
         <v>4703</v>
       </c>
       <c r="N44" s="10">
         <f>SUM(M44/F44)</f>
-        <v>0.43493942476648478</v>
+        <v>0.3031064707398814</v>
       </c>
       <c r="O44" s="21">
         <v>148</v>
       </c>
       <c r="P44" s="10">
         <f>SUM(O44/F44)</f>
-        <v>1.3687228336261906E-2</v>
+        <v>9.5385408610466609E-3</v>
       </c>
       <c r="Q44" s="21">
         <v>41</v>
       </c>
       <c r="R44" s="10">
         <f t="shared" si="7"/>
-        <v>3.7917321742347173E-3</v>
+        <v>2.6424336169115752E-3</v>
       </c>
     </row>
     <row r="45" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="39" t="s">
+      <c r="A45" s="35" t="s">
         <v>94</v>
       </c>
       <c r="B45" s="19">
@@ -3113,54 +3118,59 @@
       </c>
       <c r="C45" s="18">
         <f t="shared" si="4"/>
-        <v>11756</v>
+        <v>15932</v>
       </c>
       <c r="D45" s="10">
         <f t="shared" si="5"/>
-        <v>0.53592268417213718</v>
+        <v>0.72629467541940185</v>
       </c>
       <c r="E45" s="22">
         <v>29</v>
       </c>
       <c r="F45" s="9">
         <f t="shared" si="2"/>
-        <v>11727</v>
+        <v>15903</v>
       </c>
       <c r="G45" s="19">
         <v>6850</v>
       </c>
       <c r="H45" s="10">
         <f>SUM(G45/F45)</f>
-        <v>0.58412211136693104</v>
-      </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="10"/>
+        <v>0.43073633905552411</v>
+      </c>
+      <c r="I45" s="21">
+        <v>4176</v>
+      </c>
+      <c r="J45" s="10">
+        <f>SUM(I45/B45)</f>
+        <v>0.19037199124726478</v>
+      </c>
       <c r="K45" s="21">
         <v>471</v>
       </c>
       <c r="L45" s="10">
         <f t="shared" si="3"/>
-        <v>4.0163724737784602E-2</v>
+        <v>2.9617053386153554E-2</v>
       </c>
       <c r="M45" s="21">
         <v>4176</v>
       </c>
       <c r="N45" s="10">
         <f>SUM(M45/F45)</f>
-        <v>0.35610130468150419</v>
+        <v>0.26259196378041877</v>
       </c>
       <c r="O45" s="21">
         <v>230</v>
       </c>
       <c r="P45" s="10">
         <f>SUM(O45/F45)</f>
-        <v>1.9612859213780167E-2</v>
+        <v>1.4462679997484752E-2</v>
       </c>
       <c r="Q45" s="21"/>
       <c r="R45" s="10"/>
     </row>
     <row r="46" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="39" t="s">
+      <c r="A46" s="35" t="s">
         <v>95</v>
       </c>
       <c r="B46" s="19">
@@ -3210,7 +3220,7 @@
       <c r="R46" s="10"/>
     </row>
     <row r="47" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="39" t="s">
+      <c r="A47" s="35" t="s">
         <v>96</v>
       </c>
       <c r="B47" s="19">
@@ -3269,11 +3279,11 @@
       </c>
       <c r="C48" s="14">
         <f>SUM(C7:C47)</f>
-        <v>655845</v>
+        <v>664724</v>
       </c>
       <c r="D48" s="15">
         <f>SUM(C48/B48)</f>
-        <v>0.66215734597921994</v>
+        <v>0.67112180415904821</v>
       </c>
       <c r="E48" s="16">
         <f>SUM(E7:E47)</f>
@@ -3281,7 +3291,7 @@
       </c>
       <c r="F48" s="14">
         <f>SUM(F7:F47)</f>
-        <v>653245</v>
+        <v>662124</v>
       </c>
       <c r="G48" s="14">
         <f>SUM(G7:G47)</f>
@@ -3289,15 +3299,15 @@
       </c>
       <c r="H48" s="15">
         <f>SUM(G48/F48)</f>
-        <v>0.45991014091190902</v>
+        <v>0.4537428034627955</v>
       </c>
       <c r="I48" s="14">
         <f>SUM(I7:I47)</f>
-        <v>194968</v>
+        <v>203847</v>
       </c>
       <c r="J48" s="15">
         <f>SUM(I48/F48)</f>
-        <v>0.29846076127639709</v>
+        <v>0.30786831469634085</v>
       </c>
       <c r="K48" s="14">
         <f>SUM(K7:K47)</f>
@@ -3305,7 +3315,7 @@
       </c>
       <c r="L48" s="15">
         <f>SUM(K48/F48)</f>
-        <v>0.22708937688003736</v>
+        <v>0.22404413674779949</v>
       </c>
       <c r="M48" s="14">
         <f>SUM(M7:M47)</f>
@@ -3313,7 +3323,7 @@
       </c>
       <c r="N48" s="15">
         <f>SUM(M48/F48)</f>
-        <v>1.3592143835773715E-2</v>
+        <v>1.3409874887483311E-2</v>
       </c>
       <c r="O48" s="14">
         <f>SUM(O7:O47)</f>
@@ -3321,7 +3331,7 @@
       </c>
       <c r="P48" s="15">
         <f>SUM(O48/F48)</f>
-        <v>5.7864966436788642E-4</v>
+        <v>5.7089004476502893E-4</v>
       </c>
       <c r="Q48" s="14">
         <f>SUM(Q7:Q47)</f>
@@ -3329,7 +3339,7 @@
       </c>
       <c r="R48" s="15">
         <f>SUM(Q48/F48)</f>
-        <v>3.6892743151497524E-4</v>
+        <v>3.6398016081579885E-4</v>
       </c>
     </row>
     <row r="51" spans="4:4" x14ac:dyDescent="0.2">
@@ -3413,8 +3423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D39057C-680C-4843-89F6-29B9284CAFAA}">
   <dimension ref="A1:V74"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:A47"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K50" sqref="K50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3424,7 +3434,7 @@
     <col min="3" max="3" width="14.33203125" customWidth="1"/>
     <col min="4" max="4" width="11.1640625" style="2" customWidth="1"/>
     <col min="8" max="8" width="8.83203125" style="2"/>
-    <col min="10" max="10" width="8.83203125" style="2"/>
+    <col min="10" max="10" width="11.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.83203125" style="2"/>
     <col min="14" max="14" width="8.83203125" style="2"/>
     <col min="15" max="15" width="9.33203125" style="2" customWidth="1"/>
@@ -3433,48 +3443,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
-      <c r="O2" s="36"/>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="36"/>
-      <c r="R2" s="36"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="37"/>
     </row>
     <row r="3" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:22" s="1" customFormat="1" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3496,38 +3506,38 @@
       <c r="F4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35" t="s">
+      <c r="H4" s="36"/>
+      <c r="I4" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35" t="s">
+      <c r="J4" s="36"/>
+      <c r="K4" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35" t="s">
+      <c r="L4" s="36"/>
+      <c r="M4" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="N4" s="35"/>
-      <c r="O4" s="37" t="s">
+      <c r="N4" s="36"/>
+      <c r="O4" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="P4" s="38"/>
-      <c r="Q4" s="35" t="s">
+      <c r="P4" s="39"/>
+      <c r="Q4" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="R4" s="35"/>
-      <c r="S4" s="35" t="s">
+      <c r="R4" s="36"/>
+      <c r="S4" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="T4" s="35"/>
-      <c r="U4" s="35" t="s">
+      <c r="T4" s="36"/>
+      <c r="U4" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="V4" s="35"/>
+      <c r="V4" s="36"/>
     </row>
     <row r="5" spans="1:22" s="1" customFormat="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
@@ -3640,7 +3650,7 @@
       </c>
     </row>
     <row r="7" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="35" t="s">
         <v>56</v>
       </c>
       <c r="B7" s="9">
@@ -3648,41 +3658,46 @@
       </c>
       <c r="C7" s="9">
         <f>SUM(E7,F7)</f>
-        <v>15130</v>
+        <v>22740</v>
       </c>
       <c r="D7" s="10">
         <f>SUM(C7/B7)</f>
-        <v>0.62741032552353304</v>
+        <v>0.94298154675513168</v>
       </c>
       <c r="E7" s="11">
         <v>73</v>
       </c>
       <c r="F7" s="9">
         <f>SUM(G7,I7,K7,M7,O7,Q7,S7,U7)</f>
-        <v>15057</v>
+        <v>22667</v>
       </c>
       <c r="G7" s="9">
         <v>7246</v>
       </c>
       <c r="H7" s="10">
         <f t="shared" ref="H7" si="0">SUM(G7/F7)</f>
-        <v>0.4812379624095105</v>
-      </c>
-      <c r="I7" s="11"/>
-      <c r="J7" s="10"/>
+        <v>0.31967176953280096</v>
+      </c>
+      <c r="I7" s="9">
+        <v>7610</v>
+      </c>
+      <c r="J7" s="10">
+        <f t="shared" ref="J7:J47" si="1">SUM(I7/F7)</f>
+        <v>0.33573035690651609</v>
+      </c>
       <c r="K7" s="9">
         <v>7610</v>
       </c>
       <c r="L7" s="10">
-        <f t="shared" ref="L7:L47" si="1">SUM(K7/F7)</f>
-        <v>0.50541276482699082</v>
+        <f t="shared" ref="L7:L47" si="2">SUM(K7/F7)</f>
+        <v>0.33573035690651609</v>
       </c>
       <c r="M7" s="11">
         <v>201</v>
       </c>
       <c r="N7" s="10">
         <f>SUM(M7/F7)</f>
-        <v>1.3349272763498704E-2</v>
+        <v>8.8675166541668498E-3</v>
       </c>
       <c r="O7" s="10"/>
       <c r="P7" s="10"/>
@@ -3694,42 +3709,47 @@
       <c r="V7" s="10"/>
     </row>
     <row r="8" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="35" t="s">
         <v>57</v>
       </c>
       <c r="B8" s="9">
         <v>25019</v>
       </c>
       <c r="C8" s="9">
-        <f t="shared" ref="C8:C47" si="2">SUM(E8,F8)</f>
-        <v>17196</v>
+        <f t="shared" ref="C8:C47" si="3">SUM(E8,F8)</f>
+        <v>22716</v>
       </c>
       <c r="D8" s="10">
         <f>SUM(C8/B8)</f>
-        <v>0.6873176385946681</v>
+        <v>0.90794995803189571</v>
       </c>
       <c r="E8" s="11">
         <v>46</v>
       </c>
       <c r="F8" s="9">
-        <f t="shared" ref="F8:F47" si="3">SUM(G8,I8,K8,M8,O8,Q8,S8,U8)</f>
-        <v>17150</v>
+        <f t="shared" ref="F8:F47" si="4">SUM(G8,I8,K8,M8,O8,Q8,S8,U8)</f>
+        <v>22670</v>
       </c>
       <c r="G8" s="9">
         <v>11517</v>
       </c>
       <c r="H8" s="10">
         <f>SUM(G8/F8)</f>
-        <v>0.67154518950437314</v>
-      </c>
-      <c r="I8" s="11"/>
-      <c r="J8" s="10"/>
+        <v>0.50802823114247908</v>
+      </c>
+      <c r="I8" s="9">
+        <v>5520</v>
+      </c>
+      <c r="J8" s="10">
+        <f t="shared" si="1"/>
+        <v>0.24349360388178209</v>
+      </c>
       <c r="K8" s="9">
         <v>5520</v>
       </c>
       <c r="L8" s="10">
-        <f t="shared" si="1"/>
-        <v>0.32186588921282799</v>
+        <f t="shared" si="2"/>
+        <v>0.24349360388178209</v>
       </c>
       <c r="M8" s="11"/>
       <c r="N8" s="10"/>
@@ -3742,7 +3762,7 @@
       </c>
       <c r="T8" s="10">
         <f>SUM(S8/F8)</f>
-        <v>6.588921282798834E-3</v>
+        <v>4.9845610939567714E-3</v>
       </c>
       <c r="U8" s="11"/>
       <c r="V8" s="10">
@@ -3751,25 +3771,25 @@
       </c>
     </row>
     <row r="9" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="35" t="s">
         <v>58</v>
       </c>
       <c r="B9" s="9">
         <v>25394</v>
       </c>
       <c r="C9" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>17768</v>
       </c>
       <c r="D9" s="10">
-        <f t="shared" ref="D9:D47" si="4">SUM(C9/B9)</f>
+        <f t="shared" ref="D9:D47" si="5">SUM(C9/B9)</f>
         <v>0.69969284082854222</v>
       </c>
       <c r="E9" s="11">
         <v>76</v>
       </c>
       <c r="F9" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>17692</v>
       </c>
       <c r="G9" s="9">
@@ -3783,7 +3803,7 @@
         <v>10950</v>
       </c>
       <c r="J9" s="10">
-        <f t="shared" ref="J9:J46" si="5">SUM(I9/F9)</f>
+        <f t="shared" si="1"/>
         <v>0.61892380737056296</v>
       </c>
       <c r="K9" s="11"/>
@@ -3800,25 +3820,25 @@
       <c r="V9" s="10"/>
     </row>
     <row r="10" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="35" t="s">
         <v>59</v>
       </c>
       <c r="B10" s="9">
         <v>24601</v>
       </c>
       <c r="C10" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>18793</v>
       </c>
       <c r="D10" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.76391203609609371</v>
       </c>
       <c r="E10" s="11">
         <v>50</v>
       </c>
       <c r="F10" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>18743</v>
       </c>
       <c r="G10" s="9">
@@ -3832,7 +3852,7 @@
         <v>13863</v>
       </c>
       <c r="J10" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>0.73963613082217361</v>
       </c>
       <c r="K10" s="11"/>
@@ -3849,25 +3869,25 @@
       <c r="V10" s="10"/>
     </row>
     <row r="11" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="35" t="s">
         <v>60</v>
       </c>
       <c r="B11" s="9">
         <v>25166</v>
       </c>
       <c r="C11" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>18762</v>
       </c>
       <c r="D11" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.74552968290550747</v>
       </c>
       <c r="E11" s="11">
         <v>57</v>
       </c>
       <c r="F11" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>18705</v>
       </c>
       <c r="G11" s="9">
@@ -3881,7 +3901,7 @@
         <v>14981</v>
       </c>
       <c r="J11" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>0.80090884790163053</v>
       </c>
       <c r="K11" s="11"/>
@@ -3898,25 +3918,25 @@
       <c r="V11" s="10"/>
     </row>
     <row r="12" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="35" t="s">
         <v>61</v>
       </c>
       <c r="B12" s="9">
         <v>23653</v>
       </c>
       <c r="C12" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>17611</v>
       </c>
       <c r="D12" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.74455671584999794</v>
       </c>
       <c r="E12" s="11">
         <v>58</v>
       </c>
       <c r="F12" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>17553</v>
       </c>
       <c r="G12" s="9">
@@ -3930,7 +3950,7 @@
         <v>10797</v>
       </c>
       <c r="J12" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>0.61510852845667408</v>
       </c>
       <c r="K12" s="11"/>
@@ -3952,25 +3972,25 @@
       <c r="V12" s="10"/>
     </row>
     <row r="13" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="35" t="s">
         <v>62</v>
       </c>
       <c r="B13" s="9">
         <v>25715</v>
       </c>
       <c r="C13" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>20281</v>
       </c>
       <c r="D13" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.78868364767645338</v>
       </c>
       <c r="E13" s="11">
         <v>70</v>
       </c>
       <c r="F13" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20211</v>
       </c>
       <c r="G13" s="9">
@@ -3984,7 +4004,7 @@
         <v>18740</v>
       </c>
       <c r="J13" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>0.92721785166493498</v>
       </c>
       <c r="K13" s="11"/>
@@ -4001,25 +4021,25 @@
       <c r="V13" s="10"/>
     </row>
     <row r="14" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="35" t="s">
         <v>63</v>
       </c>
       <c r="B14" s="9">
         <v>27680</v>
       </c>
       <c r="C14" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>21286</v>
       </c>
       <c r="D14" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.76900289017341039</v>
       </c>
       <c r="E14" s="11">
         <v>70</v>
       </c>
       <c r="F14" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>21216</v>
       </c>
       <c r="G14" s="9">
@@ -4033,7 +4053,7 @@
         <v>16057</v>
       </c>
       <c r="J14" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>0.75683446455505277</v>
       </c>
       <c r="K14" s="11"/>
@@ -4050,25 +4070,25 @@
       <c r="V14" s="10"/>
     </row>
     <row r="15" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="35" t="s">
         <v>64</v>
       </c>
       <c r="B15" s="9">
         <v>26400</v>
       </c>
       <c r="C15" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>19877</v>
       </c>
       <c r="D15" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.75291666666666668</v>
       </c>
       <c r="E15" s="11">
         <v>59</v>
       </c>
       <c r="F15" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>19818</v>
       </c>
       <c r="G15" s="9">
@@ -4082,7 +4102,7 @@
         <v>15045</v>
       </c>
       <c r="J15" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>0.75915834090221013</v>
       </c>
       <c r="K15" s="11"/>
@@ -4099,25 +4119,25 @@
       <c r="V15" s="10"/>
     </row>
     <row r="16" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="35" t="s">
         <v>65</v>
       </c>
       <c r="B16" s="9">
         <v>26896</v>
       </c>
       <c r="C16" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>20527</v>
       </c>
       <c r="D16" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.76319898869720404</v>
       </c>
       <c r="E16" s="11">
         <v>121</v>
       </c>
       <c r="F16" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20406</v>
       </c>
       <c r="G16" s="9">
@@ -4131,7 +4151,7 @@
         <v>13116</v>
       </c>
       <c r="J16" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>0.64275213172596291</v>
       </c>
       <c r="K16" s="11"/>
@@ -4153,42 +4173,47 @@
       <c r="V16" s="10"/>
     </row>
     <row r="17" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="35" t="s">
         <v>66</v>
       </c>
       <c r="B17" s="9">
         <v>26019</v>
       </c>
       <c r="C17" s="9">
-        <f t="shared" si="2"/>
-        <v>18121</v>
+        <f t="shared" si="3"/>
+        <v>27816</v>
       </c>
       <c r="D17" s="10">
-        <f t="shared" si="4"/>
-        <v>0.69645259233636958</v>
+        <f t="shared" si="5"/>
+        <v>1.0690649141012336</v>
       </c>
       <c r="E17" s="11">
         <v>74</v>
       </c>
       <c r="F17" s="9">
-        <f t="shared" si="3"/>
-        <v>18047</v>
+        <f t="shared" si="4"/>
+        <v>27742</v>
       </c>
       <c r="G17" s="9">
         <v>8352</v>
       </c>
       <c r="H17" s="10">
         <f t="shared" si="6"/>
-        <v>0.46279159971186346</v>
-      </c>
-      <c r="I17" s="11"/>
-      <c r="J17" s="10"/>
+        <v>0.30105976497729076</v>
+      </c>
+      <c r="I17" s="9">
+        <v>9695</v>
+      </c>
+      <c r="J17" s="10">
+        <f t="shared" si="1"/>
+        <v>0.34947011751135465</v>
+      </c>
       <c r="K17" s="9">
         <v>9695</v>
       </c>
       <c r="L17" s="10">
         <f>SUM(K17/F17)</f>
-        <v>0.53720840028813654</v>
+        <v>0.34947011751135465</v>
       </c>
       <c r="M17" s="11"/>
       <c r="N17" s="10"/>
@@ -4202,48 +4227,54 @@
       <c r="V17" s="10"/>
     </row>
     <row r="18" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="35" t="s">
         <v>67</v>
       </c>
       <c r="B18" s="9">
         <v>27465</v>
       </c>
       <c r="C18" s="9">
-        <f t="shared" si="2"/>
-        <v>17265</v>
+        <f t="shared" si="3"/>
+        <v>25312</v>
       </c>
       <c r="D18" s="10">
-        <f t="shared" si="4"/>
-        <v>0.62861824139814304</v>
+        <f t="shared" si="5"/>
+        <v>0.92160932095394132</v>
       </c>
       <c r="E18" s="11">
         <v>33</v>
       </c>
       <c r="F18" s="9">
-        <f t="shared" si="3"/>
-        <v>17232</v>
+        <f t="shared" si="4"/>
+        <v>25279</v>
       </c>
       <c r="G18" s="9">
         <v>9040</v>
       </c>
       <c r="H18" s="10">
         <f t="shared" si="6"/>
-        <v>0.52460538532961931</v>
-      </c>
-      <c r="J18" s="10"/>
+        <v>0.35760908263776259</v>
+      </c>
+      <c r="I18" s="11">
+        <v>8047</v>
+      </c>
+      <c r="J18" s="10">
+        <f t="shared" si="1"/>
+        <v>0.31832746548518531</v>
+      </c>
       <c r="K18" s="11">
         <v>8047</v>
       </c>
       <c r="L18" s="10">
-        <f t="shared" si="1"/>
-        <v>0.46698003714020425</v>
+        <f t="shared" si="2"/>
+        <v>0.31832746548518531</v>
       </c>
       <c r="M18" s="11">
         <v>145</v>
       </c>
       <c r="N18" s="10">
         <f>SUM(M18/F18)</f>
-        <v>8.4145775301764161E-3</v>
+        <v>5.7359863918667667E-3</v>
       </c>
       <c r="O18" s="10"/>
       <c r="P18" s="10"/>
@@ -4255,25 +4286,25 @@
       <c r="V18" s="10"/>
     </row>
     <row r="19" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="39" t="s">
+      <c r="A19" s="35" t="s">
         <v>68</v>
       </c>
       <c r="B19" s="9">
         <v>27647</v>
       </c>
       <c r="C19" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>16809</v>
       </c>
       <c r="D19" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.60798639997106374</v>
       </c>
       <c r="E19" s="11">
         <v>68</v>
       </c>
       <c r="F19" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16741</v>
       </c>
       <c r="G19" s="9">
@@ -4287,7 +4318,7 @@
         <v>8076</v>
       </c>
       <c r="J19" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>0.48240845827608864</v>
       </c>
       <c r="K19" s="11"/>
@@ -4309,48 +4340,54 @@
       <c r="V19" s="10"/>
     </row>
     <row r="20" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="39" t="s">
+      <c r="A20" s="35" t="s">
         <v>69</v>
       </c>
       <c r="B20" s="9">
         <v>28366</v>
       </c>
       <c r="C20" s="9">
-        <f t="shared" si="2"/>
-        <v>17248</v>
+        <f t="shared" si="3"/>
+        <v>25244</v>
       </c>
       <c r="D20" s="10">
-        <f t="shared" si="4"/>
-        <v>0.60805189311147145</v>
+        <f t="shared" si="5"/>
+        <v>0.88993865895790736</v>
       </c>
       <c r="E20" s="11">
         <v>61</v>
       </c>
       <c r="F20" s="9">
         <f>SUM(G20,K20,I20,M20,O20,Q20,S20,U20)</f>
-        <v>17187</v>
+        <v>25183</v>
       </c>
       <c r="G20" s="9">
         <v>9042</v>
       </c>
       <c r="H20" s="10">
         <f t="shared" si="6"/>
-        <v>0.52609530459067899</v>
-      </c>
-      <c r="J20" s="10"/>
+        <v>0.35905174125402056</v>
+      </c>
+      <c r="I20" s="11">
+        <v>7996</v>
+      </c>
+      <c r="J20" s="10">
+        <f t="shared" si="1"/>
+        <v>0.31751578445776912</v>
+      </c>
       <c r="K20" s="11">
         <v>7996</v>
       </c>
       <c r="L20" s="10">
         <f>SUM(K20/F20)</f>
-        <v>0.46523535230115787</v>
+        <v>0.31751578445776912</v>
       </c>
       <c r="M20" s="11">
         <v>149</v>
       </c>
       <c r="N20" s="10">
         <f>SUM(M20/F20)</f>
-        <v>8.6693431081631463E-3</v>
+        <v>5.9166898304411708E-3</v>
       </c>
       <c r="O20" s="10"/>
       <c r="P20" s="10"/>
@@ -4362,25 +4399,25 @@
       <c r="V20" s="10"/>
     </row>
     <row r="21" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="35" t="s">
         <v>70</v>
       </c>
       <c r="B21" s="9">
         <v>25802</v>
       </c>
       <c r="C21" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>20245</v>
       </c>
       <c r="D21" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.78462909851949458</v>
       </c>
       <c r="E21" s="11">
         <v>59</v>
       </c>
       <c r="F21" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20186</v>
       </c>
       <c r="G21" s="9">
@@ -4394,7 +4431,7 @@
         <v>12888</v>
       </c>
       <c r="J21" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>0.63846230060437925</v>
       </c>
       <c r="K21" s="11"/>
@@ -4411,25 +4448,25 @@
       <c r="V21" s="10"/>
     </row>
     <row r="22" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="35" t="s">
         <v>71</v>
       </c>
       <c r="B22" s="9">
         <v>24057</v>
       </c>
       <c r="C22" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>17098</v>
       </c>
       <c r="D22" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.71072868603732797</v>
       </c>
       <c r="E22" s="11">
         <v>67</v>
       </c>
       <c r="F22" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>17031</v>
       </c>
       <c r="G22" s="9">
@@ -4443,7 +4480,7 @@
         <v>7116</v>
       </c>
       <c r="J22" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>0.41782631671657566</v>
       </c>
       <c r="K22" s="11"/>
@@ -4465,25 +4502,25 @@
       <c r="V22" s="10"/>
     </row>
     <row r="23" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="35" t="s">
         <v>72</v>
       </c>
       <c r="B23" s="9">
         <v>23959</v>
       </c>
       <c r="C23" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>16483</v>
       </c>
       <c r="D23" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.68796694352852794</v>
       </c>
       <c r="E23" s="11">
         <v>51</v>
       </c>
       <c r="F23" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16432</v>
       </c>
       <c r="G23" s="9">
@@ -4497,7 +4534,7 @@
         <v>8712</v>
       </c>
       <c r="J23" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>0.53018500486854914</v>
       </c>
       <c r="K23" s="11"/>
@@ -4524,49 +4561,54 @@
       </c>
     </row>
     <row r="24" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="39" t="s">
+      <c r="A24" s="35" t="s">
         <v>73</v>
       </c>
       <c r="B24" s="9">
         <v>27426</v>
       </c>
       <c r="C24" s="9">
-        <f t="shared" si="2"/>
-        <v>15038</v>
+        <f t="shared" si="3"/>
+        <v>18768</v>
       </c>
       <c r="D24" s="10">
-        <f t="shared" si="4"/>
-        <v>0.54831182089987607</v>
+        <f t="shared" si="5"/>
+        <v>0.68431415445197985</v>
       </c>
       <c r="E24" s="11">
         <v>62</v>
       </c>
       <c r="F24" s="9">
-        <f t="shared" si="3"/>
-        <v>14976</v>
+        <f t="shared" si="4"/>
+        <v>18706</v>
       </c>
       <c r="G24" s="9">
         <v>10797</v>
       </c>
       <c r="H24" s="10">
         <f t="shared" si="6"/>
-        <v>0.72095352564102566</v>
-      </c>
-      <c r="I24" s="11"/>
-      <c r="J24" s="10"/>
+        <v>0.57719448305356569</v>
+      </c>
+      <c r="I24" s="11">
+        <v>3730</v>
+      </c>
+      <c r="J24" s="10">
+        <f t="shared" si="1"/>
+        <v>0.19940126162728536</v>
+      </c>
       <c r="K24" s="11">
         <v>3730</v>
       </c>
       <c r="L24" s="10">
-        <f t="shared" si="1"/>
-        <v>0.24906517094017094</v>
+        <f t="shared" si="2"/>
+        <v>0.19940126162728536</v>
       </c>
       <c r="M24" s="11">
         <v>449</v>
       </c>
       <c r="N24" s="10">
         <f>SUM(M24/F24)</f>
-        <v>2.998130341880342E-2</v>
+        <v>2.4002993691863574E-2</v>
       </c>
       <c r="O24" s="10"/>
       <c r="P24" s="10"/>
@@ -4578,42 +4620,47 @@
       <c r="V24" s="10"/>
     </row>
     <row r="25" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="39" t="s">
+      <c r="A25" s="35" t="s">
         <v>74</v>
       </c>
       <c r="B25" s="9">
         <v>27426</v>
       </c>
       <c r="C25" s="9">
-        <f t="shared" si="2"/>
-        <v>13494</v>
+        <f t="shared" si="3"/>
+        <v>16219</v>
       </c>
       <c r="D25" s="10">
-        <f t="shared" si="4"/>
-        <v>0.49201487639466202</v>
+        <f t="shared" si="5"/>
+        <v>0.59137314956610521</v>
       </c>
       <c r="E25" s="11">
         <v>39</v>
       </c>
       <c r="F25" s="9">
-        <f t="shared" si="3"/>
-        <v>13455</v>
+        <f t="shared" si="4"/>
+        <v>16180</v>
       </c>
       <c r="G25" s="9">
         <v>10730</v>
       </c>
       <c r="H25" s="10">
         <f t="shared" si="6"/>
-        <v>0.79747305834262361</v>
-      </c>
-      <c r="I25" s="11"/>
-      <c r="J25" s="10"/>
+        <v>0.66316440049443759</v>
+      </c>
+      <c r="I25" s="11">
+        <v>2725</v>
+      </c>
+      <c r="J25" s="10">
+        <f t="shared" si="1"/>
+        <v>0.16841779975278121</v>
+      </c>
       <c r="K25" s="11">
         <v>2725</v>
       </c>
       <c r="L25" s="10">
-        <f t="shared" si="1"/>
-        <v>0.20252694165737645</v>
+        <f t="shared" si="2"/>
+        <v>0.16841779975278121</v>
       </c>
       <c r="M25" s="11"/>
       <c r="N25" s="10"/>
@@ -4627,42 +4674,47 @@
       <c r="V25" s="10"/>
     </row>
     <row r="26" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="39" t="s">
+      <c r="A26" s="35" t="s">
         <v>75</v>
       </c>
       <c r="B26" s="9">
         <v>24447</v>
       </c>
       <c r="C26" s="9">
-        <f t="shared" si="2"/>
-        <v>17559</v>
+        <f t="shared" si="3"/>
+        <v>26811</v>
       </c>
       <c r="D26" s="10">
-        <f t="shared" si="4"/>
-        <v>0.71824763774696276</v>
+        <f t="shared" si="5"/>
+        <v>1.0966989814701191</v>
       </c>
       <c r="E26" s="11">
         <v>58</v>
       </c>
       <c r="F26" s="9">
-        <f t="shared" si="3"/>
-        <v>17501</v>
+        <f t="shared" si="4"/>
+        <v>26753</v>
       </c>
       <c r="G26" s="9">
         <v>8249</v>
       </c>
       <c r="H26" s="10">
         <f t="shared" si="6"/>
-        <v>0.47134449460030853</v>
-      </c>
-      <c r="I26" s="11"/>
-      <c r="J26" s="10"/>
+        <v>0.30833925167270959</v>
+      </c>
+      <c r="I26" s="9">
+        <v>9252</v>
+      </c>
+      <c r="J26" s="10">
+        <f t="shared" si="1"/>
+        <v>0.3458303741636452</v>
+      </c>
       <c r="K26" s="9">
         <v>9252</v>
       </c>
       <c r="L26" s="10">
-        <f t="shared" si="1"/>
-        <v>0.52865550539969142</v>
+        <f t="shared" si="2"/>
+        <v>0.3458303741636452</v>
       </c>
       <c r="M26" s="11"/>
       <c r="N26" s="10"/>
@@ -4676,25 +4728,25 @@
       <c r="V26" s="10"/>
     </row>
     <row r="27" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="39" t="s">
+      <c r="A27" s="35" t="s">
         <v>76</v>
       </c>
       <c r="B27" s="9">
         <v>26433</v>
       </c>
       <c r="C27" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>20305</v>
       </c>
       <c r="D27" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.76816857715734121</v>
       </c>
       <c r="E27" s="11">
         <v>129</v>
       </c>
       <c r="F27" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20176</v>
       </c>
       <c r="G27" s="9">
@@ -4708,7 +4760,7 @@
         <v>12846</v>
       </c>
       <c r="J27" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>0.63669706582077712</v>
       </c>
       <c r="K27" s="11"/>
@@ -4725,25 +4777,25 @@
       <c r="V27" s="10"/>
     </row>
     <row r="28" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="39" t="s">
+      <c r="A28" s="35" t="s">
         <v>77</v>
       </c>
       <c r="B28" s="9">
         <v>26450</v>
       </c>
       <c r="C28" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>20433</v>
       </c>
       <c r="D28" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.77251417769376185</v>
       </c>
       <c r="E28" s="11">
         <v>124</v>
       </c>
       <c r="F28" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20309</v>
       </c>
       <c r="G28" s="9">
@@ -4757,7 +4809,7 @@
         <v>11628</v>
       </c>
       <c r="J28" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>0.57255404008075239</v>
       </c>
       <c r="K28" s="11"/>
@@ -4774,25 +4826,25 @@
       <c r="V28" s="10"/>
     </row>
     <row r="29" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="35" t="s">
         <v>78</v>
       </c>
       <c r="B29" s="9">
         <v>25394</v>
       </c>
       <c r="C29" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>19230</v>
       </c>
       <c r="D29" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.75726549578640623</v>
       </c>
       <c r="E29" s="11">
         <v>62</v>
       </c>
       <c r="F29" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>19168</v>
       </c>
       <c r="G29" s="9">
@@ -4806,7 +4858,7 @@
         <v>16615</v>
       </c>
       <c r="J29" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>0.866809265442404</v>
       </c>
       <c r="K29" s="11"/>
@@ -4823,25 +4875,25 @@
       <c r="V29" s="10"/>
     </row>
     <row r="30" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="35" t="s">
         <v>79</v>
       </c>
       <c r="B30" s="9">
         <v>27181</v>
       </c>
       <c r="C30" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>20861</v>
       </c>
       <c r="D30" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.76748464000588645</v>
       </c>
       <c r="E30" s="11">
         <v>62</v>
       </c>
       <c r="F30" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20799</v>
       </c>
       <c r="G30" s="9">
@@ -4855,7 +4907,7 @@
         <v>17927</v>
       </c>
       <c r="J30" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>0.8619164382903024</v>
       </c>
       <c r="K30" s="11"/>
@@ -4872,25 +4924,25 @@
       <c r="V30" s="10"/>
     </row>
     <row r="31" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="39" t="s">
+      <c r="A31" s="35" t="s">
         <v>80</v>
       </c>
       <c r="B31" s="9">
         <v>23427</v>
       </c>
       <c r="C31" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>17772</v>
       </c>
       <c r="D31" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.75861185811243437</v>
       </c>
       <c r="E31" s="11">
         <v>58</v>
       </c>
       <c r="F31" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>17714</v>
       </c>
       <c r="G31" s="9">
@@ -4904,7 +4956,7 @@
         <v>14188</v>
       </c>
       <c r="J31" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>0.800948402393587</v>
       </c>
       <c r="K31" s="11"/>
@@ -4921,42 +4973,47 @@
       <c r="V31" s="10"/>
     </row>
     <row r="32" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="39" t="s">
+      <c r="A32" s="35" t="s">
         <v>81</v>
       </c>
       <c r="B32" s="9">
         <v>24607</v>
       </c>
       <c r="C32" s="9">
-        <f t="shared" si="2"/>
-        <v>16888</v>
+        <f t="shared" si="3"/>
+        <v>24981</v>
       </c>
       <c r="D32" s="10">
-        <f t="shared" si="4"/>
-        <v>0.68630877392611855</v>
+        <f t="shared" si="5"/>
+        <v>1.0151989271345552</v>
       </c>
       <c r="E32" s="11">
         <v>47</v>
       </c>
       <c r="F32" s="9">
-        <f t="shared" si="3"/>
-        <v>16841</v>
+        <f t="shared" si="4"/>
+        <v>24934</v>
       </c>
       <c r="G32" s="9">
         <v>8748</v>
       </c>
       <c r="H32" s="10">
         <f t="shared" si="6"/>
-        <v>0.51944658868238225</v>
-      </c>
-      <c r="I32" s="9"/>
-      <c r="J32" s="10"/>
+        <v>0.35084623405791288</v>
+      </c>
+      <c r="I32" s="11">
+        <v>8093</v>
+      </c>
+      <c r="J32" s="10">
+        <f t="shared" si="1"/>
+        <v>0.32457688297104353</v>
+      </c>
       <c r="K32" s="11">
         <v>8093</v>
       </c>
       <c r="L32" s="10">
-        <f t="shared" si="1"/>
-        <v>0.4805534113176177</v>
+        <f t="shared" si="2"/>
+        <v>0.32457688297104353</v>
       </c>
       <c r="M32" s="11"/>
       <c r="N32" s="10"/>
@@ -4970,25 +5027,25 @@
       <c r="V32" s="10"/>
     </row>
     <row r="33" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="39" t="s">
+      <c r="A33" s="35" t="s">
         <v>82</v>
       </c>
       <c r="B33" s="9">
         <v>23504</v>
       </c>
       <c r="C33" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>17959</v>
       </c>
       <c r="D33" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.76408270932607214</v>
       </c>
       <c r="E33" s="11">
         <v>81</v>
       </c>
       <c r="F33" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>17878</v>
       </c>
       <c r="G33" s="9">
@@ -5002,7 +5059,7 @@
         <v>10922</v>
       </c>
       <c r="J33" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>0.61091844725360778</v>
       </c>
       <c r="K33" s="11"/>
@@ -5019,25 +5076,25 @@
       <c r="V33" s="10"/>
     </row>
     <row r="34" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="39" t="s">
+      <c r="A34" s="35" t="s">
         <v>83</v>
       </c>
       <c r="B34" s="9">
         <v>23154</v>
       </c>
       <c r="C34" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13344</v>
       </c>
       <c r="D34" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.57631510754081372</v>
       </c>
       <c r="E34" s="11">
         <v>43</v>
       </c>
       <c r="F34" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>13301</v>
       </c>
       <c r="G34" s="9">
@@ -5051,7 +5108,7 @@
         <v>5120</v>
       </c>
       <c r="J34" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>0.38493346364934966</v>
       </c>
       <c r="K34" s="11"/>
@@ -5073,49 +5130,54 @@
       <c r="V34" s="10"/>
     </row>
     <row r="35" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="39" t="s">
+      <c r="A35" s="35" t="s">
         <v>84</v>
       </c>
       <c r="B35" s="9">
         <v>23711</v>
       </c>
       <c r="C35" s="9">
-        <f t="shared" si="2"/>
-        <v>12700</v>
+        <f t="shared" si="3"/>
+        <v>17469</v>
       </c>
       <c r="D35" s="10">
-        <f t="shared" si="4"/>
-        <v>0.53561638058285188</v>
+        <f t="shared" si="5"/>
+        <v>0.73674665766943614</v>
       </c>
       <c r="E35" s="11">
         <v>52</v>
       </c>
       <c r="F35" s="9">
-        <f t="shared" si="3"/>
-        <v>12648</v>
+        <f t="shared" si="4"/>
+        <v>17417</v>
       </c>
       <c r="G35" s="9">
         <v>7539</v>
       </c>
       <c r="H35" s="10">
         <f t="shared" si="6"/>
-        <v>0.59606261859582543</v>
-      </c>
-      <c r="I35" s="11"/>
-      <c r="J35" s="10"/>
+        <v>0.43285295975196647</v>
+      </c>
+      <c r="I35" s="9">
+        <v>4769</v>
+      </c>
+      <c r="J35" s="10">
+        <f t="shared" si="1"/>
+        <v>0.27381294137911238</v>
+      </c>
       <c r="K35" s="9">
         <v>4769</v>
       </c>
       <c r="L35" s="10">
-        <f t="shared" si="1"/>
-        <v>0.37705566097406706</v>
+        <f t="shared" si="2"/>
+        <v>0.27381294137911238</v>
       </c>
       <c r="M35" s="11">
         <v>340</v>
       </c>
       <c r="N35" s="10">
         <f>SUM(M35/F35)</f>
-        <v>2.6881720430107527E-2</v>
+        <v>1.9521157489808809E-2</v>
       </c>
       <c r="O35" s="10"/>
       <c r="P35" s="10"/>
@@ -5127,25 +5189,25 @@
       <c r="V35" s="10"/>
     </row>
     <row r="36" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="39" t="s">
+      <c r="A36" s="35" t="s">
         <v>85</v>
       </c>
       <c r="B36" s="9">
         <v>25259</v>
       </c>
       <c r="C36" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>19272</v>
       </c>
       <c r="D36" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.76297557306306663</v>
       </c>
       <c r="E36" s="11">
         <v>72</v>
       </c>
       <c r="F36" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>19200</v>
       </c>
       <c r="G36" s="9">
@@ -5159,7 +5221,7 @@
         <v>14149</v>
       </c>
       <c r="J36" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>0.73692708333333334</v>
       </c>
       <c r="K36" s="11"/>
@@ -5176,25 +5238,25 @@
       <c r="V36" s="10"/>
     </row>
     <row r="37" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="39" t="s">
+      <c r="A37" s="35" t="s">
         <v>86</v>
       </c>
       <c r="B37" s="9">
         <v>22813</v>
       </c>
       <c r="C37" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15893</v>
       </c>
       <c r="D37" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.69666418270284491</v>
       </c>
       <c r="E37" s="11">
         <v>48</v>
       </c>
       <c r="F37" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15845</v>
       </c>
       <c r="G37" s="9">
@@ -5208,7 +5270,7 @@
         <v>6109</v>
       </c>
       <c r="J37" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>0.38554749132218363</v>
       </c>
       <c r="K37" s="9"/>
@@ -5225,49 +5287,54 @@
       <c r="V37" s="10"/>
     </row>
     <row r="38" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="39" t="s">
+      <c r="A38" s="35" t="s">
         <v>87</v>
       </c>
       <c r="B38" s="9">
         <v>23554</v>
       </c>
       <c r="C38" s="9">
-        <f t="shared" si="2"/>
-        <v>17148</v>
+        <f t="shared" si="3"/>
+        <v>26259</v>
       </c>
       <c r="D38" s="10">
-        <f t="shared" si="4"/>
-        <v>0.72802920947609751</v>
+        <f t="shared" si="5"/>
+        <v>1.1148424895983697</v>
       </c>
       <c r="E38" s="11">
         <v>49</v>
       </c>
       <c r="F38" s="9">
-        <f t="shared" si="3"/>
-        <v>17099</v>
+        <f t="shared" si="4"/>
+        <v>26210</v>
       </c>
       <c r="G38" s="9">
         <v>7860</v>
       </c>
       <c r="H38" s="10">
         <f t="shared" si="6"/>
-        <v>0.45967600444470436</v>
-      </c>
-      <c r="I38" s="9"/>
-      <c r="J38" s="10"/>
+        <v>0.29988553987027849</v>
+      </c>
+      <c r="I38" s="11">
+        <v>9111</v>
+      </c>
+      <c r="J38" s="10">
+        <f t="shared" si="1"/>
+        <v>0.34761541396413581</v>
+      </c>
       <c r="K38" s="11">
         <v>9111</v>
       </c>
       <c r="L38" s="10">
-        <f t="shared" si="1"/>
-        <v>0.53283817767120889</v>
+        <f t="shared" si="2"/>
+        <v>0.34761541396413581</v>
       </c>
       <c r="M38" s="11">
         <v>128</v>
       </c>
       <c r="N38" s="10">
         <f>SUM(M38/F38)</f>
-        <v>7.4858178840867887E-3</v>
+        <v>4.8836322014498279E-3</v>
       </c>
       <c r="O38" s="10"/>
       <c r="P38" s="10"/>
@@ -5279,25 +5346,25 @@
       <c r="V38" s="10"/>
     </row>
     <row r="39" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="39" t="s">
+      <c r="A39" s="35" t="s">
         <v>88</v>
       </c>
       <c r="B39" s="9">
         <v>26657</v>
       </c>
       <c r="C39" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>19907</v>
       </c>
       <c r="D39" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.74678320891323102</v>
       </c>
       <c r="E39" s="11">
         <v>82</v>
       </c>
       <c r="F39" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>19825</v>
       </c>
       <c r="G39" s="9">
@@ -5311,7 +5378,7 @@
         <v>15650</v>
       </c>
       <c r="J39" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>0.78940731399747788</v>
       </c>
       <c r="K39" s="11"/>
@@ -5328,25 +5395,25 @@
       <c r="V39" s="10"/>
     </row>
     <row r="40" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="39" t="s">
+      <c r="A40" s="35" t="s">
         <v>89</v>
       </c>
       <c r="B40" s="9">
         <v>26940</v>
       </c>
       <c r="C40" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>16267</v>
       </c>
       <c r="D40" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.60382331106161846</v>
       </c>
       <c r="E40" s="11">
         <v>103</v>
       </c>
       <c r="F40" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16164</v>
       </c>
       <c r="G40" s="9">
@@ -5360,7 +5427,7 @@
         <v>6635</v>
       </c>
       <c r="J40" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>0.41048007918831975</v>
       </c>
       <c r="K40" s="11"/>
@@ -5382,42 +5449,47 @@
       <c r="V40" s="10"/>
     </row>
     <row r="41" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="39" t="s">
+      <c r="A41" s="35" t="s">
         <v>90</v>
       </c>
       <c r="B41" s="9">
         <v>25582</v>
       </c>
       <c r="C41" s="9">
-        <f t="shared" si="2"/>
-        <v>19284</v>
+        <f t="shared" si="3"/>
+        <v>34555</v>
       </c>
       <c r="D41" s="10">
-        <f t="shared" si="4"/>
-        <v>0.75381127355171607</v>
+        <f t="shared" si="5"/>
+        <v>1.350754436713314</v>
       </c>
       <c r="E41" s="11">
         <v>58</v>
       </c>
       <c r="F41" s="9">
-        <f t="shared" si="3"/>
-        <v>19226</v>
+        <f t="shared" si="4"/>
+        <v>34497</v>
       </c>
       <c r="G41" s="9">
         <v>3955</v>
       </c>
       <c r="H41" s="10">
         <f t="shared" si="6"/>
-        <v>0.20571101633205036</v>
-      </c>
-      <c r="I41" s="11"/>
-      <c r="J41" s="10"/>
+        <v>0.1146476505203351</v>
+      </c>
+      <c r="I41" s="9">
+        <v>15271</v>
+      </c>
+      <c r="J41" s="10">
+        <f t="shared" si="1"/>
+        <v>0.44267617473983245</v>
+      </c>
       <c r="K41" s="9">
         <v>15271</v>
       </c>
       <c r="L41" s="10">
-        <f t="shared" si="1"/>
-        <v>0.79428898366794964</v>
+        <f t="shared" si="2"/>
+        <v>0.44267617473983245</v>
       </c>
       <c r="M41" s="11"/>
       <c r="N41" s="10"/>
@@ -5431,25 +5503,25 @@
       <c r="V41" s="10"/>
     </row>
     <row r="42" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="35" t="s">
         <v>91</v>
       </c>
       <c r="B42" s="9">
         <v>25943</v>
       </c>
       <c r="C42" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>18711</v>
       </c>
       <c r="D42" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.72123501522568711</v>
       </c>
       <c r="E42" s="11">
         <v>64</v>
       </c>
       <c r="F42" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>18647</v>
       </c>
       <c r="G42" s="9">
@@ -5463,7 +5535,7 @@
         <v>10835</v>
       </c>
       <c r="J42" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>0.5810586153268622</v>
       </c>
       <c r="K42" s="11"/>
@@ -5485,25 +5557,25 @@
       <c r="V42" s="10"/>
     </row>
     <row r="43" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="39" t="s">
+      <c r="A43" s="35" t="s">
         <v>92</v>
       </c>
       <c r="B43" s="9">
         <v>26775</v>
       </c>
       <c r="C43" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>19727</v>
       </c>
       <c r="D43" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.7367693744164332</v>
       </c>
       <c r="E43" s="11">
         <v>67</v>
       </c>
       <c r="F43" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>19660</v>
       </c>
       <c r="G43" s="9">
@@ -5517,7 +5589,7 @@
         <v>14310</v>
       </c>
       <c r="J43" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>0.72787385554425232</v>
       </c>
       <c r="K43" s="11"/>
@@ -5534,36 +5606,41 @@
       <c r="V43" s="10"/>
     </row>
     <row r="44" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="39" t="s">
+      <c r="A44" s="35" t="s">
         <v>93</v>
       </c>
       <c r="B44" s="9">
         <v>20424</v>
       </c>
       <c r="C44" s="9">
-        <f t="shared" si="2"/>
-        <v>13233</v>
+        <f t="shared" si="3"/>
+        <v>20882</v>
       </c>
       <c r="D44" s="10">
-        <f t="shared" si="4"/>
-        <v>0.64791421856639253</v>
+        <f t="shared" si="5"/>
+        <v>1.022424598511555</v>
       </c>
       <c r="E44" s="11">
         <v>61</v>
       </c>
       <c r="F44" s="9">
-        <f t="shared" si="3"/>
-        <v>13172</v>
+        <f t="shared" si="4"/>
+        <v>20821</v>
       </c>
       <c r="G44" s="9">
         <v>5523</v>
       </c>
       <c r="H44" s="10">
         <f t="shared" si="6"/>
-        <v>0.41929851199514123</v>
-      </c>
-      <c r="I44" s="11"/>
-      <c r="J44" s="10"/>
+        <v>0.26526103453244321</v>
+      </c>
+      <c r="I44" s="12">
+        <v>7649</v>
+      </c>
+      <c r="J44" s="10">
+        <f t="shared" si="1"/>
+        <v>0.3673694827337784</v>
+      </c>
       <c r="K44" s="11"/>
       <c r="L44" s="10"/>
       <c r="M44" s="11"/>
@@ -5573,7 +5650,7 @@
       </c>
       <c r="P44" s="10">
         <f>SUM(O44/F44)</f>
-        <v>0.58070148800485877</v>
+        <v>0.3673694827337784</v>
       </c>
       <c r="Q44" s="11"/>
       <c r="R44" s="10"/>
@@ -5583,36 +5660,41 @@
       <c r="V44" s="10"/>
     </row>
     <row r="45" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="39" t="s">
+      <c r="A45" s="35" t="s">
         <v>94</v>
       </c>
       <c r="B45" s="9">
         <v>23674</v>
       </c>
       <c r="C45" s="9">
-        <f t="shared" si="2"/>
-        <v>14545</v>
+        <f t="shared" si="3"/>
+        <v>22267</v>
       </c>
       <c r="D45" s="10">
-        <f t="shared" si="4"/>
-        <v>0.61438709132381519</v>
+        <f t="shared" si="5"/>
+        <v>0.94056771141336493</v>
       </c>
       <c r="E45" s="11">
         <v>41</v>
       </c>
       <c r="F45" s="9">
-        <f t="shared" si="3"/>
-        <v>14504</v>
+        <f t="shared" si="4"/>
+        <v>22226</v>
       </c>
       <c r="G45" s="9">
         <v>6782</v>
       </c>
       <c r="H45" s="10">
         <f>SUM(G45/F45)</f>
-        <v>0.46759514616657472</v>
-      </c>
-      <c r="I45" s="11"/>
-      <c r="J45" s="10"/>
+        <v>0.30513812651849187</v>
+      </c>
+      <c r="I45" s="12">
+        <v>7722</v>
+      </c>
+      <c r="J45" s="10">
+        <f t="shared" si="1"/>
+        <v>0.34743093674075409</v>
+      </c>
       <c r="K45" s="11"/>
       <c r="L45" s="10"/>
       <c r="M45" s="11"/>
@@ -5622,7 +5704,7 @@
       </c>
       <c r="P45" s="10">
         <f>SUM(O45/F45)</f>
-        <v>0.53240485383342528</v>
+        <v>0.34743093674075409</v>
       </c>
       <c r="Q45" s="11"/>
       <c r="R45" s="10"/>
@@ -5632,25 +5714,25 @@
       <c r="V45" s="10"/>
     </row>
     <row r="46" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="39" t="s">
+      <c r="A46" s="35" t="s">
         <v>95</v>
       </c>
       <c r="B46" s="9">
         <v>27298</v>
       </c>
       <c r="C46" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>18069</v>
       </c>
       <c r="D46" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.66191662392849293</v>
       </c>
       <c r="E46" s="11">
         <v>44</v>
       </c>
       <c r="F46" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>18025</v>
       </c>
       <c r="G46" s="9">
@@ -5664,7 +5746,7 @@
         <v>9325</v>
       </c>
       <c r="J46" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>0.51733703190013869</v>
       </c>
       <c r="K46" s="11"/>
@@ -5686,42 +5768,47 @@
       <c r="V46" s="10"/>
     </row>
     <row r="47" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="39" t="s">
+      <c r="A47" s="35" t="s">
         <v>96</v>
       </c>
       <c r="B47" s="9">
         <v>25191</v>
       </c>
       <c r="C47" s="9">
-        <f t="shared" si="2"/>
-        <v>18662</v>
+        <f t="shared" si="3"/>
+        <v>29108</v>
       </c>
       <c r="D47" s="10">
-        <f t="shared" si="4"/>
-        <v>0.74082013417490378</v>
+        <f t="shared" si="5"/>
+        <v>1.1554920408082252</v>
       </c>
       <c r="E47" s="11">
         <v>67</v>
       </c>
       <c r="F47" s="9">
-        <f t="shared" si="3"/>
-        <v>18595</v>
+        <f t="shared" si="4"/>
+        <v>29041</v>
       </c>
       <c r="G47" s="9">
         <v>8149</v>
       </c>
       <c r="H47" s="10">
         <f t="shared" si="6"/>
-        <v>0.43823608496907773</v>
-      </c>
-      <c r="I47" s="9"/>
-      <c r="J47" s="10"/>
+        <v>0.28060328501084675</v>
+      </c>
+      <c r="I47" s="11">
+        <v>10446</v>
+      </c>
+      <c r="J47" s="10">
+        <f t="shared" si="1"/>
+        <v>0.35969835749457663</v>
+      </c>
       <c r="K47" s="11">
         <v>10446</v>
       </c>
       <c r="L47" s="10">
-        <f t="shared" si="1"/>
-        <v>0.56176391503092227</v>
+        <f t="shared" si="2"/>
+        <v>0.35969835749457663</v>
       </c>
       <c r="M47" s="11"/>
       <c r="N47" s="10"/>
@@ -5744,11 +5831,11 @@
       </c>
       <c r="C48" s="14">
         <f>SUM(C7:C47)</f>
-        <v>726801</v>
+        <v>844437</v>
       </c>
       <c r="D48" s="15">
         <f>SUM(C48/B48)</f>
-        <v>0.69802559295598254</v>
+        <v>0.81100416432967348</v>
       </c>
       <c r="E48" s="16">
         <f>SUM(E7:E47)</f>
@@ -5756,7 +5843,7 @@
       </c>
       <c r="F48" s="14">
         <f>SUM(F7:F47)</f>
-        <v>724135</v>
+        <v>841771</v>
       </c>
       <c r="G48" s="14">
         <f>SUM(G7:G47)</f>
@@ -5764,15 +5851,15 @@
       </c>
       <c r="H48" s="15">
         <f>SUM(G48/F48)</f>
-        <v>0.39696741629668503</v>
+        <v>0.3414919259513573</v>
       </c>
       <c r="I48" s="14">
         <f>SUM(I7:I47)</f>
-        <v>316600</v>
+        <v>434236</v>
       </c>
       <c r="J48" s="15">
         <f>SUM(I48/F48)</f>
-        <v>0.43721129347428311</v>
+        <v>0.51586001418438032</v>
       </c>
       <c r="K48" s="14">
         <f>SUM(K7:K47)</f>
@@ -5780,7 +5867,7 @@
       </c>
       <c r="L48" s="15">
         <f>SUM(K48/F48)</f>
-        <v>0.14122366685769919</v>
+        <v>0.12148791060751678</v>
       </c>
       <c r="M48" s="14">
         <f>SUM(M7:M47)</f>
@@ -5788,7 +5875,7 @@
       </c>
       <c r="N48" s="15">
         <f>SUM(M48/F48)</f>
-        <v>2.8972498222016611E-3</v>
+        <v>2.4923643128594358E-3</v>
       </c>
       <c r="O48" s="14">
         <f>SUM(O7:O47)</f>
@@ -5796,7 +5883,7 @@
       </c>
       <c r="P48" s="15">
         <f>SUM(O48/F48)</f>
-        <v>2.1226704965234384E-2</v>
+        <v>1.8260310702079306E-2</v>
       </c>
       <c r="Q48" s="14">
         <f>SUM(Q7:Q47)</f>
@@ -5804,7 +5891,7 @@
       </c>
       <c r="R48" s="15">
         <f>SUM(Q48/F48)</f>
-        <v>4.6952570998501662E-5</v>
+        <v>4.0391032715548525E-5</v>
       </c>
       <c r="S48" s="14">
         <f>SUM(S7:S47)</f>
@@ -5812,7 +5899,7 @@
       </c>
       <c r="T48" s="15">
         <f>SUM(S48/F48)</f>
-        <v>3.866682317523666E-4</v>
+        <v>3.3263203412804671E-4</v>
       </c>
       <c r="U48" s="14">
         <f>SUM(U7:U47)</f>
@@ -5820,7 +5907,7 @@
       </c>
       <c r="V48" s="15">
         <f>SUM(U48/F48)</f>
-        <v>4.0047781145780829E-5</v>
+        <v>3.4451174963261977E-5</v>
       </c>
     </row>
     <row r="51" spans="4:4" x14ac:dyDescent="0.2">
@@ -5906,8 +5993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B29ADA29-60E2-5C49-A453-E54C505FD3C8}">
   <dimension ref="A1:AP74"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:A47"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5938,96 +6025,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
-      <c r="S1" s="36"/>
-      <c r="T1" s="36"/>
-      <c r="U1" s="36"/>
-      <c r="V1" s="36"/>
-      <c r="W1" s="36"/>
-      <c r="X1" s="36"/>
-      <c r="Y1" s="36"/>
-      <c r="Z1" s="36"/>
-      <c r="AA1" s="36"/>
-      <c r="AB1" s="36"/>
-      <c r="AC1" s="36"/>
-      <c r="AD1" s="36"/>
-      <c r="AE1" s="36"/>
-      <c r="AF1" s="36"/>
-      <c r="AG1" s="36"/>
-      <c r="AH1" s="36"/>
-      <c r="AI1" s="36"/>
-      <c r="AJ1" s="36"/>
-      <c r="AK1" s="36"/>
-      <c r="AL1" s="36"/>
-      <c r="AM1" s="36"/>
-      <c r="AN1" s="36"/>
-      <c r="AO1" s="36"/>
-      <c r="AP1" s="36"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="37"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="37"/>
+      <c r="W1" s="37"/>
+      <c r="X1" s="37"/>
+      <c r="Y1" s="37"/>
+      <c r="Z1" s="37"/>
+      <c r="AA1" s="37"/>
+      <c r="AB1" s="37"/>
+      <c r="AC1" s="37"/>
+      <c r="AD1" s="37"/>
+      <c r="AE1" s="37"/>
+      <c r="AF1" s="37"/>
+      <c r="AG1" s="37"/>
+      <c r="AH1" s="37"/>
+      <c r="AI1" s="37"/>
+      <c r="AJ1" s="37"/>
+      <c r="AK1" s="37"/>
+      <c r="AL1" s="37"/>
+      <c r="AM1" s="37"/>
+      <c r="AN1" s="37"/>
+      <c r="AO1" s="37"/>
+      <c r="AP1" s="37"/>
     </row>
     <row r="2" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
-      <c r="O2" s="36"/>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="36"/>
-      <c r="R2" s="36"/>
-      <c r="S2" s="36"/>
-      <c r="T2" s="36"/>
-      <c r="U2" s="36"/>
-      <c r="V2" s="36"/>
-      <c r="W2" s="36"/>
-      <c r="X2" s="36"/>
-      <c r="Y2" s="36"/>
-      <c r="Z2" s="36"/>
-      <c r="AA2" s="36"/>
-      <c r="AB2" s="36"/>
-      <c r="AC2" s="36"/>
-      <c r="AD2" s="36"/>
-      <c r="AE2" s="36"/>
-      <c r="AF2" s="36"/>
-      <c r="AG2" s="36"/>
-      <c r="AH2" s="36"/>
-      <c r="AI2" s="36"/>
-      <c r="AJ2" s="36"/>
-      <c r="AK2" s="36"/>
-      <c r="AL2" s="36"/>
-      <c r="AM2" s="36"/>
-      <c r="AN2" s="36"/>
-      <c r="AO2" s="36"/>
-      <c r="AP2" s="36"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="37"/>
+      <c r="V2" s="37"/>
+      <c r="W2" s="37"/>
+      <c r="X2" s="37"/>
+      <c r="Y2" s="37"/>
+      <c r="Z2" s="37"/>
+      <c r="AA2" s="37"/>
+      <c r="AB2" s="37"/>
+      <c r="AC2" s="37"/>
+      <c r="AD2" s="37"/>
+      <c r="AE2" s="37"/>
+      <c r="AF2" s="37"/>
+      <c r="AG2" s="37"/>
+      <c r="AH2" s="37"/>
+      <c r="AI2" s="37"/>
+      <c r="AJ2" s="37"/>
+      <c r="AK2" s="37"/>
+      <c r="AL2" s="37"/>
+      <c r="AM2" s="37"/>
+      <c r="AN2" s="37"/>
+      <c r="AO2" s="37"/>
+      <c r="AP2" s="37"/>
     </row>
     <row r="3" spans="1:42" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:42" s="1" customFormat="1" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6049,78 +6136,78 @@
       <c r="F4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35" t="s">
+      <c r="H4" s="36"/>
+      <c r="I4" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35" t="s">
+      <c r="J4" s="36"/>
+      <c r="K4" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35" t="s">
+      <c r="L4" s="36"/>
+      <c r="M4" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="N4" s="35"/>
-      <c r="O4" s="35" t="s">
+      <c r="N4" s="36"/>
+      <c r="O4" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="P4" s="35"/>
-      <c r="Q4" s="35" t="s">
+      <c r="P4" s="36"/>
+      <c r="Q4" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="R4" s="35"/>
-      <c r="S4" s="35" t="s">
+      <c r="R4" s="36"/>
+      <c r="S4" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="T4" s="35"/>
-      <c r="U4" s="35" t="s">
+      <c r="T4" s="36"/>
+      <c r="U4" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="V4" s="35"/>
-      <c r="W4" s="35" t="s">
+      <c r="V4" s="36"/>
+      <c r="W4" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="X4" s="35"/>
-      <c r="Y4" s="35" t="s">
+      <c r="X4" s="36"/>
+      <c r="Y4" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="Z4" s="35"/>
-      <c r="AA4" s="35" t="s">
+      <c r="Z4" s="36"/>
+      <c r="AA4" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="AB4" s="35"/>
-      <c r="AC4" s="35" t="s">
+      <c r="AB4" s="36"/>
+      <c r="AC4" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="AD4" s="35"/>
-      <c r="AE4" s="37" t="s">
+      <c r="AD4" s="36"/>
+      <c r="AE4" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="AF4" s="38"/>
-      <c r="AG4" s="35" t="s">
+      <c r="AF4" s="39"/>
+      <c r="AG4" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="AH4" s="35"/>
-      <c r="AI4" s="35" t="s">
+      <c r="AH4" s="36"/>
+      <c r="AI4" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="AJ4" s="35"/>
-      <c r="AK4" s="35" t="s">
+      <c r="AJ4" s="36"/>
+      <c r="AK4" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="AL4" s="35"/>
-      <c r="AM4" s="35" t="s">
+      <c r="AL4" s="36"/>
+      <c r="AM4" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="AN4" s="35"/>
-      <c r="AO4" s="35" t="s">
+      <c r="AN4" s="36"/>
+      <c r="AO4" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="AP4" s="35"/>
+      <c r="AP4" s="36"/>
     </row>
     <row r="5" spans="1:42" s="1" customFormat="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
@@ -6333,7 +6420,7 @@
       </c>
     </row>
     <row r="7" spans="1:42" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="35" t="s">
         <v>56</v>
       </c>
       <c r="B7" s="9">
@@ -6359,8 +6446,12 @@
       <c r="H7" s="10">
         <v>0.69520000000000004</v>
       </c>
-      <c r="I7" s="11"/>
-      <c r="J7" s="10"/>
+      <c r="I7" s="9">
+        <v>4578</v>
+      </c>
+      <c r="J7" s="10">
+        <v>0.29249999999999998</v>
+      </c>
       <c r="K7" s="9">
         <v>4578</v>
       </c>
@@ -6403,7 +6494,7 @@
       <c r="AP7" s="10"/>
     </row>
     <row r="8" spans="1:42" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="35" t="s">
         <v>57</v>
       </c>
       <c r="B8" s="9">
@@ -6429,8 +6520,12 @@
       <c r="H8" s="10">
         <v>0.8155</v>
       </c>
-      <c r="I8" s="11"/>
-      <c r="J8" s="10"/>
+      <c r="I8" s="9">
+        <v>3357</v>
+      </c>
+      <c r="J8" s="10">
+        <v>0.1845</v>
+      </c>
       <c r="K8" s="9">
         <v>3357</v>
       </c>
@@ -6469,7 +6564,7 @@
       <c r="AP8" s="10"/>
     </row>
     <row r="9" spans="1:42" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="35" t="s">
         <v>58</v>
       </c>
       <c r="B9" s="9">
@@ -6542,7 +6637,7 @@
       <c r="AP9" s="10"/>
     </row>
     <row r="10" spans="1:42" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="35" t="s">
         <v>59</v>
       </c>
       <c r="B10" s="9">
@@ -6615,7 +6710,7 @@
       <c r="AP10" s="10"/>
     </row>
     <row r="11" spans="1:42" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="35" t="s">
         <v>60</v>
       </c>
       <c r="B11" s="9">
@@ -6688,7 +6783,7 @@
       <c r="AP11" s="10"/>
     </row>
     <row r="12" spans="1:42" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="35" t="s">
         <v>61</v>
       </c>
       <c r="B12" s="9">
@@ -6760,7 +6855,7 @@
       <c r="AP12" s="10"/>
     </row>
     <row r="13" spans="1:42" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="35" t="s">
         <v>62</v>
       </c>
       <c r="B13" s="9">
@@ -6833,7 +6928,7 @@
       <c r="AP13" s="10"/>
     </row>
     <row r="14" spans="1:42" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="35" t="s">
         <v>63</v>
       </c>
       <c r="B14" s="9">
@@ -6906,7 +7001,7 @@
       <c r="AP14" s="10"/>
     </row>
     <row r="15" spans="1:42" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="35" t="s">
         <v>64</v>
       </c>
       <c r="B15" s="9">
@@ -6979,7 +7074,7 @@
       <c r="AP15" s="10"/>
     </row>
     <row r="16" spans="1:42" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="35" t="s">
         <v>65</v>
       </c>
       <c r="B16" s="9">
@@ -7056,7 +7151,7 @@
       <c r="AP16" s="10"/>
     </row>
     <row r="17" spans="1:42" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="35" t="s">
         <v>66</v>
       </c>
       <c r="B17" s="9">
@@ -7083,8 +7178,13 @@
         <f t="shared" si="3"/>
         <v>0.66343390804597702</v>
       </c>
-      <c r="I17" s="11"/>
-      <c r="J17" s="10"/>
+      <c r="I17" s="9">
+        <v>6233</v>
+      </c>
+      <c r="J17" s="10">
+        <f t="shared" si="2"/>
+        <v>0.31983784893267653</v>
+      </c>
       <c r="K17" s="9">
         <v>6233</v>
       </c>
@@ -7134,7 +7234,7 @@
       <c r="AP17" s="10"/>
     </row>
     <row r="18" spans="1:42" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="35" t="s">
         <v>67</v>
       </c>
       <c r="B18" s="9">
@@ -7161,8 +7261,13 @@
         <f t="shared" si="3"/>
         <v>0.77018705704658996</v>
       </c>
-      <c r="I18" s="11"/>
-      <c r="J18" s="10"/>
+      <c r="I18" s="9">
+        <v>2969</v>
+      </c>
+      <c r="J18" s="10">
+        <f t="shared" si="2"/>
+        <v>0.17247589171604508</v>
+      </c>
       <c r="K18" s="11"/>
       <c r="L18" s="10"/>
       <c r="M18" s="11">
@@ -7212,7 +7317,7 @@
       <c r="AP18" s="10"/>
     </row>
     <row r="19" spans="1:42" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="39" t="s">
+      <c r="A19" s="35" t="s">
         <v>68</v>
       </c>
       <c r="B19" s="9">
@@ -7285,7 +7390,7 @@
       <c r="AP19" s="10"/>
     </row>
     <row r="20" spans="1:42" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="39" t="s">
+      <c r="A20" s="35" t="s">
         <v>69</v>
       </c>
       <c r="B20" s="9">
@@ -7312,8 +7417,13 @@
         <f t="shared" si="3"/>
         <v>0.76033595552138167</v>
       </c>
-      <c r="I20" s="11"/>
-      <c r="J20" s="10"/>
+      <c r="I20" s="9">
+        <v>3411</v>
+      </c>
+      <c r="J20" s="10">
+        <f t="shared" si="2"/>
+        <v>0.20175075412551013</v>
+      </c>
       <c r="K20" s="9">
         <v>3411</v>
       </c>
@@ -7373,7 +7483,7 @@
       <c r="AP20" s="10"/>
     </row>
     <row r="21" spans="1:42" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="35" t="s">
         <v>70</v>
       </c>
       <c r="B21" s="9">
@@ -7446,7 +7556,7 @@
       <c r="AP21" s="10"/>
     </row>
     <row r="22" spans="1:42" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="35" t="s">
         <v>71</v>
       </c>
       <c r="B22" s="9">
@@ -7519,7 +7629,7 @@
       <c r="AP22" s="10"/>
     </row>
     <row r="23" spans="1:42" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="35" t="s">
         <v>72</v>
       </c>
       <c r="B23" s="9">
@@ -7550,7 +7660,7 @@
         <v>7606</v>
       </c>
       <c r="J23" s="10">
-        <f>SUM(I23/F23)</f>
+        <f t="shared" si="2"/>
         <v>0.41940998070030328</v>
       </c>
       <c r="K23" s="11"/>
@@ -7592,7 +7702,7 @@
       <c r="AP23" s="10"/>
     </row>
     <row r="24" spans="1:42" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="39" t="s">
+      <c r="A24" s="35" t="s">
         <v>73</v>
       </c>
       <c r="B24" s="9">
@@ -7618,8 +7728,13 @@
         <f t="shared" si="3"/>
         <v>0.86814513566753515</v>
       </c>
-      <c r="I24" s="11"/>
-      <c r="J24" s="10"/>
+      <c r="I24" s="9">
+        <v>1599</v>
+      </c>
+      <c r="J24" s="10">
+        <f t="shared" si="2"/>
+        <v>0.1016076761771621</v>
+      </c>
       <c r="K24" s="11"/>
       <c r="L24" s="10"/>
       <c r="M24" s="11">
@@ -7669,7 +7784,7 @@
       <c r="AP24" s="10"/>
     </row>
     <row r="25" spans="1:42" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="39" t="s">
+      <c r="A25" s="35" t="s">
         <v>74</v>
       </c>
       <c r="B25" s="9">
@@ -7695,8 +7810,13 @@
         <f t="shared" si="3"/>
         <v>0.89420448332422087</v>
       </c>
-      <c r="I25" s="11"/>
-      <c r="J25" s="10"/>
+      <c r="I25" s="9">
+        <v>1222</v>
+      </c>
+      <c r="J25" s="10">
+        <f t="shared" si="2"/>
+        <v>8.351558228540186E-2</v>
+      </c>
       <c r="K25" s="11"/>
       <c r="L25" s="10"/>
       <c r="M25" s="11">
@@ -7746,7 +7866,7 @@
       <c r="AP25" s="10"/>
     </row>
     <row r="26" spans="1:42" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="39" t="s">
+      <c r="A26" s="35" t="s">
         <v>75</v>
       </c>
       <c r="B26" s="9">
@@ -7772,8 +7892,13 @@
         <f t="shared" si="3"/>
         <v>0.62558544820825623</v>
       </c>
-      <c r="I26" s="11"/>
-      <c r="J26" s="10"/>
+      <c r="I26" s="9">
+        <v>6326</v>
+      </c>
+      <c r="J26" s="10">
+        <f t="shared" si="2"/>
+        <v>0.34451584794684675</v>
+      </c>
       <c r="K26" s="9">
         <v>6326</v>
       </c>
@@ -7823,7 +7948,7 @@
       <c r="AP26" s="10"/>
     </row>
     <row r="27" spans="1:42" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="39" t="s">
+      <c r="A27" s="35" t="s">
         <v>76</v>
       </c>
       <c r="B27" s="9">
@@ -7896,7 +8021,7 @@
       <c r="AP27" s="10"/>
     </row>
     <row r="28" spans="1:42" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="39" t="s">
+      <c r="A28" s="35" t="s">
         <v>77</v>
       </c>
       <c r="B28" s="9">
@@ -7969,7 +8094,7 @@
       <c r="AP28" s="10"/>
     </row>
     <row r="29" spans="1:42" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="35" t="s">
         <v>78</v>
       </c>
       <c r="B29" s="9">
@@ -8042,7 +8167,7 @@
       <c r="AP29" s="10"/>
     </row>
     <row r="30" spans="1:42" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="35" t="s">
         <v>79</v>
       </c>
       <c r="B30" s="9">
@@ -8110,7 +8235,7 @@
       <c r="AP30" s="10"/>
     </row>
     <row r="31" spans="1:42" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="39" t="s">
+      <c r="A31" s="35" t="s">
         <v>80</v>
       </c>
       <c r="B31" s="9">
@@ -8178,7 +8303,7 @@
       <c r="AP31" s="10"/>
     </row>
     <row r="32" spans="1:42" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="39" t="s">
+      <c r="A32" s="35" t="s">
         <v>81</v>
       </c>
       <c r="B32" s="9">
@@ -8246,7 +8371,7 @@
       <c r="AP32" s="10"/>
     </row>
     <row r="33" spans="1:42" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="39" t="s">
+      <c r="A33" s="35" t="s">
         <v>82</v>
       </c>
       <c r="B33" s="9">
@@ -8319,7 +8444,7 @@
       <c r="AP33" s="10"/>
     </row>
     <row r="34" spans="1:42" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="39" t="s">
+      <c r="A34" s="35" t="s">
         <v>83</v>
       </c>
       <c r="B34" s="9">
@@ -8387,7 +8512,7 @@
       <c r="AP34" s="10"/>
     </row>
     <row r="35" spans="1:42" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="39" t="s">
+      <c r="A35" s="35" t="s">
         <v>84</v>
       </c>
       <c r="B35" s="9">
@@ -8414,8 +8539,13 @@
         <f t="shared" si="3"/>
         <v>0.80089503661513428</v>
       </c>
-      <c r="I35" s="11"/>
-      <c r="J35" s="10"/>
+      <c r="I35" s="9">
+        <v>2319</v>
+      </c>
+      <c r="J35" s="10">
+        <f t="shared" si="2"/>
+        <v>0.18868999186330349</v>
+      </c>
       <c r="K35" s="9">
         <v>2319</v>
       </c>
@@ -8465,7 +8595,7 @@
       </c>
     </row>
     <row r="36" spans="1:42" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="39" t="s">
+      <c r="A36" s="35" t="s">
         <v>85</v>
       </c>
       <c r="B36" s="9">
@@ -8533,7 +8663,7 @@
       <c r="AP36" s="10"/>
     </row>
     <row r="37" spans="1:42" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="39" t="s">
+      <c r="A37" s="35" t="s">
         <v>86</v>
       </c>
       <c r="B37" s="9">
@@ -8560,8 +8690,13 @@
         <f t="shared" si="3"/>
         <v>0.67806402169427582</v>
       </c>
-      <c r="I37" s="11"/>
-      <c r="J37" s="10"/>
+      <c r="I37" s="9">
+        <v>5161</v>
+      </c>
+      <c r="J37" s="10">
+        <f t="shared" si="2"/>
+        <v>0.30425042740081354</v>
+      </c>
       <c r="K37" s="9">
         <v>5161</v>
       </c>
@@ -8606,7 +8741,7 @@
       <c r="AP37" s="10"/>
     </row>
     <row r="38" spans="1:42" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="39" t="s">
+      <c r="A38" s="35" t="s">
         <v>87</v>
       </c>
       <c r="B38" s="9">
@@ -8684,7 +8819,7 @@
       <c r="AP38" s="10"/>
     </row>
     <row r="39" spans="1:42" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="39" t="s">
+      <c r="A39" s="35" t="s">
         <v>88</v>
       </c>
       <c r="B39" s="9">
@@ -8752,7 +8887,7 @@
       <c r="AP39" s="10"/>
     </row>
     <row r="40" spans="1:42" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="39" t="s">
+      <c r="A40" s="35" t="s">
         <v>89</v>
       </c>
       <c r="B40" s="9">
@@ -8825,7 +8960,7 @@
       <c r="AP40" s="10"/>
     </row>
     <row r="41" spans="1:42" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="39" t="s">
+      <c r="A41" s="35" t="s">
         <v>90</v>
       </c>
       <c r="B41" s="9">
@@ -8852,8 +8987,13 @@
         <f t="shared" si="3"/>
         <v>0.3234848088689013</v>
       </c>
-      <c r="I41" s="11"/>
-      <c r="J41" s="10"/>
+      <c r="I41" s="9">
+        <v>12606</v>
+      </c>
+      <c r="J41" s="10">
+        <f t="shared" si="2"/>
+        <v>0.65920619149714998</v>
+      </c>
       <c r="K41" s="9">
         <v>12606</v>
       </c>
@@ -8898,7 +9038,7 @@
       <c r="AP41" s="10"/>
     </row>
     <row r="42" spans="1:42" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="35" t="s">
         <v>91</v>
       </c>
       <c r="B42" s="9">
@@ -8971,7 +9111,7 @@
       <c r="AP42" s="10"/>
     </row>
     <row r="43" spans="1:42" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="39" t="s">
+      <c r="A43" s="35" t="s">
         <v>92</v>
       </c>
       <c r="B43" s="9">
@@ -9039,7 +9179,7 @@
       <c r="AP43" s="10"/>
     </row>
     <row r="44" spans="1:42" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="39" t="s">
+      <c r="A44" s="35" t="s">
         <v>93</v>
       </c>
       <c r="B44" s="9">
@@ -9066,8 +9206,13 @@
         <f t="shared" si="3"/>
         <v>0.69483527047103033</v>
       </c>
-      <c r="I44" s="11"/>
-      <c r="J44" s="10"/>
+      <c r="I44" s="12">
+        <v>984</v>
+      </c>
+      <c r="J44" s="10">
+        <f t="shared" si="2"/>
+        <v>8.5991435812286993E-2</v>
+      </c>
       <c r="K44" s="11"/>
       <c r="L44" s="10"/>
       <c r="M44" s="11">
@@ -9127,7 +9272,7 @@
       <c r="AP44" s="10"/>
     </row>
     <row r="45" spans="1:42" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="39" t="s">
+      <c r="A45" s="35" t="s">
         <v>94</v>
       </c>
       <c r="B45" s="9">
@@ -9154,8 +9299,13 @@
         <f t="shared" si="3"/>
         <v>0.79195282173783221</v>
       </c>
-      <c r="I45" s="11"/>
-      <c r="J45" s="10"/>
+      <c r="I45" s="12">
+        <v>766</v>
+      </c>
+      <c r="J45" s="10">
+        <f t="shared" si="2"/>
+        <v>5.7181248133771276E-2</v>
+      </c>
       <c r="K45" s="11"/>
       <c r="L45" s="10"/>
       <c r="M45" s="11">
@@ -9210,7 +9360,7 @@
       <c r="AP45" s="10"/>
     </row>
     <row r="46" spans="1:42" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="39" t="s">
+      <c r="A46" s="35" t="s">
         <v>95</v>
       </c>
       <c r="B46" s="9">
@@ -9283,7 +9433,7 @@
       <c r="AP46" s="10"/>
     </row>
     <row r="47" spans="1:42" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="39" t="s">
+      <c r="A47" s="35" t="s">
         <v>96</v>
       </c>
       <c r="B47" s="9">
@@ -9389,11 +9539,11 @@
       </c>
       <c r="I48" s="14">
         <f>SUM(I7:I47)</f>
-        <v>290066</v>
+        <v>341597</v>
       </c>
       <c r="J48" s="15">
         <f>SUM(I48/F48)</f>
-        <v>0.3960810552475626</v>
+        <v>0.46644591310047245</v>
       </c>
       <c r="K48" s="14">
         <f>SUM(K7:K47)</f>
@@ -9587,6 +9737,10 @@
     <row r="74" spans="4:4" ht="16.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="AA4:AB4"/>
+    <mergeCell ref="AC4:AD4"/>
+    <mergeCell ref="AE4:AF4"/>
+    <mergeCell ref="AG4:AH4"/>
     <mergeCell ref="A1:AP1"/>
     <mergeCell ref="A2:AP2"/>
     <mergeCell ref="G4:H4"/>
@@ -9603,10 +9757,6 @@
     <mergeCell ref="AO4:AP4"/>
     <mergeCell ref="W4:X4"/>
     <mergeCell ref="Y4:Z4"/>
-    <mergeCell ref="AA4:AB4"/>
-    <mergeCell ref="AC4:AD4"/>
-    <mergeCell ref="AE4:AF4"/>
-    <mergeCell ref="AG4:AH4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -9618,7 +9768,7 @@
   <dimension ref="A1:AT49"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:A47"/>
+      <selection activeCell="J43" sqref="J43:J45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9627,96 +9777,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
-      <c r="S1" s="36"/>
-      <c r="T1" s="36"/>
-      <c r="U1" s="36"/>
-      <c r="V1" s="36"/>
-      <c r="W1" s="36"/>
-      <c r="X1" s="36"/>
-      <c r="Y1" s="36"/>
-      <c r="Z1" s="36"/>
-      <c r="AA1" s="36"/>
-      <c r="AB1" s="36"/>
-      <c r="AC1" s="36"/>
-      <c r="AD1" s="36"/>
-      <c r="AE1" s="36"/>
-      <c r="AF1" s="36"/>
-      <c r="AG1" s="36"/>
-      <c r="AH1" s="36"/>
-      <c r="AI1" s="36"/>
-      <c r="AJ1" s="36"/>
-      <c r="AK1" s="36"/>
-      <c r="AL1" s="36"/>
-      <c r="AM1" s="36"/>
-      <c r="AN1" s="36"/>
-      <c r="AO1" s="36"/>
-      <c r="AP1" s="36"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="37"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="37"/>
+      <c r="W1" s="37"/>
+      <c r="X1" s="37"/>
+      <c r="Y1" s="37"/>
+      <c r="Z1" s="37"/>
+      <c r="AA1" s="37"/>
+      <c r="AB1" s="37"/>
+      <c r="AC1" s="37"/>
+      <c r="AD1" s="37"/>
+      <c r="AE1" s="37"/>
+      <c r="AF1" s="37"/>
+      <c r="AG1" s="37"/>
+      <c r="AH1" s="37"/>
+      <c r="AI1" s="37"/>
+      <c r="AJ1" s="37"/>
+      <c r="AK1" s="37"/>
+      <c r="AL1" s="37"/>
+      <c r="AM1" s="37"/>
+      <c r="AN1" s="37"/>
+      <c r="AO1" s="37"/>
+      <c r="AP1" s="37"/>
     </row>
     <row r="2" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
-      <c r="O2" s="36"/>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="36"/>
-      <c r="R2" s="36"/>
-      <c r="S2" s="36"/>
-      <c r="T2" s="36"/>
-      <c r="U2" s="36"/>
-      <c r="V2" s="36"/>
-      <c r="W2" s="36"/>
-      <c r="X2" s="36"/>
-      <c r="Y2" s="36"/>
-      <c r="Z2" s="36"/>
-      <c r="AA2" s="36"/>
-      <c r="AB2" s="36"/>
-      <c r="AC2" s="36"/>
-      <c r="AD2" s="36"/>
-      <c r="AE2" s="36"/>
-      <c r="AF2" s="36"/>
-      <c r="AG2" s="36"/>
-      <c r="AH2" s="36"/>
-      <c r="AI2" s="36"/>
-      <c r="AJ2" s="36"/>
-      <c r="AK2" s="36"/>
-      <c r="AL2" s="36"/>
-      <c r="AM2" s="36"/>
-      <c r="AN2" s="36"/>
-      <c r="AO2" s="36"/>
-      <c r="AP2" s="36"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="37"/>
+      <c r="V2" s="37"/>
+      <c r="W2" s="37"/>
+      <c r="X2" s="37"/>
+      <c r="Y2" s="37"/>
+      <c r="Z2" s="37"/>
+      <c r="AA2" s="37"/>
+      <c r="AB2" s="37"/>
+      <c r="AC2" s="37"/>
+      <c r="AD2" s="37"/>
+      <c r="AE2" s="37"/>
+      <c r="AF2" s="37"/>
+      <c r="AG2" s="37"/>
+      <c r="AH2" s="37"/>
+      <c r="AI2" s="37"/>
+      <c r="AJ2" s="37"/>
+      <c r="AK2" s="37"/>
+      <c r="AL2" s="37"/>
+      <c r="AM2" s="37"/>
+      <c r="AN2" s="37"/>
+      <c r="AO2" s="37"/>
+      <c r="AP2" s="37"/>
     </row>
     <row r="3" spans="1:46" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D3" s="2"/>
@@ -9759,86 +9909,86 @@
       <c r="F4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35" t="s">
+      <c r="H4" s="36"/>
+      <c r="I4" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35" t="s">
+      <c r="J4" s="36"/>
+      <c r="K4" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="L4" s="35"/>
-      <c r="M4" s="37" t="s">
+      <c r="L4" s="36"/>
+      <c r="M4" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="38"/>
-      <c r="O4" s="35" t="s">
+      <c r="N4" s="39"/>
+      <c r="O4" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="P4" s="35"/>
-      <c r="Q4" s="35" t="s">
+      <c r="P4" s="36"/>
+      <c r="Q4" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="R4" s="35"/>
-      <c r="S4" s="35" t="s">
+      <c r="R4" s="36"/>
+      <c r="S4" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="T4" s="35"/>
-      <c r="U4" s="35" t="s">
+      <c r="T4" s="36"/>
+      <c r="U4" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="V4" s="35"/>
-      <c r="W4" s="35" t="s">
+      <c r="V4" s="36"/>
+      <c r="W4" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="X4" s="35"/>
-      <c r="Y4" s="35" t="s">
+      <c r="X4" s="36"/>
+      <c r="Y4" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="Z4" s="35"/>
-      <c r="AA4" s="37" t="s">
+      <c r="Z4" s="36"/>
+      <c r="AA4" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="AB4" s="38"/>
-      <c r="AC4" s="35" t="s">
+      <c r="AB4" s="39"/>
+      <c r="AC4" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="AD4" s="35"/>
-      <c r="AE4" s="35" t="s">
+      <c r="AD4" s="36"/>
+      <c r="AE4" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="AF4" s="35"/>
-      <c r="AG4" s="35" t="s">
+      <c r="AF4" s="36"/>
+      <c r="AG4" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="AH4" s="35"/>
-      <c r="AI4" s="35" t="s">
+      <c r="AH4" s="36"/>
+      <c r="AI4" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="AJ4" s="35"/>
-      <c r="AK4" s="37" t="s">
+      <c r="AJ4" s="36"/>
+      <c r="AK4" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="AL4" s="38"/>
-      <c r="AM4" s="37" t="s">
+      <c r="AL4" s="39"/>
+      <c r="AM4" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="AN4" s="38"/>
-      <c r="AO4" s="37" t="s">
+      <c r="AN4" s="39"/>
+      <c r="AO4" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="AP4" s="38"/>
-      <c r="AQ4" s="37" t="s">
+      <c r="AP4" s="39"/>
+      <c r="AQ4" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="AR4" s="38"/>
-      <c r="AS4" s="35" t="s">
+      <c r="AR4" s="39"/>
+      <c r="AS4" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="AT4" s="35"/>
+      <c r="AT4" s="36"/>
     </row>
     <row r="5" spans="1:46" s="1" customFormat="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
@@ -10071,7 +10221,7 @@
       </c>
     </row>
     <row r="7" spans="1:46" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="35" t="s">
         <v>56</v>
       </c>
       <c r="B7" s="24">
@@ -10152,7 +10302,7 @@
       <c r="AT7" s="10"/>
     </row>
     <row r="8" spans="1:46" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="35" t="s">
         <v>57</v>
       </c>
       <c r="B8" s="24">
@@ -10223,7 +10373,7 @@
       <c r="AT8" s="10"/>
     </row>
     <row r="9" spans="1:46" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="35" t="s">
         <v>58</v>
       </c>
       <c r="B9" s="24">
@@ -10300,7 +10450,7 @@
       <c r="AT9" s="10"/>
     </row>
     <row r="10" spans="1:46" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="35" t="s">
         <v>59</v>
       </c>
       <c r="B10" s="24">
@@ -10377,7 +10527,7 @@
       <c r="AT10" s="10"/>
     </row>
     <row r="11" spans="1:46" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="35" t="s">
         <v>60</v>
       </c>
       <c r="B11" s="24">
@@ -10454,7 +10604,7 @@
       <c r="AT11" s="10"/>
     </row>
     <row r="12" spans="1:46" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="35" t="s">
         <v>61</v>
       </c>
       <c r="B12" s="24">
@@ -10536,7 +10686,7 @@
       <c r="AT12" s="10"/>
     </row>
     <row r="13" spans="1:46" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="35" t="s">
         <v>62</v>
       </c>
       <c r="B13" s="24">
@@ -10613,7 +10763,7 @@
       <c r="AT13" s="10"/>
     </row>
     <row r="14" spans="1:46" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="35" t="s">
         <v>63</v>
       </c>
       <c r="B14" s="24">
@@ -10695,7 +10845,7 @@
       <c r="AT14" s="10"/>
     </row>
     <row r="15" spans="1:46" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="35" t="s">
         <v>64</v>
       </c>
       <c r="B15" s="24">
@@ -10772,7 +10922,7 @@
       <c r="AT15" s="10"/>
     </row>
     <row r="16" spans="1:46" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="35" t="s">
         <v>65</v>
       </c>
       <c r="B16" s="24">
@@ -10854,7 +11004,7 @@
       <c r="AT16" s="10"/>
     </row>
     <row r="17" spans="1:46" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="35" t="s">
         <v>66</v>
       </c>
       <c r="B17" s="24">
@@ -10931,7 +11081,7 @@
       <c r="AT17" s="10"/>
     </row>
     <row r="18" spans="1:46" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="35" t="s">
         <v>67</v>
       </c>
       <c r="B18" s="24">
@@ -11023,7 +11173,7 @@
       <c r="AT18" s="10"/>
     </row>
     <row r="19" spans="1:46" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="39" t="s">
+      <c r="A19" s="35" t="s">
         <v>68</v>
       </c>
       <c r="B19" s="24">
@@ -11110,7 +11260,7 @@
       <c r="AT19" s="10"/>
     </row>
     <row r="20" spans="1:46" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="39" t="s">
+      <c r="A20" s="35" t="s">
         <v>69</v>
       </c>
       <c r="B20" s="24">
@@ -11192,7 +11342,7 @@
       <c r="AT20" s="10"/>
     </row>
     <row r="21" spans="1:46" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="35" t="s">
         <v>70</v>
       </c>
       <c r="B21" s="24">
@@ -11274,7 +11424,7 @@
       <c r="AT21" s="10"/>
     </row>
     <row r="22" spans="1:46" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="35" t="s">
         <v>71</v>
       </c>
       <c r="B22" s="24">
@@ -11361,7 +11511,7 @@
       <c r="AT22" s="10"/>
     </row>
     <row r="23" spans="1:46" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="35" t="s">
         <v>72</v>
       </c>
       <c r="B23" s="24">
@@ -11438,7 +11588,7 @@
       <c r="AT23" s="10"/>
     </row>
     <row r="24" spans="1:46" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="39" t="s">
+      <c r="A24" s="35" t="s">
         <v>73</v>
       </c>
       <c r="B24" s="24">
@@ -11520,7 +11670,7 @@
       <c r="AT24" s="10"/>
     </row>
     <row r="25" spans="1:46" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="39" t="s">
+      <c r="A25" s="35" t="s">
         <v>74</v>
       </c>
       <c r="B25" s="24">
@@ -11612,7 +11762,7 @@
       <c r="AT25" s="10"/>
     </row>
     <row r="26" spans="1:46" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="39" t="s">
+      <c r="A26" s="35" t="s">
         <v>75</v>
       </c>
       <c r="B26" s="24">
@@ -11694,7 +11844,7 @@
       <c r="AT26" s="10"/>
     </row>
     <row r="27" spans="1:46" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="39" t="s">
+      <c r="A27" s="35" t="s">
         <v>76</v>
       </c>
       <c r="B27" s="24">
@@ -11771,7 +11921,7 @@
       <c r="AT27" s="10"/>
     </row>
     <row r="28" spans="1:46" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="39" t="s">
+      <c r="A28" s="35" t="s">
         <v>77</v>
       </c>
       <c r="B28" s="24">
@@ -11858,7 +12008,7 @@
       <c r="AT28" s="10"/>
     </row>
     <row r="29" spans="1:46" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="35" t="s">
         <v>78</v>
       </c>
       <c r="B29" s="24">
@@ -11930,7 +12080,7 @@
       <c r="AT29" s="10"/>
     </row>
     <row r="30" spans="1:46" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="35" t="s">
         <v>79</v>
       </c>
       <c r="B30" s="24">
@@ -12002,7 +12152,7 @@
       <c r="AT30" s="10"/>
     </row>
     <row r="31" spans="1:46" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="39" t="s">
+      <c r="A31" s="35" t="s">
         <v>80</v>
       </c>
       <c r="B31" s="24">
@@ -12079,7 +12229,7 @@
       <c r="AT31" s="10"/>
     </row>
     <row r="32" spans="1:46" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="39" t="s">
+      <c r="A32" s="35" t="s">
         <v>81</v>
       </c>
       <c r="B32" s="24">
@@ -12166,7 +12316,7 @@
       <c r="AT32" s="10"/>
     </row>
     <row r="33" spans="1:46" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="39" t="s">
+      <c r="A33" s="35" t="s">
         <v>82</v>
       </c>
       <c r="B33" s="24">
@@ -12248,7 +12398,7 @@
       <c r="AT33" s="10"/>
     </row>
     <row r="34" spans="1:46" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="39" t="s">
+      <c r="A34" s="35" t="s">
         <v>83</v>
       </c>
       <c r="B34" s="24">
@@ -12330,7 +12480,7 @@
       <c r="AT34" s="10"/>
     </row>
     <row r="35" spans="1:46" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="39" t="s">
+      <c r="A35" s="35" t="s">
         <v>84</v>
       </c>
       <c r="B35" s="24">
@@ -12412,7 +12562,7 @@
       <c r="AT35" s="10"/>
     </row>
     <row r="36" spans="1:46" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="39" t="s">
+      <c r="A36" s="35" t="s">
         <v>85</v>
       </c>
       <c r="B36" s="24">
@@ -12489,7 +12639,7 @@
       <c r="AT36" s="10"/>
     </row>
     <row r="37" spans="1:46" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="39" t="s">
+      <c r="A37" s="35" t="s">
         <v>86</v>
       </c>
       <c r="B37" s="24">
@@ -12561,7 +12711,7 @@
       <c r="AT37" s="10"/>
     </row>
     <row r="38" spans="1:46" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="39" t="s">
+      <c r="A38" s="35" t="s">
         <v>87</v>
       </c>
       <c r="B38" s="24">
@@ -12648,7 +12798,7 @@
       <c r="AT38" s="10"/>
     </row>
     <row r="39" spans="1:46" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="39" t="s">
+      <c r="A39" s="35" t="s">
         <v>88</v>
       </c>
       <c r="B39" s="24">
@@ -12720,7 +12870,7 @@
       <c r="AT39" s="10"/>
     </row>
     <row r="40" spans="1:46" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="39" t="s">
+      <c r="A40" s="35" t="s">
         <v>89</v>
       </c>
       <c r="B40" s="24">
@@ -12797,7 +12947,7 @@
       <c r="AT40" s="10"/>
     </row>
     <row r="41" spans="1:46" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="39" t="s">
+      <c r="A41" s="35" t="s">
         <v>90</v>
       </c>
       <c r="B41" s="24">
@@ -12884,7 +13034,7 @@
       <c r="AT41" s="10"/>
     </row>
     <row r="42" spans="1:46" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="35" t="s">
         <v>91</v>
       </c>
       <c r="B42" s="24">
@@ -12966,7 +13116,7 @@
       <c r="AT42" s="10"/>
     </row>
     <row r="43" spans="1:46" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="39" t="s">
+      <c r="A43" s="35" t="s">
         <v>92</v>
       </c>
       <c r="B43" s="24">
@@ -13043,7 +13193,7 @@
       <c r="AT43" s="10"/>
     </row>
     <row r="44" spans="1:46" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="39" t="s">
+      <c r="A44" s="35" t="s">
         <v>93</v>
       </c>
       <c r="B44" s="24">
@@ -13070,8 +13220,13 @@
         <f t="shared" si="3"/>
         <v>0.54516943318289601</v>
       </c>
-      <c r="I44" s="21"/>
-      <c r="J44" s="10"/>
+      <c r="I44" s="27">
+        <v>5866</v>
+      </c>
+      <c r="J44" s="10">
+        <f t="shared" si="4"/>
+        <v>0.4487110839134093</v>
+      </c>
       <c r="K44" s="21"/>
       <c r="L44" s="10"/>
       <c r="M44" s="21"/>
@@ -13120,7 +13275,7 @@
       <c r="AT44" s="10"/>
     </row>
     <row r="45" spans="1:46" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="39" t="s">
+      <c r="A45" s="35" t="s">
         <v>94</v>
       </c>
       <c r="B45" s="24">
@@ -13147,8 +13302,13 @@
         <f t="shared" si="3"/>
         <v>0.66924020492099001</v>
       </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="10"/>
+      <c r="I45" s="27">
+        <v>4501</v>
+      </c>
+      <c r="J45" s="10">
+        <f t="shared" si="4"/>
+        <v>0.32477090699184646</v>
+      </c>
       <c r="K45" s="21"/>
       <c r="L45" s="10"/>
       <c r="M45" s="21"/>
@@ -13202,7 +13362,7 @@
       </c>
     </row>
     <row r="46" spans="1:46" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="39" t="s">
+      <c r="A46" s="35" t="s">
         <v>95</v>
       </c>
       <c r="B46" s="24">
@@ -13279,7 +13439,7 @@
       <c r="AT46" s="10"/>
     </row>
     <row r="47" spans="1:46" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="39" t="s">
+      <c r="A47" s="35" t="s">
         <v>96</v>
       </c>
       <c r="B47" s="19">
@@ -13399,11 +13559,11 @@
       </c>
       <c r="I48" s="14">
         <f>SUM(I7:I47)</f>
-        <v>309188</v>
+        <v>319555</v>
       </c>
       <c r="J48" s="15">
         <f>SUM(I48/F48)</f>
-        <v>0.47094842213969978</v>
+        <v>0.4867392105672011</v>
       </c>
       <c r="K48" s="14">
         <f>SUM(K7:K47)</f>
@@ -13555,6 +13715,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="AS4:AT4"/>
+    <mergeCell ref="AG4:AH4"/>
+    <mergeCell ref="AK4:AL4"/>
+    <mergeCell ref="AM4:AN4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AQ4:AR4"/>
     <mergeCell ref="A1:AP1"/>
     <mergeCell ref="A2:AP2"/>
     <mergeCell ref="AI4:AJ4"/>
@@ -13571,12 +13737,6 @@
     <mergeCell ref="AA4:AB4"/>
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AE4:AF4"/>
-    <mergeCell ref="AG4:AH4"/>
-    <mergeCell ref="AK4:AL4"/>
-    <mergeCell ref="AM4:AN4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AQ4:AR4"/>
-    <mergeCell ref="AS4:AT4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
changes to excel file
</commit_message>
<xml_diff>
--- a/csvs/collated-tt-election-results.xlsx
+++ b/csvs/collated-tt-election-results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophegittens/Desktop/my docs/U.W.I. YEAR 4/U.W.I. YEAR 4 - SEMESTER II/COMP 3610/Assignments/Election-Project/csvs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE7EDA57-0421-5D49-AA4F-977BDB44FBFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A65ED4-62DE-E949-BADC-6EE91521888D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="24000" windowHeight="21600" activeTab="4" xr2:uid="{00CD0EB4-DA0B-AB45-875C-9354388CE2C5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{00CD0EB4-DA0B-AB45-875C-9354388CE2C5}"/>
   </bookViews>
   <sheets>
     <sheet name="2007" sheetId="1" r:id="rId1"/>
@@ -982,7 +982,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B489430B-CE8D-294E-B0B8-BF19555E0C9E}">
   <dimension ref="A1:R74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="H32" sqref="H32"/>
@@ -3424,8 +3424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D39057C-680C-4843-89F6-29B9284CAFAA}">
   <dimension ref="A1:V74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K50" sqref="K50"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7:P47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3659,46 +3659,41 @@
       </c>
       <c r="C7" s="9">
         <f>SUM(E7,F7)</f>
-        <v>22740</v>
+        <v>15130</v>
       </c>
       <c r="D7" s="10">
         <f>SUM(C7/B7)</f>
-        <v>0.94298154675513168</v>
+        <v>0.62741032552353304</v>
       </c>
       <c r="E7" s="11">
         <v>73</v>
       </c>
       <c r="F7" s="9">
         <f>SUM(G7,I7,K7,M7,O7,Q7,S7,U7)</f>
-        <v>22667</v>
+        <v>15057</v>
       </c>
       <c r="G7" s="9">
         <v>7246</v>
       </c>
       <c r="H7" s="10">
         <f t="shared" ref="H7" si="0">SUM(G7/F7)</f>
-        <v>0.31967176953280096</v>
+        <v>0.4812379624095105</v>
       </c>
       <c r="I7" s="9">
         <v>7610</v>
       </c>
       <c r="J7" s="10">
         <f t="shared" ref="J7:J47" si="1">SUM(I7/F7)</f>
-        <v>0.33573035690651609</v>
-      </c>
-      <c r="K7" s="9">
-        <v>7610</v>
-      </c>
-      <c r="L7" s="10">
-        <f t="shared" ref="L7:L47" si="2">SUM(K7/F7)</f>
-        <v>0.33573035690651609</v>
-      </c>
+        <v>0.50541276482699082</v>
+      </c>
+      <c r="K7" s="9"/>
+      <c r="L7" s="10"/>
       <c r="M7" s="11">
         <v>201</v>
       </c>
       <c r="N7" s="10">
         <f>SUM(M7/F7)</f>
-        <v>8.8675166541668498E-3</v>
+        <v>1.3349272763498704E-2</v>
       </c>
       <c r="O7" s="10"/>
       <c r="P7" s="10"/>
@@ -3717,41 +3712,36 @@
         <v>25019</v>
       </c>
       <c r="C8" s="9">
-        <f t="shared" ref="C8:C47" si="3">SUM(E8,F8)</f>
-        <v>22716</v>
+        <f t="shared" ref="C8:C47" si="2">SUM(E8,F8)</f>
+        <v>17196</v>
       </c>
       <c r="D8" s="10">
         <f>SUM(C8/B8)</f>
-        <v>0.90794995803189571</v>
+        <v>0.6873176385946681</v>
       </c>
       <c r="E8" s="11">
         <v>46</v>
       </c>
       <c r="F8" s="9">
-        <f t="shared" ref="F8:F47" si="4">SUM(G8,I8,K8,M8,O8,Q8,S8,U8)</f>
-        <v>22670</v>
+        <f t="shared" ref="F8:F47" si="3">SUM(G8,I8,K8,M8,O8,Q8,S8,U8)</f>
+        <v>17150</v>
       </c>
       <c r="G8" s="9">
         <v>11517</v>
       </c>
       <c r="H8" s="10">
         <f>SUM(G8/F8)</f>
-        <v>0.50802823114247908</v>
+        <v>0.67154518950437314</v>
       </c>
       <c r="I8" s="9">
         <v>5520</v>
       </c>
       <c r="J8" s="10">
         <f t="shared" si="1"/>
-        <v>0.24349360388178209</v>
-      </c>
-      <c r="K8" s="9">
-        <v>5520</v>
-      </c>
-      <c r="L8" s="10">
-        <f t="shared" si="2"/>
-        <v>0.24349360388178209</v>
-      </c>
+        <v>0.32186588921282799</v>
+      </c>
+      <c r="K8" s="9"/>
+      <c r="L8" s="10"/>
       <c r="M8" s="11"/>
       <c r="N8" s="10"/>
       <c r="O8" s="10"/>
@@ -3763,7 +3753,7 @@
       </c>
       <c r="T8" s="10">
         <f>SUM(S8/F8)</f>
-        <v>4.9845610939567714E-3</v>
+        <v>6.588921282798834E-3</v>
       </c>
       <c r="U8" s="11"/>
       <c r="V8" s="10">
@@ -3779,18 +3769,18 @@
         <v>25394</v>
       </c>
       <c r="C9" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>17768</v>
       </c>
       <c r="D9" s="10">
-        <f t="shared" ref="D9:D47" si="5">SUM(C9/B9)</f>
+        <f t="shared" ref="D9:D47" si="4">SUM(C9/B9)</f>
         <v>0.69969284082854222</v>
       </c>
       <c r="E9" s="11">
         <v>76</v>
       </c>
       <c r="F9" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>17692</v>
       </c>
       <c r="G9" s="9">
@@ -3828,25 +3818,25 @@
         <v>24601</v>
       </c>
       <c r="C10" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>18793</v>
       </c>
       <c r="D10" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.76391203609609371</v>
       </c>
       <c r="E10" s="11">
         <v>50</v>
       </c>
       <c r="F10" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>18743</v>
       </c>
       <c r="G10" s="9">
         <v>4880</v>
       </c>
       <c r="H10" s="10">
-        <f t="shared" ref="H10:H47" si="6">SUM(G10/F10)</f>
+        <f t="shared" ref="H10:H47" si="5">SUM(G10/F10)</f>
         <v>0.26036386917782639</v>
       </c>
       <c r="I10" s="9">
@@ -3877,25 +3867,25 @@
         <v>25166</v>
       </c>
       <c r="C11" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>18762</v>
       </c>
       <c r="D11" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.74552968290550747</v>
       </c>
       <c r="E11" s="11">
         <v>57</v>
       </c>
       <c r="F11" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>18705</v>
       </c>
       <c r="G11" s="9">
         <v>3724</v>
       </c>
       <c r="H11" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.19909115209836942</v>
       </c>
       <c r="I11" s="9">
@@ -3926,25 +3916,25 @@
         <v>23653</v>
       </c>
       <c r="C12" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>17611</v>
       </c>
       <c r="D12" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.74455671584999794</v>
       </c>
       <c r="E12" s="11">
         <v>58</v>
       </c>
       <c r="F12" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>17553</v>
       </c>
       <c r="G12" s="9">
         <v>6717</v>
       </c>
       <c r="H12" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.38266962912322677</v>
       </c>
       <c r="I12" s="9">
@@ -3980,25 +3970,25 @@
         <v>25715</v>
       </c>
       <c r="C13" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>20281</v>
       </c>
       <c r="D13" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.78868364767645338</v>
       </c>
       <c r="E13" s="11">
         <v>70</v>
       </c>
       <c r="F13" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>20211</v>
       </c>
       <c r="G13" s="9">
         <v>1471</v>
       </c>
       <c r="H13" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>7.2782148335065064E-2</v>
       </c>
       <c r="I13" s="9">
@@ -4029,25 +4019,25 @@
         <v>27680</v>
       </c>
       <c r="C14" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>21286</v>
       </c>
       <c r="D14" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.76900289017341039</v>
       </c>
       <c r="E14" s="11">
         <v>70</v>
       </c>
       <c r="F14" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>21216</v>
       </c>
       <c r="G14" s="9">
         <v>5159</v>
       </c>
       <c r="H14" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.24316553544494721</v>
       </c>
       <c r="I14" s="9">
@@ -4078,25 +4068,25 @@
         <v>26400</v>
       </c>
       <c r="C15" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>19877</v>
       </c>
       <c r="D15" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.75291666666666668</v>
       </c>
       <c r="E15" s="11">
         <v>59</v>
       </c>
       <c r="F15" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>19818</v>
       </c>
       <c r="G15" s="9">
         <v>4773</v>
       </c>
       <c r="H15" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.2408416590977899</v>
       </c>
       <c r="I15" s="9">
@@ -4127,25 +4117,25 @@
         <v>26896</v>
       </c>
       <c r="C16" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>20527</v>
       </c>
       <c r="D16" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.76319898869720404</v>
       </c>
       <c r="E16" s="11">
         <v>121</v>
       </c>
       <c r="F16" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>20406</v>
       </c>
       <c r="G16" s="9">
         <v>7181</v>
       </c>
       <c r="H16" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.35190630206801921</v>
       </c>
       <c r="I16" s="9">
@@ -4167,7 +4157,7 @@
         <v>109</v>
       </c>
       <c r="T16" s="10">
-        <f t="shared" ref="T16" si="7">SUM(S16/F16)</f>
+        <f t="shared" ref="T16" si="6">SUM(S16/F16)</f>
         <v>5.3415662060178381E-3</v>
       </c>
       <c r="U16" s="11"/>
@@ -4181,41 +4171,36 @@
         <v>26019</v>
       </c>
       <c r="C17" s="9">
-        <f t="shared" si="3"/>
-        <v>27816</v>
+        <f t="shared" si="2"/>
+        <v>18121</v>
       </c>
       <c r="D17" s="10">
-        <f t="shared" si="5"/>
-        <v>1.0690649141012336</v>
+        <f t="shared" si="4"/>
+        <v>0.69645259233636958</v>
       </c>
       <c r="E17" s="11">
         <v>74</v>
       </c>
       <c r="F17" s="9">
-        <f t="shared" si="4"/>
-        <v>27742</v>
+        <f t="shared" si="3"/>
+        <v>18047</v>
       </c>
       <c r="G17" s="9">
         <v>8352</v>
       </c>
       <c r="H17" s="10">
-        <f t="shared" si="6"/>
-        <v>0.30105976497729076</v>
+        <f t="shared" si="5"/>
+        <v>0.46279159971186346</v>
       </c>
       <c r="I17" s="9">
         <v>9695</v>
       </c>
       <c r="J17" s="10">
         <f t="shared" si="1"/>
-        <v>0.34947011751135465</v>
-      </c>
-      <c r="K17" s="9">
-        <v>9695</v>
-      </c>
-      <c r="L17" s="10">
-        <f>SUM(K17/F17)</f>
-        <v>0.34947011751135465</v>
-      </c>
+        <v>0.53720840028813654</v>
+      </c>
+      <c r="K17" s="9"/>
+      <c r="L17" s="10"/>
       <c r="M17" s="11"/>
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
@@ -4235,47 +4220,42 @@
         <v>27465</v>
       </c>
       <c r="C18" s="9">
-        <f t="shared" si="3"/>
-        <v>25312</v>
+        <f t="shared" si="2"/>
+        <v>17265</v>
       </c>
       <c r="D18" s="10">
-        <f t="shared" si="5"/>
-        <v>0.92160932095394132</v>
+        <f t="shared" si="4"/>
+        <v>0.62861824139814304</v>
       </c>
       <c r="E18" s="11">
         <v>33</v>
       </c>
       <c r="F18" s="9">
-        <f t="shared" si="4"/>
-        <v>25279</v>
+        <f t="shared" si="3"/>
+        <v>17232</v>
       </c>
       <c r="G18" s="9">
         <v>9040</v>
       </c>
       <c r="H18" s="10">
-        <f t="shared" si="6"/>
-        <v>0.35760908263776259</v>
+        <f t="shared" si="5"/>
+        <v>0.52460538532961931</v>
       </c>
       <c r="I18" s="11">
         <v>8047</v>
       </c>
       <c r="J18" s="10">
         <f t="shared" si="1"/>
-        <v>0.31832746548518531</v>
-      </c>
-      <c r="K18" s="11">
-        <v>8047</v>
-      </c>
-      <c r="L18" s="10">
-        <f t="shared" si="2"/>
-        <v>0.31832746548518531</v>
-      </c>
+        <v>0.46698003714020425</v>
+      </c>
+      <c r="K18" s="11"/>
+      <c r="L18" s="10"/>
       <c r="M18" s="11">
         <v>145</v>
       </c>
       <c r="N18" s="10">
         <f>SUM(M18/F18)</f>
-        <v>5.7359863918667667E-3</v>
+        <v>8.4145775301764161E-3</v>
       </c>
       <c r="O18" s="10"/>
       <c r="P18" s="10"/>
@@ -4294,25 +4274,25 @@
         <v>27647</v>
       </c>
       <c r="C19" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>16809</v>
       </c>
       <c r="D19" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.60798639997106374</v>
       </c>
       <c r="E19" s="11">
         <v>68</v>
       </c>
       <c r="F19" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>16741</v>
       </c>
       <c r="G19" s="9">
         <v>8539</v>
       </c>
       <c r="H19" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.51006510961113438</v>
       </c>
       <c r="I19" s="9">
@@ -4348,47 +4328,42 @@
         <v>28366</v>
       </c>
       <c r="C20" s="9">
-        <f t="shared" si="3"/>
-        <v>25244</v>
+        <f t="shared" si="2"/>
+        <v>17248</v>
       </c>
       <c r="D20" s="10">
-        <f t="shared" si="5"/>
-        <v>0.88993865895790736</v>
+        <f t="shared" si="4"/>
+        <v>0.60805189311147145</v>
       </c>
       <c r="E20" s="11">
         <v>61</v>
       </c>
       <c r="F20" s="9">
         <f>SUM(G20,K20,I20,M20,O20,Q20,S20,U20)</f>
-        <v>25183</v>
+        <v>17187</v>
       </c>
       <c r="G20" s="9">
         <v>9042</v>
       </c>
       <c r="H20" s="10">
-        <f t="shared" si="6"/>
-        <v>0.35905174125402056</v>
+        <f t="shared" si="5"/>
+        <v>0.52609530459067899</v>
       </c>
       <c r="I20" s="11">
         <v>7996</v>
       </c>
       <c r="J20" s="10">
         <f t="shared" si="1"/>
-        <v>0.31751578445776912</v>
-      </c>
-      <c r="K20" s="11">
-        <v>7996</v>
-      </c>
-      <c r="L20" s="10">
-        <f>SUM(K20/F20)</f>
-        <v>0.31751578445776912</v>
-      </c>
+        <v>0.46523535230115787</v>
+      </c>
+      <c r="K20" s="11"/>
+      <c r="L20" s="10"/>
       <c r="M20" s="11">
         <v>149</v>
       </c>
       <c r="N20" s="10">
         <f>SUM(M20/F20)</f>
-        <v>5.9166898304411708E-3</v>
+        <v>8.6693431081631463E-3</v>
       </c>
       <c r="O20" s="10"/>
       <c r="P20" s="10"/>
@@ -4407,25 +4382,25 @@
         <v>25802</v>
       </c>
       <c r="C21" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>20245</v>
       </c>
       <c r="D21" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.78462909851949458</v>
       </c>
       <c r="E21" s="11">
         <v>59</v>
       </c>
       <c r="F21" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>20186</v>
       </c>
       <c r="G21" s="9">
         <v>7298</v>
       </c>
       <c r="H21" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.36153769939562075</v>
       </c>
       <c r="I21" s="9">
@@ -4456,25 +4431,25 @@
         <v>24057</v>
       </c>
       <c r="C22" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>17098</v>
       </c>
       <c r="D22" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.71072868603732797</v>
       </c>
       <c r="E22" s="11">
         <v>67</v>
       </c>
       <c r="F22" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>17031</v>
       </c>
       <c r="G22" s="9">
         <v>9680</v>
       </c>
       <c r="H22" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.56837531560096299</v>
       </c>
       <c r="I22" s="9">
@@ -4510,25 +4485,25 @@
         <v>23959</v>
       </c>
       <c r="C23" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>16483</v>
       </c>
       <c r="D23" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.68796694352852794</v>
       </c>
       <c r="E23" s="11">
         <v>51</v>
       </c>
       <c r="F23" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>16432</v>
       </c>
       <c r="G23" s="9">
         <v>7633</v>
       </c>
       <c r="H23" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.46452044790652386</v>
       </c>
       <c r="I23" s="9">
@@ -4569,47 +4544,42 @@
         <v>27426</v>
       </c>
       <c r="C24" s="9">
-        <f t="shared" si="3"/>
-        <v>18768</v>
+        <f t="shared" si="2"/>
+        <v>15038</v>
       </c>
       <c r="D24" s="10">
-        <f t="shared" si="5"/>
-        <v>0.68431415445197985</v>
+        <f t="shared" si="4"/>
+        <v>0.54831182089987607</v>
       </c>
       <c r="E24" s="11">
         <v>62</v>
       </c>
       <c r="F24" s="9">
-        <f t="shared" si="4"/>
-        <v>18706</v>
+        <f t="shared" si="3"/>
+        <v>14976</v>
       </c>
       <c r="G24" s="9">
         <v>10797</v>
       </c>
       <c r="H24" s="10">
-        <f t="shared" si="6"/>
-        <v>0.57719448305356569</v>
+        <f t="shared" si="5"/>
+        <v>0.72095352564102566</v>
       </c>
       <c r="I24" s="11">
         <v>3730</v>
       </c>
       <c r="J24" s="10">
         <f t="shared" si="1"/>
-        <v>0.19940126162728536</v>
-      </c>
-      <c r="K24" s="11">
-        <v>3730</v>
-      </c>
-      <c r="L24" s="10">
-        <f t="shared" si="2"/>
-        <v>0.19940126162728536</v>
-      </c>
+        <v>0.24906517094017094</v>
+      </c>
+      <c r="K24" s="11"/>
+      <c r="L24" s="10"/>
       <c r="M24" s="11">
         <v>449</v>
       </c>
       <c r="N24" s="10">
         <f>SUM(M24/F24)</f>
-        <v>2.4002993691863574E-2</v>
+        <v>2.998130341880342E-2</v>
       </c>
       <c r="O24" s="10"/>
       <c r="P24" s="10"/>
@@ -4628,41 +4598,36 @@
         <v>27426</v>
       </c>
       <c r="C25" s="9">
-        <f t="shared" si="3"/>
-        <v>16219</v>
+        <f t="shared" si="2"/>
+        <v>13494</v>
       </c>
       <c r="D25" s="10">
-        <f t="shared" si="5"/>
-        <v>0.59137314956610521</v>
+        <f t="shared" si="4"/>
+        <v>0.49201487639466202</v>
       </c>
       <c r="E25" s="11">
         <v>39</v>
       </c>
       <c r="F25" s="9">
-        <f t="shared" si="4"/>
-        <v>16180</v>
+        <f t="shared" si="3"/>
+        <v>13455</v>
       </c>
       <c r="G25" s="9">
         <v>10730</v>
       </c>
       <c r="H25" s="10">
-        <f t="shared" si="6"/>
-        <v>0.66316440049443759</v>
+        <f t="shared" si="5"/>
+        <v>0.79747305834262361</v>
       </c>
       <c r="I25" s="11">
         <v>2725</v>
       </c>
       <c r="J25" s="10">
         <f t="shared" si="1"/>
-        <v>0.16841779975278121</v>
-      </c>
-      <c r="K25" s="11">
-        <v>2725</v>
-      </c>
-      <c r="L25" s="10">
-        <f t="shared" si="2"/>
-        <v>0.16841779975278121</v>
-      </c>
+        <v>0.20252694165737645</v>
+      </c>
+      <c r="K25" s="11"/>
+      <c r="L25" s="10"/>
       <c r="M25" s="11"/>
       <c r="N25" s="10"/>
       <c r="O25" s="10"/>
@@ -4682,41 +4647,36 @@
         <v>24447</v>
       </c>
       <c r="C26" s="9">
-        <f t="shared" si="3"/>
-        <v>26811</v>
+        <f t="shared" si="2"/>
+        <v>17559</v>
       </c>
       <c r="D26" s="10">
-        <f t="shared" si="5"/>
-        <v>1.0966989814701191</v>
+        <f t="shared" si="4"/>
+        <v>0.71824763774696276</v>
       </c>
       <c r="E26" s="11">
         <v>58</v>
       </c>
       <c r="F26" s="9">
-        <f t="shared" si="4"/>
-        <v>26753</v>
+        <f t="shared" si="3"/>
+        <v>17501</v>
       </c>
       <c r="G26" s="9">
         <v>8249</v>
       </c>
       <c r="H26" s="10">
-        <f t="shared" si="6"/>
-        <v>0.30833925167270959</v>
+        <f t="shared" si="5"/>
+        <v>0.47134449460030853</v>
       </c>
       <c r="I26" s="9">
         <v>9252</v>
       </c>
       <c r="J26" s="10">
         <f t="shared" si="1"/>
-        <v>0.3458303741636452</v>
-      </c>
-      <c r="K26" s="9">
-        <v>9252</v>
-      </c>
-      <c r="L26" s="10">
-        <f t="shared" si="2"/>
-        <v>0.3458303741636452</v>
-      </c>
+        <v>0.52865550539969142</v>
+      </c>
+      <c r="K26" s="9"/>
+      <c r="L26" s="10"/>
       <c r="M26" s="11"/>
       <c r="N26" s="10"/>
       <c r="O26" s="10"/>
@@ -4736,25 +4696,25 @@
         <v>26433</v>
       </c>
       <c r="C27" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>20305</v>
       </c>
       <c r="D27" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.76816857715734121</v>
       </c>
       <c r="E27" s="11">
         <v>129</v>
       </c>
       <c r="F27" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>20176</v>
       </c>
       <c r="G27" s="9">
         <v>7330</v>
       </c>
       <c r="H27" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.36330293417922283</v>
       </c>
       <c r="I27" s="9">
@@ -4785,25 +4745,25 @@
         <v>26450</v>
       </c>
       <c r="C28" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>20433</v>
       </c>
       <c r="D28" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.77251417769376185</v>
       </c>
       <c r="E28" s="11">
         <v>124</v>
       </c>
       <c r="F28" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>20309</v>
       </c>
       <c r="G28" s="9">
         <v>8681</v>
       </c>
       <c r="H28" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.42744595991924761</v>
       </c>
       <c r="I28" s="9">
@@ -4834,25 +4794,25 @@
         <v>25394</v>
       </c>
       <c r="C29" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>19230</v>
       </c>
       <c r="D29" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.75726549578640623</v>
       </c>
       <c r="E29" s="11">
         <v>62</v>
       </c>
       <c r="F29" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>19168</v>
       </c>
       <c r="G29" s="9">
         <v>2553</v>
       </c>
       <c r="H29" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.133190734557596</v>
       </c>
       <c r="I29" s="9">
@@ -4883,25 +4843,25 @@
         <v>27181</v>
       </c>
       <c r="C30" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>20861</v>
       </c>
       <c r="D30" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.76748464000588645</v>
       </c>
       <c r="E30" s="11">
         <v>62</v>
       </c>
       <c r="F30" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>20799</v>
       </c>
       <c r="G30" s="9">
         <v>2872</v>
       </c>
       <c r="H30" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.13808356170969757</v>
       </c>
       <c r="I30" s="9">
@@ -4932,25 +4892,25 @@
         <v>23427</v>
       </c>
       <c r="C31" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>17772</v>
       </c>
       <c r="D31" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.75861185811243437</v>
       </c>
       <c r="E31" s="11">
         <v>58</v>
       </c>
       <c r="F31" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>17714</v>
       </c>
       <c r="G31" s="9">
         <v>3526</v>
       </c>
       <c r="H31" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.199051597606413</v>
       </c>
       <c r="I31" s="9">
@@ -4981,41 +4941,36 @@
         <v>24607</v>
       </c>
       <c r="C32" s="9">
-        <f t="shared" si="3"/>
-        <v>24981</v>
+        <f t="shared" si="2"/>
+        <v>16888</v>
       </c>
       <c r="D32" s="10">
-        <f t="shared" si="5"/>
-        <v>1.0151989271345552</v>
+        <f t="shared" si="4"/>
+        <v>0.68630877392611855</v>
       </c>
       <c r="E32" s="11">
         <v>47</v>
       </c>
       <c r="F32" s="9">
-        <f t="shared" si="4"/>
-        <v>24934</v>
+        <f t="shared" si="3"/>
+        <v>16841</v>
       </c>
       <c r="G32" s="9">
         <v>8748</v>
       </c>
       <c r="H32" s="10">
-        <f t="shared" si="6"/>
-        <v>0.35084623405791288</v>
+        <f t="shared" si="5"/>
+        <v>0.51944658868238225</v>
       </c>
       <c r="I32" s="11">
         <v>8093</v>
       </c>
       <c r="J32" s="10">
         <f t="shared" si="1"/>
-        <v>0.32457688297104353</v>
-      </c>
-      <c r="K32" s="11">
-        <v>8093</v>
-      </c>
-      <c r="L32" s="10">
-        <f t="shared" si="2"/>
-        <v>0.32457688297104353</v>
-      </c>
+        <v>0.4805534113176177</v>
+      </c>
+      <c r="K32" s="11"/>
+      <c r="L32" s="10"/>
       <c r="M32" s="11"/>
       <c r="N32" s="10"/>
       <c r="O32" s="10"/>
@@ -5035,25 +4990,25 @@
         <v>23504</v>
       </c>
       <c r="C33" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>17959</v>
       </c>
       <c r="D33" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.76408270932607214</v>
       </c>
       <c r="E33" s="11">
         <v>81</v>
       </c>
       <c r="F33" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>17878</v>
       </c>
       <c r="G33" s="9">
         <v>6956</v>
       </c>
       <c r="H33" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.38908155274639222</v>
       </c>
       <c r="I33" s="9">
@@ -5084,25 +5039,25 @@
         <v>23154</v>
       </c>
       <c r="C34" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>13344</v>
       </c>
       <c r="D34" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.57631510754081372</v>
       </c>
       <c r="E34" s="11">
         <v>43</v>
       </c>
       <c r="F34" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>13301</v>
       </c>
       <c r="G34" s="9">
         <v>8088</v>
       </c>
       <c r="H34" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.60807458085858201</v>
       </c>
       <c r="I34" s="9">
@@ -5138,47 +5093,42 @@
         <v>23711</v>
       </c>
       <c r="C35" s="9">
-        <f t="shared" si="3"/>
-        <v>17469</v>
+        <f t="shared" si="2"/>
+        <v>12700</v>
       </c>
       <c r="D35" s="10">
-        <f t="shared" si="5"/>
-        <v>0.73674665766943614</v>
+        <f t="shared" si="4"/>
+        <v>0.53561638058285188</v>
       </c>
       <c r="E35" s="11">
         <v>52</v>
       </c>
       <c r="F35" s="9">
-        <f t="shared" si="4"/>
-        <v>17417</v>
+        <f t="shared" si="3"/>
+        <v>12648</v>
       </c>
       <c r="G35" s="9">
         <v>7539</v>
       </c>
       <c r="H35" s="10">
-        <f t="shared" si="6"/>
-        <v>0.43285295975196647</v>
+        <f t="shared" si="5"/>
+        <v>0.59606261859582543</v>
       </c>
       <c r="I35" s="9">
         <v>4769</v>
       </c>
       <c r="J35" s="10">
         <f t="shared" si="1"/>
-        <v>0.27381294137911238</v>
-      </c>
-      <c r="K35" s="9">
-        <v>4769</v>
-      </c>
-      <c r="L35" s="10">
-        <f t="shared" si="2"/>
-        <v>0.27381294137911238</v>
-      </c>
+        <v>0.37705566097406706</v>
+      </c>
+      <c r="K35" s="9"/>
+      <c r="L35" s="10"/>
       <c r="M35" s="11">
         <v>340</v>
       </c>
       <c r="N35" s="10">
         <f>SUM(M35/F35)</f>
-        <v>1.9521157489808809E-2</v>
+        <v>2.6881720430107527E-2</v>
       </c>
       <c r="O35" s="10"/>
       <c r="P35" s="10"/>
@@ -5197,25 +5147,25 @@
         <v>25259</v>
       </c>
       <c r="C36" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>19272</v>
       </c>
       <c r="D36" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.76297557306306663</v>
       </c>
       <c r="E36" s="11">
         <v>72</v>
       </c>
       <c r="F36" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>19200</v>
       </c>
       <c r="G36" s="9">
         <v>5051</v>
       </c>
       <c r="H36" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.26307291666666666</v>
       </c>
       <c r="I36" s="9">
@@ -5246,25 +5196,25 @@
         <v>22813</v>
       </c>
       <c r="C37" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>15893</v>
       </c>
       <c r="D37" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.69666418270284491</v>
       </c>
       <c r="E37" s="11">
         <v>48</v>
       </c>
       <c r="F37" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>15845</v>
       </c>
       <c r="G37" s="9">
         <v>9736</v>
       </c>
       <c r="H37" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.61445250867781631</v>
       </c>
       <c r="I37" s="11">
@@ -5295,47 +5245,42 @@
         <v>23554</v>
       </c>
       <c r="C38" s="9">
-        <f t="shared" si="3"/>
-        <v>26259</v>
+        <f t="shared" si="2"/>
+        <v>17148</v>
       </c>
       <c r="D38" s="10">
-        <f t="shared" si="5"/>
-        <v>1.1148424895983697</v>
+        <f t="shared" si="4"/>
+        <v>0.72802920947609751</v>
       </c>
       <c r="E38" s="11">
         <v>49</v>
       </c>
       <c r="F38" s="9">
-        <f t="shared" si="4"/>
-        <v>26210</v>
+        <f t="shared" si="3"/>
+        <v>17099</v>
       </c>
       <c r="G38" s="9">
         <v>7860</v>
       </c>
       <c r="H38" s="10">
-        <f t="shared" si="6"/>
-        <v>0.29988553987027849</v>
+        <f t="shared" si="5"/>
+        <v>0.45967600444470436</v>
       </c>
       <c r="I38" s="11">
         <v>9111</v>
       </c>
       <c r="J38" s="10">
         <f t="shared" si="1"/>
-        <v>0.34761541396413581</v>
-      </c>
-      <c r="K38" s="11">
-        <v>9111</v>
-      </c>
-      <c r="L38" s="10">
-        <f t="shared" si="2"/>
-        <v>0.34761541396413581</v>
-      </c>
+        <v>0.53283817767120889</v>
+      </c>
+      <c r="K38" s="11"/>
+      <c r="L38" s="10"/>
       <c r="M38" s="11">
         <v>128</v>
       </c>
       <c r="N38" s="10">
         <f>SUM(M38/F38)</f>
-        <v>4.8836322014498279E-3</v>
+        <v>7.4858178840867887E-3</v>
       </c>
       <c r="O38" s="10"/>
       <c r="P38" s="10"/>
@@ -5354,25 +5299,25 @@
         <v>26657</v>
       </c>
       <c r="C39" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>19907</v>
       </c>
       <c r="D39" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.74678320891323102</v>
       </c>
       <c r="E39" s="11">
         <v>82</v>
       </c>
       <c r="F39" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>19825</v>
       </c>
       <c r="G39" s="9">
         <v>4175</v>
       </c>
       <c r="H39" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.21059268600252207</v>
       </c>
       <c r="I39" s="9">
@@ -5403,25 +5348,25 @@
         <v>26940</v>
       </c>
       <c r="C40" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>16267</v>
       </c>
       <c r="D40" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.60382331106161846</v>
       </c>
       <c r="E40" s="11">
         <v>103</v>
       </c>
       <c r="F40" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>16164</v>
       </c>
       <c r="G40" s="9">
         <v>9411</v>
       </c>
       <c r="H40" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.58221974758723083</v>
       </c>
       <c r="I40" s="9">
@@ -5457,41 +5402,36 @@
         <v>25582</v>
       </c>
       <c r="C41" s="9">
-        <f t="shared" si="3"/>
-        <v>34555</v>
+        <f t="shared" si="2"/>
+        <v>19284</v>
       </c>
       <c r="D41" s="10">
-        <f t="shared" si="5"/>
-        <v>1.350754436713314</v>
+        <f t="shared" si="4"/>
+        <v>0.75381127355171607</v>
       </c>
       <c r="E41" s="11">
         <v>58</v>
       </c>
       <c r="F41" s="9">
-        <f t="shared" si="4"/>
-        <v>34497</v>
+        <f t="shared" si="3"/>
+        <v>19226</v>
       </c>
       <c r="G41" s="9">
         <v>3955</v>
       </c>
       <c r="H41" s="10">
-        <f t="shared" si="6"/>
-        <v>0.1146476505203351</v>
+        <f t="shared" si="5"/>
+        <v>0.20571101633205036</v>
       </c>
       <c r="I41" s="9">
         <v>15271</v>
       </c>
       <c r="J41" s="10">
         <f t="shared" si="1"/>
-        <v>0.44267617473983245</v>
-      </c>
-      <c r="K41" s="9">
-        <v>15271</v>
-      </c>
-      <c r="L41" s="10">
-        <f t="shared" si="2"/>
-        <v>0.44267617473983245</v>
-      </c>
+        <v>0.79428898366794964</v>
+      </c>
+      <c r="K41" s="9"/>
+      <c r="L41" s="10"/>
       <c r="M41" s="11"/>
       <c r="N41" s="10"/>
       <c r="O41" s="10"/>
@@ -5511,25 +5451,25 @@
         <v>25943</v>
       </c>
       <c r="C42" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>18711</v>
       </c>
       <c r="D42" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.72123501522568711</v>
       </c>
       <c r="E42" s="11">
         <v>64</v>
       </c>
       <c r="F42" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>18647</v>
       </c>
       <c r="G42" s="9">
         <v>7778</v>
       </c>
       <c r="H42" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.41711803507266587</v>
       </c>
       <c r="I42" s="9">
@@ -5565,25 +5505,25 @@
         <v>26775</v>
       </c>
       <c r="C43" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>19727</v>
       </c>
       <c r="D43" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.7367693744164332</v>
       </c>
       <c r="E43" s="11">
         <v>67</v>
       </c>
       <c r="F43" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>19660</v>
       </c>
       <c r="G43" s="9">
         <v>5350</v>
       </c>
       <c r="H43" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.27212614445574773</v>
       </c>
       <c r="I43" s="9">
@@ -5614,45 +5554,40 @@
         <v>20424</v>
       </c>
       <c r="C44" s="9">
-        <f t="shared" si="3"/>
-        <v>20882</v>
+        <f t="shared" si="2"/>
+        <v>13233</v>
       </c>
       <c r="D44" s="10">
-        <f t="shared" si="5"/>
-        <v>1.022424598511555</v>
+        <f t="shared" si="4"/>
+        <v>0.64791421856639253</v>
       </c>
       <c r="E44" s="11">
         <v>61</v>
       </c>
       <c r="F44" s="9">
-        <f t="shared" si="4"/>
-        <v>20821</v>
+        <f t="shared" si="3"/>
+        <v>13172</v>
       </c>
       <c r="G44" s="9">
         <v>5523</v>
       </c>
       <c r="H44" s="10">
-        <f t="shared" si="6"/>
-        <v>0.26526103453244321</v>
+        <f t="shared" si="5"/>
+        <v>0.41929851199514123</v>
       </c>
       <c r="I44" s="12">
         <v>7649</v>
       </c>
       <c r="J44" s="10">
         <f t="shared" si="1"/>
-        <v>0.3673694827337784</v>
+        <v>0.58070148800485877</v>
       </c>
       <c r="K44" s="11"/>
       <c r="L44" s="10"/>
       <c r="M44" s="11"/>
       <c r="N44" s="10"/>
-      <c r="O44" s="12">
-        <v>7649</v>
-      </c>
-      <c r="P44" s="10">
-        <f>SUM(O44/F44)</f>
-        <v>0.3673694827337784</v>
-      </c>
+      <c r="O44" s="12"/>
+      <c r="P44" s="10"/>
       <c r="Q44" s="11"/>
       <c r="R44" s="10"/>
       <c r="S44" s="9"/>
@@ -5668,45 +5603,40 @@
         <v>23674</v>
       </c>
       <c r="C45" s="9">
-        <f t="shared" si="3"/>
-        <v>22267</v>
+        <f t="shared" si="2"/>
+        <v>14545</v>
       </c>
       <c r="D45" s="10">
-        <f t="shared" si="5"/>
-        <v>0.94056771141336493</v>
+        <f t="shared" si="4"/>
+        <v>0.61438709132381519</v>
       </c>
       <c r="E45" s="11">
         <v>41</v>
       </c>
       <c r="F45" s="9">
-        <f t="shared" si="4"/>
-        <v>22226</v>
+        <f t="shared" si="3"/>
+        <v>14504</v>
       </c>
       <c r="G45" s="9">
         <v>6782</v>
       </c>
       <c r="H45" s="10">
         <f>SUM(G45/F45)</f>
-        <v>0.30513812651849187</v>
+        <v>0.46759514616657472</v>
       </c>
       <c r="I45" s="12">
         <v>7722</v>
       </c>
       <c r="J45" s="10">
         <f t="shared" si="1"/>
-        <v>0.34743093674075409</v>
+        <v>0.53240485383342528</v>
       </c>
       <c r="K45" s="11"/>
       <c r="L45" s="10"/>
       <c r="M45" s="11"/>
       <c r="N45" s="10"/>
-      <c r="O45" s="12">
-        <v>7722</v>
-      </c>
-      <c r="P45" s="10">
-        <f>SUM(O45/F45)</f>
-        <v>0.34743093674075409</v>
-      </c>
+      <c r="O45" s="12"/>
+      <c r="P45" s="10"/>
       <c r="Q45" s="11"/>
       <c r="R45" s="10"/>
       <c r="S45" s="11"/>
@@ -5722,18 +5652,18 @@
         <v>27298</v>
       </c>
       <c r="C46" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>18069</v>
       </c>
       <c r="D46" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.66191662392849293</v>
       </c>
       <c r="E46" s="11">
         <v>44</v>
       </c>
       <c r="F46" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>18025</v>
       </c>
       <c r="G46" s="9">
@@ -5776,41 +5706,36 @@
         <v>25191</v>
       </c>
       <c r="C47" s="9">
-        <f t="shared" si="3"/>
-        <v>29108</v>
+        <f t="shared" si="2"/>
+        <v>18662</v>
       </c>
       <c r="D47" s="10">
-        <f t="shared" si="5"/>
-        <v>1.1554920408082252</v>
+        <f t="shared" si="4"/>
+        <v>0.74082013417490378</v>
       </c>
       <c r="E47" s="11">
         <v>67</v>
       </c>
       <c r="F47" s="9">
-        <f t="shared" si="4"/>
-        <v>29041</v>
+        <f t="shared" si="3"/>
+        <v>18595</v>
       </c>
       <c r="G47" s="9">
         <v>8149</v>
       </c>
       <c r="H47" s="10">
-        <f t="shared" si="6"/>
-        <v>0.28060328501084675</v>
+        <f t="shared" si="5"/>
+        <v>0.43823608496907773</v>
       </c>
       <c r="I47" s="11">
         <v>10446</v>
       </c>
       <c r="J47" s="10">
         <f t="shared" si="1"/>
-        <v>0.35969835749457663</v>
-      </c>
-      <c r="K47" s="11">
-        <v>10446</v>
-      </c>
-      <c r="L47" s="10">
-        <f t="shared" si="2"/>
-        <v>0.35969835749457663</v>
-      </c>
+        <v>0.56176391503092227</v>
+      </c>
+      <c r="K47" s="11"/>
+      <c r="L47" s="10"/>
       <c r="M47" s="11"/>
       <c r="N47" s="10"/>
       <c r="O47" s="10"/>
@@ -5832,11 +5757,11 @@
       </c>
       <c r="C48" s="14">
         <f>SUM(C7:C47)</f>
-        <v>844437</v>
+        <v>726801</v>
       </c>
       <c r="D48" s="15">
         <f>SUM(C48/B48)</f>
-        <v>0.81100416432967348</v>
+        <v>0.69802559295598254</v>
       </c>
       <c r="E48" s="16">
         <f>SUM(E7:E47)</f>
@@ -5844,7 +5769,7 @@
       </c>
       <c r="F48" s="14">
         <f>SUM(F7:F47)</f>
-        <v>841771</v>
+        <v>724135</v>
       </c>
       <c r="G48" s="14">
         <f>SUM(G7:G47)</f>
@@ -5852,7 +5777,7 @@
       </c>
       <c r="H48" s="15">
         <f>SUM(G48/F48)</f>
-        <v>0.3414919259513573</v>
+        <v>0.39696741629668503</v>
       </c>
       <c r="I48" s="14">
         <f>SUM(I7:I47)</f>
@@ -5860,15 +5785,15 @@
       </c>
       <c r="J48" s="15">
         <f>SUM(I48/F48)</f>
-        <v>0.51586001418438032</v>
+        <v>0.59966166529721665</v>
       </c>
       <c r="K48" s="14">
         <f>SUM(K7:K47)</f>
-        <v>102265</v>
+        <v>0</v>
       </c>
       <c r="L48" s="15">
         <f>SUM(K48/F48)</f>
-        <v>0.12148791060751678</v>
+        <v>0</v>
       </c>
       <c r="M48" s="14">
         <f>SUM(M7:M47)</f>
@@ -5876,15 +5801,15 @@
       </c>
       <c r="N48" s="15">
         <f>SUM(M48/F48)</f>
-        <v>2.4923643128594358E-3</v>
+        <v>2.8972498222016611E-3</v>
       </c>
       <c r="O48" s="14">
         <f>SUM(O7:O47)</f>
-        <v>15371</v>
+        <v>0</v>
       </c>
       <c r="P48" s="15">
         <f>SUM(O48/F48)</f>
-        <v>1.8260310702079306E-2</v>
+        <v>0</v>
       </c>
       <c r="Q48" s="14">
         <f>SUM(Q7:Q47)</f>
@@ -5892,7 +5817,7 @@
       </c>
       <c r="R48" s="15">
         <f>SUM(Q48/F48)</f>
-        <v>4.0391032715548525E-5</v>
+        <v>4.6952570998501662E-5</v>
       </c>
       <c r="S48" s="14">
         <f>SUM(S7:S47)</f>
@@ -5900,7 +5825,7 @@
       </c>
       <c r="T48" s="15">
         <f>SUM(S48/F48)</f>
-        <v>3.3263203412804671E-4</v>
+        <v>3.866682317523666E-4</v>
       </c>
       <c r="U48" s="14">
         <f>SUM(U7:U47)</f>
@@ -5908,7 +5833,7 @@
       </c>
       <c r="V48" s="15">
         <f>SUM(U48/F48)</f>
-        <v>3.4451174963261977E-5</v>
+        <v>4.0047781145780829E-5</v>
       </c>
     </row>
     <row r="51" spans="4:4" x14ac:dyDescent="0.2">
@@ -5995,7 +5920,7 @@
   <dimension ref="A1:AP74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I49" sqref="I49"/>
+      <selection activeCell="AE7" sqref="AE7:AF47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6453,12 +6378,8 @@
       <c r="J7" s="10">
         <v>0.29249999999999998</v>
       </c>
-      <c r="K7" s="9">
-        <v>4578</v>
-      </c>
-      <c r="L7" s="10">
-        <v>0.29249999999999998</v>
-      </c>
+      <c r="K7" s="9"/>
+      <c r="L7" s="10"/>
       <c r="M7" s="11">
         <v>248</v>
       </c>
@@ -6527,12 +6448,8 @@
       <c r="J8" s="10">
         <v>0.1845</v>
       </c>
-      <c r="K8" s="9">
-        <v>3357</v>
-      </c>
-      <c r="L8" s="10">
-        <v>0.1845</v>
-      </c>
+      <c r="K8" s="9"/>
+      <c r="L8" s="10"/>
       <c r="M8" s="11"/>
       <c r="N8" s="10"/>
       <c r="O8" s="11"/>
@@ -7186,13 +7103,8 @@
         <f t="shared" si="2"/>
         <v>0.31983784893267653</v>
       </c>
-      <c r="K17" s="9">
-        <v>6233</v>
-      </c>
-      <c r="L17" s="10">
-        <f t="shared" ref="L17:L41" si="5">SUM(K17/F17)</f>
-        <v>0.31983784893267653</v>
-      </c>
+      <c r="K17" s="9"/>
+      <c r="L17" s="10"/>
       <c r="M17" s="11">
         <v>173</v>
       </c>
@@ -7278,13 +7190,8 @@
         <f t="shared" si="4"/>
         <v>2.3294992448007437E-2</v>
       </c>
-      <c r="O18" s="9">
-        <v>2969</v>
-      </c>
-      <c r="P18" s="10">
-        <f t="shared" ref="P18:P25" si="6">SUM(O18/F18)</f>
-        <v>0.17247589171604508</v>
-      </c>
+      <c r="O18" s="9"/>
+      <c r="P18" s="10"/>
       <c r="Q18" s="11"/>
       <c r="R18" s="10"/>
       <c r="S18" s="11"/>
@@ -7425,13 +7332,8 @@
         <f t="shared" si="2"/>
         <v>0.20175075412551013</v>
       </c>
-      <c r="K20" s="9">
-        <v>3411</v>
-      </c>
-      <c r="L20" s="10">
-        <f t="shared" si="5"/>
-        <v>0.20175075412551013</v>
-      </c>
+      <c r="K20" s="9"/>
+      <c r="L20" s="10"/>
       <c r="M20" s="11">
         <v>118</v>
       </c>
@@ -7745,13 +7647,8 @@
         <f t="shared" si="4"/>
         <v>1.8300819724216814E-2</v>
       </c>
-      <c r="O24" s="9">
-        <v>1599</v>
-      </c>
-      <c r="P24" s="10">
-        <f t="shared" si="6"/>
-        <v>0.1016076761771621</v>
-      </c>
+      <c r="O24" s="9"/>
+      <c r="P24" s="10"/>
       <c r="Q24" s="11"/>
       <c r="R24" s="10"/>
       <c r="S24" s="11"/>
@@ -7827,13 +7724,8 @@
         <f t="shared" si="4"/>
         <v>1.530891197375615E-2</v>
       </c>
-      <c r="O25" s="9">
-        <v>1222</v>
-      </c>
-      <c r="P25" s="10">
-        <f t="shared" si="6"/>
-        <v>8.351558228540186E-2</v>
-      </c>
+      <c r="O25" s="9"/>
+      <c r="P25" s="10"/>
       <c r="Q25" s="11"/>
       <c r="R25" s="10"/>
       <c r="S25" s="11"/>
@@ -7900,13 +7792,8 @@
         <f t="shared" si="2"/>
         <v>0.34451584794684675</v>
       </c>
-      <c r="K26" s="9">
-        <v>6326</v>
-      </c>
-      <c r="L26" s="10">
-        <f t="shared" si="5"/>
-        <v>0.34451584794684675</v>
-      </c>
+      <c r="K26" s="9"/>
+      <c r="L26" s="10"/>
       <c r="M26" s="11">
         <v>417</v>
       </c>
@@ -8547,13 +8434,8 @@
         <f t="shared" si="2"/>
         <v>0.18868999186330349</v>
       </c>
-      <c r="K35" s="9">
-        <v>2319</v>
-      </c>
-      <c r="L35" s="10">
-        <f t="shared" si="5"/>
-        <v>0.18868999186330349</v>
-      </c>
+      <c r="K35" s="9"/>
+      <c r="L35" s="10"/>
       <c r="M35" s="11"/>
       <c r="N35" s="10"/>
       <c r="O35" s="11"/>
@@ -8698,13 +8580,8 @@
         <f t="shared" si="2"/>
         <v>0.30425042740081354</v>
       </c>
-      <c r="K37" s="9">
-        <v>5161</v>
-      </c>
-      <c r="L37" s="10">
-        <f t="shared" si="5"/>
-        <v>0.30425042740081354</v>
-      </c>
+      <c r="K37" s="9"/>
+      <c r="L37" s="10"/>
       <c r="M37" s="11">
         <v>300</v>
       </c>
@@ -8995,13 +8872,8 @@
         <f t="shared" si="2"/>
         <v>0.65920619149714998</v>
       </c>
-      <c r="K41" s="9">
-        <v>12606</v>
-      </c>
-      <c r="L41" s="10">
-        <f t="shared" si="5"/>
-        <v>0.65920619149714998</v>
-      </c>
+      <c r="K41" s="9"/>
+      <c r="L41" s="10"/>
       <c r="M41" s="11"/>
       <c r="N41" s="10"/>
       <c r="O41" s="11"/>
@@ -9249,13 +9121,8 @@
         <f>SUM(AC44/F44)</f>
         <v>4.8938215502927554E-2</v>
       </c>
-      <c r="AE44" s="12">
-        <v>984</v>
-      </c>
-      <c r="AF44" s="10">
-        <f>SUM(AE44/F44)</f>
-        <v>8.5991435812286993E-2</v>
-      </c>
+      <c r="AE44" s="12"/>
+      <c r="AF44" s="10"/>
       <c r="AG44" s="11"/>
       <c r="AH44" s="10"/>
       <c r="AI44" s="11"/>
@@ -9337,13 +9204,8 @@
         <f>SUM(AC45/F45)</f>
         <v>0.11958793669752164</v>
       </c>
-      <c r="AE45" s="12">
-        <v>766</v>
-      </c>
-      <c r="AF45" s="10">
-        <f>SUM(AE45/F45)</f>
-        <v>5.7181248133771276E-2</v>
-      </c>
+      <c r="AE45" s="12"/>
+      <c r="AF45" s="10"/>
       <c r="AG45" s="11"/>
       <c r="AH45" s="10"/>
       <c r="AI45" s="11"/>
@@ -9548,11 +9410,11 @@
       </c>
       <c r="K48" s="14">
         <f>SUM(K7:K47)</f>
-        <v>43991</v>
+        <v>0</v>
       </c>
       <c r="L48" s="15">
         <f>SUM(K48/F48)</f>
-        <v>6.006909359040883E-2</v>
+        <v>0</v>
       </c>
       <c r="M48" s="14">
         <f>SUM(M7:M47)</f>
@@ -9564,11 +9426,11 @@
       </c>
       <c r="O48" s="14">
         <f>SUM(O7:O47)</f>
-        <v>5790</v>
+        <v>0</v>
       </c>
       <c r="P48" s="15">
         <f>SUM(O48/F48)</f>
-        <v>7.9061638036977359E-3</v>
+        <v>0</v>
       </c>
       <c r="Q48" s="14">
         <f>SUM(Q7:Q47)</f>
@@ -9628,11 +9490,11 @@
       </c>
       <c r="AE48" s="14">
         <f>SUM(AE7:AE47)</f>
-        <v>1750</v>
+        <v>0</v>
       </c>
       <c r="AF48" s="15">
         <f>SUM(AE48/F48)</f>
-        <v>2.3896004588032883E-3</v>
+        <v>0</v>
       </c>
       <c r="AG48" s="14">
         <f>SUM(AG7:AG47)</f>
@@ -9738,14 +9600,6 @@
     <row r="74" spans="4:4" ht="16.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="AM4:AN4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="Y4:Z4"/>
-    <mergeCell ref="AA4:AB4"/>
-    <mergeCell ref="AC4:AD4"/>
-    <mergeCell ref="AE4:AF4"/>
-    <mergeCell ref="AG4:AH4"/>
     <mergeCell ref="A1:AP1"/>
     <mergeCell ref="A2:AP2"/>
     <mergeCell ref="G4:H4"/>
@@ -9758,6 +9612,14 @@
     <mergeCell ref="U4:V4"/>
     <mergeCell ref="AI4:AJ4"/>
     <mergeCell ref="AK4:AL4"/>
+    <mergeCell ref="AM4:AN4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="Y4:Z4"/>
+    <mergeCell ref="AA4:AB4"/>
+    <mergeCell ref="AC4:AD4"/>
+    <mergeCell ref="AE4:AF4"/>
+    <mergeCell ref="AG4:AH4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -9768,8 +9630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E88AD3D-CF93-0A4B-A3CC-3A8B28D063CB}">
   <dimension ref="A1:AT49"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AG44" sqref="AG44:AH45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13255,13 +13117,8 @@
         <f>SUM(AE44/F44)</f>
         <v>6.1194829036946381E-3</v>
       </c>
-      <c r="AG44" s="27">
-        <v>5866</v>
-      </c>
-      <c r="AH44" s="10">
-        <f>SUM(AG44/F44)</f>
-        <v>0.4487110839134093</v>
-      </c>
+      <c r="AG44" s="27"/>
+      <c r="AH44" s="10"/>
       <c r="AI44" s="11"/>
       <c r="AJ44" s="10"/>
       <c r="AK44" s="21"/>
@@ -13337,13 +13194,8 @@
       <c r="AD45" s="10"/>
       <c r="AE45" s="11"/>
       <c r="AF45" s="10"/>
-      <c r="AG45" s="27">
-        <v>4501</v>
-      </c>
-      <c r="AH45" s="10">
-        <f>SUM(AG45/F45)</f>
-        <v>0.32477090699184646</v>
-      </c>
+      <c r="AG45" s="27"/>
+      <c r="AH45" s="10"/>
       <c r="AI45" s="11"/>
       <c r="AJ45" s="10"/>
       <c r="AK45" s="21"/>
@@ -13656,11 +13508,11 @@
       </c>
       <c r="AG48" s="14">
         <f>SUM(AG7:AG47)</f>
-        <v>10367</v>
+        <v>0</v>
       </c>
       <c r="AH48" s="15">
         <f>SUM(AG48/F48)</f>
-        <v>1.5790788427501288E-2</v>
+        <v>0</v>
       </c>
       <c r="AI48" s="14">
         <f>SUM(AI7:AI47)</f>
@@ -13716,6 +13568,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="AS4:AT4"/>
+    <mergeCell ref="AG4:AH4"/>
+    <mergeCell ref="AK4:AL4"/>
+    <mergeCell ref="AM4:AN4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AQ4:AR4"/>
     <mergeCell ref="A1:AP1"/>
     <mergeCell ref="A2:AP2"/>
     <mergeCell ref="AI4:AJ4"/>
@@ -13732,12 +13590,6 @@
     <mergeCell ref="AA4:AB4"/>
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AE4:AF4"/>
-    <mergeCell ref="AS4:AT4"/>
-    <mergeCell ref="AG4:AH4"/>
-    <mergeCell ref="AK4:AL4"/>
-    <mergeCell ref="AM4:AN4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AQ4:AR4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -13748,8 +13600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B29F297E-8049-4148-8F8E-E868EC898AC2}">
   <dimension ref="A1:AP49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14005,7 +13857,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:42" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:42" ht="19" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="35" t="s">
         <v>56</v>
       </c>
@@ -15029,5 +14881,6 @@
     <mergeCell ref="O4:P4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
constituency IDS, hover, progress bar
</commit_message>
<xml_diff>
--- a/csvs/collated-tt-election-results.xlsx
+++ b/csvs/collated-tt-election-results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophegittens/Desktop/my docs/U.W.I. YEAR 4/U.W.I. YEAR 4 - SEMESTER II/COMP 3610/Assignments/Election-Project/csvs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A65ED4-62DE-E949-BADC-6EE91521888D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17771DCF-D6DE-7B4D-BB20-C2890109FDCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{00CD0EB4-DA0B-AB45-875C-9354388CE2C5}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="5" xr2:uid="{00CD0EB4-DA0B-AB45-875C-9354388CE2C5}"/>
   </bookViews>
   <sheets>
     <sheet name="2007" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="2015" sheetId="3" r:id="rId3"/>
     <sheet name="2020" sheetId="4" r:id="rId4"/>
     <sheet name="2025" sheetId="5" r:id="rId5"/>
+    <sheet name="ELECTORAL_ELASTICITY" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="106">
   <si>
     <t>ELECTIONS AND BOUNDARIES COMMISSION</t>
   </si>
@@ -332,6 +333,33 @@
   <si>
     <t>TUNAPUNA</t>
   </si>
+  <si>
+    <t>ELASTICITY</t>
+  </si>
+  <si>
+    <t>SWING_PROB</t>
+  </si>
+  <si>
+    <t>LOW</t>
+  </si>
+  <si>
+    <t>VERY HIGH</t>
+  </si>
+  <si>
+    <t>HIGH</t>
+  </si>
+  <si>
+    <t>VERY LOW</t>
+  </si>
+  <si>
+    <t>MODERATE</t>
+  </si>
+  <si>
+    <t>YEAR</t>
+  </si>
+  <si>
+    <t>INCUMBENT</t>
+  </si>
 </sst>
 </file>
 
@@ -581,7 +609,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -634,6 +662,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -982,10 +1013,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B489430B-CE8D-294E-B0B8-BF19555E0C9E}">
   <dimension ref="A1:R74"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="H32" sqref="H32"/>
+      <selection pane="topRight" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1004,45 +1035,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
       <c r="R1"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
       <c r="R2"/>
     </row>
     <row r="3" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -1065,30 +1096,30 @@
       <c r="F4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="36" t="s">
+      <c r="G4" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36" t="s">
+      <c r="H4" s="37"/>
+      <c r="I4" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36" t="s">
+      <c r="J4" s="37"/>
+      <c r="K4" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="36"/>
-      <c r="M4" s="38" t="s">
+      <c r="L4" s="37"/>
+      <c r="M4" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="N4" s="39"/>
-      <c r="O4" s="36" t="s">
+      <c r="N4" s="40"/>
+      <c r="O4" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="P4" s="36"/>
-      <c r="Q4" s="36" t="s">
+      <c r="P4" s="37"/>
+      <c r="Q4" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="R4" s="36"/>
+      <c r="R4" s="37"/>
     </row>
     <row r="5" spans="1:18" s="1" customFormat="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
@@ -3444,48 +3475,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="37"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="37"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
     </row>
     <row r="3" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:22" s="1" customFormat="1" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3507,38 +3538,38 @@
       <c r="F4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="36" t="s">
+      <c r="G4" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36" t="s">
+      <c r="H4" s="37"/>
+      <c r="I4" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36" t="s">
+      <c r="J4" s="37"/>
+      <c r="K4" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="36"/>
-      <c r="M4" s="36" t="s">
+      <c r="L4" s="37"/>
+      <c r="M4" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="N4" s="36"/>
-      <c r="O4" s="38" t="s">
+      <c r="N4" s="37"/>
+      <c r="O4" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="P4" s="39"/>
-      <c r="Q4" s="36" t="s">
+      <c r="P4" s="40"/>
+      <c r="Q4" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="R4" s="36"/>
-      <c r="S4" s="36" t="s">
+      <c r="R4" s="37"/>
+      <c r="S4" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="T4" s="36"/>
-      <c r="U4" s="36" t="s">
+      <c r="T4" s="37"/>
+      <c r="U4" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="V4" s="36"/>
+      <c r="V4" s="37"/>
     </row>
     <row r="5" spans="1:22" s="1" customFormat="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
@@ -5951,96 +5982,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="37"/>
-      <c r="S1" s="37"/>
-      <c r="T1" s="37"/>
-      <c r="U1" s="37"/>
-      <c r="V1" s="37"/>
-      <c r="W1" s="37"/>
-      <c r="X1" s="37"/>
-      <c r="Y1" s="37"/>
-      <c r="Z1" s="37"/>
-      <c r="AA1" s="37"/>
-      <c r="AB1" s="37"/>
-      <c r="AC1" s="37"/>
-      <c r="AD1" s="37"/>
-      <c r="AE1" s="37"/>
-      <c r="AF1" s="37"/>
-      <c r="AG1" s="37"/>
-      <c r="AH1" s="37"/>
-      <c r="AI1" s="37"/>
-      <c r="AJ1" s="37"/>
-      <c r="AK1" s="37"/>
-      <c r="AL1" s="37"/>
-      <c r="AM1" s="37"/>
-      <c r="AN1" s="37"/>
-      <c r="AO1" s="37"/>
-      <c r="AP1" s="37"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="38"/>
+      <c r="V1" s="38"/>
+      <c r="W1" s="38"/>
+      <c r="X1" s="38"/>
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="38"/>
+      <c r="AA1" s="38"/>
+      <c r="AB1" s="38"/>
+      <c r="AC1" s="38"/>
+      <c r="AD1" s="38"/>
+      <c r="AE1" s="38"/>
+      <c r="AF1" s="38"/>
+      <c r="AG1" s="38"/>
+      <c r="AH1" s="38"/>
+      <c r="AI1" s="38"/>
+      <c r="AJ1" s="38"/>
+      <c r="AK1" s="38"/>
+      <c r="AL1" s="38"/>
+      <c r="AM1" s="38"/>
+      <c r="AN1" s="38"/>
+      <c r="AO1" s="38"/>
+      <c r="AP1" s="38"/>
     </row>
     <row r="2" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="37"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="37"/>
-      <c r="U2" s="37"/>
-      <c r="V2" s="37"/>
-      <c r="W2" s="37"/>
-      <c r="X2" s="37"/>
-      <c r="Y2" s="37"/>
-      <c r="Z2" s="37"/>
-      <c r="AA2" s="37"/>
-      <c r="AB2" s="37"/>
-      <c r="AC2" s="37"/>
-      <c r="AD2" s="37"/>
-      <c r="AE2" s="37"/>
-      <c r="AF2" s="37"/>
-      <c r="AG2" s="37"/>
-      <c r="AH2" s="37"/>
-      <c r="AI2" s="37"/>
-      <c r="AJ2" s="37"/>
-      <c r="AK2" s="37"/>
-      <c r="AL2" s="37"/>
-      <c r="AM2" s="37"/>
-      <c r="AN2" s="37"/>
-      <c r="AO2" s="37"/>
-      <c r="AP2" s="37"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="38"/>
+      <c r="V2" s="38"/>
+      <c r="W2" s="38"/>
+      <c r="X2" s="38"/>
+      <c r="Y2" s="38"/>
+      <c r="Z2" s="38"/>
+      <c r="AA2" s="38"/>
+      <c r="AB2" s="38"/>
+      <c r="AC2" s="38"/>
+      <c r="AD2" s="38"/>
+      <c r="AE2" s="38"/>
+      <c r="AF2" s="38"/>
+      <c r="AG2" s="38"/>
+      <c r="AH2" s="38"/>
+      <c r="AI2" s="38"/>
+      <c r="AJ2" s="38"/>
+      <c r="AK2" s="38"/>
+      <c r="AL2" s="38"/>
+      <c r="AM2" s="38"/>
+      <c r="AN2" s="38"/>
+      <c r="AO2" s="38"/>
+      <c r="AP2" s="38"/>
     </row>
     <row r="3" spans="1:42" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:42" s="1" customFormat="1" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6062,78 +6093,78 @@
       <c r="F4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="36" t="s">
+      <c r="G4" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36" t="s">
+      <c r="H4" s="37"/>
+      <c r="I4" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36" t="s">
+      <c r="J4" s="37"/>
+      <c r="K4" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="36"/>
-      <c r="M4" s="36" t="s">
+      <c r="L4" s="37"/>
+      <c r="M4" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="N4" s="36"/>
-      <c r="O4" s="36" t="s">
+      <c r="N4" s="37"/>
+      <c r="O4" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="P4" s="36"/>
-      <c r="Q4" s="36" t="s">
+      <c r="P4" s="37"/>
+      <c r="Q4" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="R4" s="36"/>
-      <c r="S4" s="36" t="s">
+      <c r="R4" s="37"/>
+      <c r="S4" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="T4" s="36"/>
-      <c r="U4" s="36" t="s">
+      <c r="T4" s="37"/>
+      <c r="U4" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="V4" s="36"/>
-      <c r="W4" s="36" t="s">
+      <c r="V4" s="37"/>
+      <c r="W4" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="X4" s="36"/>
-      <c r="Y4" s="36" t="s">
+      <c r="X4" s="37"/>
+      <c r="Y4" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="Z4" s="36"/>
-      <c r="AA4" s="36" t="s">
+      <c r="Z4" s="37"/>
+      <c r="AA4" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="AB4" s="36"/>
-      <c r="AC4" s="36" t="s">
+      <c r="AB4" s="37"/>
+      <c r="AC4" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="AD4" s="36"/>
-      <c r="AE4" s="38" t="s">
+      <c r="AD4" s="37"/>
+      <c r="AE4" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="AF4" s="39"/>
-      <c r="AG4" s="36" t="s">
+      <c r="AF4" s="40"/>
+      <c r="AG4" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="AH4" s="36"/>
-      <c r="AI4" s="36" t="s">
+      <c r="AH4" s="37"/>
+      <c r="AI4" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="AJ4" s="36"/>
-      <c r="AK4" s="36" t="s">
+      <c r="AJ4" s="37"/>
+      <c r="AK4" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="AL4" s="36"/>
-      <c r="AM4" s="36" t="s">
+      <c r="AL4" s="37"/>
+      <c r="AM4" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="AN4" s="36"/>
-      <c r="AO4" s="36" t="s">
+      <c r="AN4" s="37"/>
+      <c r="AO4" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="AP4" s="36"/>
+      <c r="AP4" s="37"/>
     </row>
     <row r="5" spans="1:42" s="1" customFormat="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
@@ -9630,8 +9661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E88AD3D-CF93-0A4B-A3CC-3A8B28D063CB}">
   <dimension ref="A1:AT49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AG44" sqref="AG44:AH45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9640,96 +9671,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="37"/>
-      <c r="S1" s="37"/>
-      <c r="T1" s="37"/>
-      <c r="U1" s="37"/>
-      <c r="V1" s="37"/>
-      <c r="W1" s="37"/>
-      <c r="X1" s="37"/>
-      <c r="Y1" s="37"/>
-      <c r="Z1" s="37"/>
-      <c r="AA1" s="37"/>
-      <c r="AB1" s="37"/>
-      <c r="AC1" s="37"/>
-      <c r="AD1" s="37"/>
-      <c r="AE1" s="37"/>
-      <c r="AF1" s="37"/>
-      <c r="AG1" s="37"/>
-      <c r="AH1" s="37"/>
-      <c r="AI1" s="37"/>
-      <c r="AJ1" s="37"/>
-      <c r="AK1" s="37"/>
-      <c r="AL1" s="37"/>
-      <c r="AM1" s="37"/>
-      <c r="AN1" s="37"/>
-      <c r="AO1" s="37"/>
-      <c r="AP1" s="37"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="38"/>
+      <c r="V1" s="38"/>
+      <c r="W1" s="38"/>
+      <c r="X1" s="38"/>
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="38"/>
+      <c r="AA1" s="38"/>
+      <c r="AB1" s="38"/>
+      <c r="AC1" s="38"/>
+      <c r="AD1" s="38"/>
+      <c r="AE1" s="38"/>
+      <c r="AF1" s="38"/>
+      <c r="AG1" s="38"/>
+      <c r="AH1" s="38"/>
+      <c r="AI1" s="38"/>
+      <c r="AJ1" s="38"/>
+      <c r="AK1" s="38"/>
+      <c r="AL1" s="38"/>
+      <c r="AM1" s="38"/>
+      <c r="AN1" s="38"/>
+      <c r="AO1" s="38"/>
+      <c r="AP1" s="38"/>
     </row>
     <row r="2" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="37"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="37"/>
-      <c r="U2" s="37"/>
-      <c r="V2" s="37"/>
-      <c r="W2" s="37"/>
-      <c r="X2" s="37"/>
-      <c r="Y2" s="37"/>
-      <c r="Z2" s="37"/>
-      <c r="AA2" s="37"/>
-      <c r="AB2" s="37"/>
-      <c r="AC2" s="37"/>
-      <c r="AD2" s="37"/>
-      <c r="AE2" s="37"/>
-      <c r="AF2" s="37"/>
-      <c r="AG2" s="37"/>
-      <c r="AH2" s="37"/>
-      <c r="AI2" s="37"/>
-      <c r="AJ2" s="37"/>
-      <c r="AK2" s="37"/>
-      <c r="AL2" s="37"/>
-      <c r="AM2" s="37"/>
-      <c r="AN2" s="37"/>
-      <c r="AO2" s="37"/>
-      <c r="AP2" s="37"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="38"/>
+      <c r="V2" s="38"/>
+      <c r="W2" s="38"/>
+      <c r="X2" s="38"/>
+      <c r="Y2" s="38"/>
+      <c r="Z2" s="38"/>
+      <c r="AA2" s="38"/>
+      <c r="AB2" s="38"/>
+      <c r="AC2" s="38"/>
+      <c r="AD2" s="38"/>
+      <c r="AE2" s="38"/>
+      <c r="AF2" s="38"/>
+      <c r="AG2" s="38"/>
+      <c r="AH2" s="38"/>
+      <c r="AI2" s="38"/>
+      <c r="AJ2" s="38"/>
+      <c r="AK2" s="38"/>
+      <c r="AL2" s="38"/>
+      <c r="AM2" s="38"/>
+      <c r="AN2" s="38"/>
+      <c r="AO2" s="38"/>
+      <c r="AP2" s="38"/>
     </row>
     <row r="3" spans="1:46" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D3" s="2"/>
@@ -9772,86 +9803,86 @@
       <c r="F4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="36" t="s">
+      <c r="G4" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36" t="s">
+      <c r="H4" s="37"/>
+      <c r="I4" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36" t="s">
+      <c r="J4" s="37"/>
+      <c r="K4" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="L4" s="36"/>
-      <c r="M4" s="38" t="s">
+      <c r="L4" s="37"/>
+      <c r="M4" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="39"/>
-      <c r="O4" s="36" t="s">
+      <c r="N4" s="40"/>
+      <c r="O4" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="P4" s="36"/>
-      <c r="Q4" s="36" t="s">
+      <c r="P4" s="37"/>
+      <c r="Q4" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="R4" s="36"/>
-      <c r="S4" s="36" t="s">
+      <c r="R4" s="37"/>
+      <c r="S4" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="T4" s="36"/>
-      <c r="U4" s="36" t="s">
+      <c r="T4" s="37"/>
+      <c r="U4" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="V4" s="36"/>
-      <c r="W4" s="36" t="s">
+      <c r="V4" s="37"/>
+      <c r="W4" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="X4" s="36"/>
-      <c r="Y4" s="36" t="s">
+      <c r="X4" s="37"/>
+      <c r="Y4" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="Z4" s="36"/>
-      <c r="AA4" s="38" t="s">
+      <c r="Z4" s="37"/>
+      <c r="AA4" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="AB4" s="39"/>
-      <c r="AC4" s="36" t="s">
+      <c r="AB4" s="40"/>
+      <c r="AC4" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="AD4" s="36"/>
-      <c r="AE4" s="36" t="s">
+      <c r="AD4" s="37"/>
+      <c r="AE4" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="AF4" s="36"/>
-      <c r="AG4" s="36" t="s">
+      <c r="AF4" s="37"/>
+      <c r="AG4" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="AH4" s="36"/>
-      <c r="AI4" s="36" t="s">
+      <c r="AH4" s="37"/>
+      <c r="AI4" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="AJ4" s="36"/>
-      <c r="AK4" s="38" t="s">
+      <c r="AJ4" s="37"/>
+      <c r="AK4" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="AL4" s="39"/>
-      <c r="AM4" s="38" t="s">
+      <c r="AL4" s="40"/>
+      <c r="AM4" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="AN4" s="39"/>
-      <c r="AO4" s="38" t="s">
+      <c r="AN4" s="40"/>
+      <c r="AO4" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="AP4" s="39"/>
-      <c r="AQ4" s="38" t="s">
+      <c r="AP4" s="40"/>
+      <c r="AQ4" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="AR4" s="39"/>
-      <c r="AS4" s="36" t="s">
+      <c r="AR4" s="40"/>
+      <c r="AS4" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="AT4" s="36"/>
+      <c r="AT4" s="37"/>
     </row>
     <row r="5" spans="1:46" s="1" customFormat="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
@@ -13568,12 +13599,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="AS4:AT4"/>
-    <mergeCell ref="AG4:AH4"/>
-    <mergeCell ref="AK4:AL4"/>
-    <mergeCell ref="AM4:AN4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AQ4:AR4"/>
     <mergeCell ref="A1:AP1"/>
     <mergeCell ref="A2:AP2"/>
     <mergeCell ref="AI4:AJ4"/>
@@ -13590,6 +13615,12 @@
     <mergeCell ref="AA4:AB4"/>
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AE4:AF4"/>
+    <mergeCell ref="AS4:AT4"/>
+    <mergeCell ref="AG4:AH4"/>
+    <mergeCell ref="AK4:AL4"/>
+    <mergeCell ref="AM4:AN4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AQ4:AR4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -13610,96 +13641,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="37"/>
-      <c r="S1" s="37"/>
-      <c r="T1" s="37"/>
-      <c r="U1" s="37"/>
-      <c r="V1" s="37"/>
-      <c r="W1" s="37"/>
-      <c r="X1" s="37"/>
-      <c r="Y1" s="37"/>
-      <c r="Z1" s="37"/>
-      <c r="AA1" s="37"/>
-      <c r="AB1" s="37"/>
-      <c r="AC1" s="37"/>
-      <c r="AD1" s="37"/>
-      <c r="AE1" s="37"/>
-      <c r="AF1" s="37"/>
-      <c r="AG1" s="37"/>
-      <c r="AH1" s="37"/>
-      <c r="AI1" s="37"/>
-      <c r="AJ1" s="37"/>
-      <c r="AK1" s="37"/>
-      <c r="AL1" s="37"/>
-      <c r="AM1" s="37"/>
-      <c r="AN1" s="37"/>
-      <c r="AO1" s="37"/>
-      <c r="AP1" s="37"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="38"/>
+      <c r="V1" s="38"/>
+      <c r="W1" s="38"/>
+      <c r="X1" s="38"/>
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="38"/>
+      <c r="AA1" s="38"/>
+      <c r="AB1" s="38"/>
+      <c r="AC1" s="38"/>
+      <c r="AD1" s="38"/>
+      <c r="AE1" s="38"/>
+      <c r="AF1" s="38"/>
+      <c r="AG1" s="38"/>
+      <c r="AH1" s="38"/>
+      <c r="AI1" s="38"/>
+      <c r="AJ1" s="38"/>
+      <c r="AK1" s="38"/>
+      <c r="AL1" s="38"/>
+      <c r="AM1" s="38"/>
+      <c r="AN1" s="38"/>
+      <c r="AO1" s="38"/>
+      <c r="AP1" s="38"/>
     </row>
     <row r="2" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="37"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="37"/>
-      <c r="U2" s="37"/>
-      <c r="V2" s="37"/>
-      <c r="W2" s="37"/>
-      <c r="X2" s="37"/>
-      <c r="Y2" s="37"/>
-      <c r="Z2" s="37"/>
-      <c r="AA2" s="37"/>
-      <c r="AB2" s="37"/>
-      <c r="AC2" s="37"/>
-      <c r="AD2" s="37"/>
-      <c r="AE2" s="37"/>
-      <c r="AF2" s="37"/>
-      <c r="AG2" s="37"/>
-      <c r="AH2" s="37"/>
-      <c r="AI2" s="37"/>
-      <c r="AJ2" s="37"/>
-      <c r="AK2" s="37"/>
-      <c r="AL2" s="37"/>
-      <c r="AM2" s="37"/>
-      <c r="AN2" s="37"/>
-      <c r="AO2" s="37"/>
-      <c r="AP2" s="37"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="38"/>
+      <c r="V2" s="38"/>
+      <c r="W2" s="38"/>
+      <c r="X2" s="38"/>
+      <c r="Y2" s="38"/>
+      <c r="Z2" s="38"/>
+      <c r="AA2" s="38"/>
+      <c r="AB2" s="38"/>
+      <c r="AC2" s="38"/>
+      <c r="AD2" s="38"/>
+      <c r="AE2" s="38"/>
+      <c r="AF2" s="38"/>
+      <c r="AG2" s="38"/>
+      <c r="AH2" s="38"/>
+      <c r="AI2" s="38"/>
+      <c r="AJ2" s="38"/>
+      <c r="AK2" s="38"/>
+      <c r="AL2" s="38"/>
+      <c r="AM2" s="38"/>
+      <c r="AN2" s="38"/>
+      <c r="AO2" s="38"/>
+      <c r="AP2" s="38"/>
     </row>
     <row r="3" spans="1:42" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D3" s="2"/>
@@ -13742,30 +13773,30 @@
       <c r="F4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="36" t="s">
+      <c r="G4" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36" t="s">
+      <c r="H4" s="37"/>
+      <c r="I4" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36" t="s">
+      <c r="J4" s="37"/>
+      <c r="K4" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="L4" s="36"/>
-      <c r="M4" s="38" t="s">
+      <c r="L4" s="37"/>
+      <c r="M4" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="39"/>
-      <c r="O4" s="36" t="s">
+      <c r="N4" s="40"/>
+      <c r="O4" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="P4" s="36"/>
-      <c r="Q4" s="36" t="s">
+      <c r="P4" s="37"/>
+      <c r="Q4" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="R4" s="36"/>
+      <c r="R4" s="37"/>
     </row>
     <row r="5" spans="1:42" s="1" customFormat="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
@@ -14883,4 +14914,1083 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80A4F573-B339-FF41-B352-70D57E35F1E4}">
+  <dimension ref="A1:L63"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" customWidth="1"/>
+    <col min="3" max="12" width="11.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>98</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="11">
+        <v>2024</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="E3" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="11">
+        <v>2024</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="E4" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="11">
+        <v>2024</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="E5" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="11">
+        <v>2024</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="11">
+        <v>2024</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="E7" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="11">
+        <v>2024</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="E8" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="11">
+        <v>2024</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="E9" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" s="11">
+        <v>2024</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="E10" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="11">
+        <v>2024</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D11" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="E11" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="B12" s="11">
+        <v>2024</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="E12" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="B13" s="11">
+        <v>2024</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="E13" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" s="11">
+        <v>2024</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D14" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="E14" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" s="11">
+        <v>2020</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D15" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="E15" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="11">
+        <v>2020</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="E16" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="11">
+        <v>2020</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D17" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="E17" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="11">
+        <v>2020</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D18" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="E18" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="11">
+        <v>2020</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D19" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="E19" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" s="11">
+        <v>2020</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D20" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="E20" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" s="11">
+        <v>2020</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="E21" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" s="11">
+        <v>2020</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D22" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="E22" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="B23" s="11">
+        <v>2020</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D23" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="E23" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="11">
+        <v>2020</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D24" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="E24" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" s="11">
+        <v>2020</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D25" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="E25" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="B26" s="11">
+        <v>2020</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D26" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="E26" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" s="11">
+        <v>2015</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D27" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="E27" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" s="11">
+        <v>2015</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D28" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="E28" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" s="11">
+        <v>2015</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D29" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="E29" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="11">
+        <v>2015</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D30" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="E30" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31" s="11">
+        <v>2015</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D31" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="E31" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32" s="11">
+        <v>2015</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D32" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="E32" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="B33" s="11">
+        <v>2015</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D33" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="E33" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="B34" s="11">
+        <v>2015</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D34" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="E34" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="B35" s="11">
+        <v>2015</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D35" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="E35" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="B36" s="11">
+        <v>2015</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D36" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="E36" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="B37" s="11">
+        <v>2015</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D37" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="E37" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="B38" s="11">
+        <v>2015</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D38" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="E38" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="B39" s="11">
+        <v>2010</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D39" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="E39" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="B40" s="11">
+        <v>2010</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D40" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="E40" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="B41" s="11">
+        <v>2010</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D41" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="E41" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="B42" s="11">
+        <v>2010</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D42" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="E42" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="B43" s="11">
+        <v>2010</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D43" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="E43" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="B44" s="11">
+        <v>2010</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D44" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="E44" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="B45" s="11">
+        <v>2010</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D45" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="E45" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="B46" s="11">
+        <v>2010</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D46" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="E46" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="B47" s="11">
+        <v>2010</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D47" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="E47" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="B48" s="11">
+        <v>2010</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D48" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="E48" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="B49" s="11">
+        <v>2010</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D49" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="E49" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="B50" s="11">
+        <v>2010</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D50" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="E50" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="B51" s="11">
+        <v>2007</v>
+      </c>
+      <c r="C51" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D51" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="E51" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="B52" s="11">
+        <v>2007</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D52" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="E52" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="B53" s="11">
+        <v>2007</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D53" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="E53" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="B54" s="11">
+        <v>2007</v>
+      </c>
+      <c r="C54" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D54" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="E54" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="B55" s="11">
+        <v>2007</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D55" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="E55" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="B56" s="11">
+        <v>2007</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D56" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="E56" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="B57" s="11">
+        <v>2007</v>
+      </c>
+      <c r="C57" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D57" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="E57" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="B58" s="11">
+        <v>2007</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D58" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="E58" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="B59" s="11">
+        <v>2007</v>
+      </c>
+      <c r="C59" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D59" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="E59" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="B60" s="11">
+        <v>2007</v>
+      </c>
+      <c r="C60" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D60" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="E60" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="B61" s="11">
+        <v>2007</v>
+      </c>
+      <c r="C61" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D61" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="E61" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="B62" s="11">
+        <v>2007</v>
+      </c>
+      <c r="C62" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D62" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="E62" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
changes to election excel files
</commit_message>
<xml_diff>
--- a/csvs/collated-tt-election-results.xlsx
+++ b/csvs/collated-tt-election-results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophegittens/Desktop/my docs/U.W.I. YEAR 4/U.W.I. YEAR 4 - SEMESTER II/COMP 3610/Assignments/Election-Project/csvs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17771DCF-D6DE-7B4D-BB20-C2890109FDCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F824F883-DBCB-B54A-B7FB-98ACDF7A6A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="5" xr2:uid="{00CD0EB4-DA0B-AB45-875C-9354388CE2C5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="1" activeTab="5" xr2:uid="{00CD0EB4-DA0B-AB45-875C-9354388CE2C5}"/>
   </bookViews>
   <sheets>
     <sheet name="2007" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="2015" sheetId="3" r:id="rId3"/>
     <sheet name="2020" sheetId="4" r:id="rId4"/>
     <sheet name="2025" sheetId="5" r:id="rId5"/>
-    <sheet name="ELECTORAL_ELASTICITY" sheetId="7" r:id="rId6"/>
+    <sheet name="2025_ACTUAL" sheetId="8" r:id="rId6"/>
+    <sheet name="ELECTORAL_ELASTICITY" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="120">
   <si>
     <t>ELECTIONS AND BOUNDARIES COMMISSION</t>
   </si>
@@ -360,6 +361,48 @@
   <si>
     <t>INCUMBENT</t>
   </si>
+  <si>
+    <t>PORT OF SPAIN NORTH/ST. ANN'S WEST</t>
+  </si>
+  <si>
+    <t>PORT OF SPAIN SOUTH</t>
+  </si>
+  <si>
+    <t>T.P.P.</t>
+  </si>
+  <si>
+    <t>N.T.A.</t>
+  </si>
+  <si>
+    <t>A.P.P.</t>
+  </si>
+  <si>
+    <t>P.F.</t>
+  </si>
+  <si>
+    <t>RESULTS OF THE PARLIAMENTARY ELECTION HELD ON MONDAY 28TH APRIL, 2025</t>
+  </si>
+  <si>
+    <t>C.A.R.M.</t>
+  </si>
+  <si>
+    <t>H.M.</t>
+  </si>
+  <si>
+    <t>I.D.A.</t>
+  </si>
+  <si>
+    <t>I.N.D.4.</t>
+  </si>
+  <si>
+    <t>I.N.D.3.</t>
+  </si>
+  <si>
+    <t>I.N.D.2.</t>
+  </si>
+  <si>
+    <t>I.N.D.1.</t>
+  </si>
 </sst>
 </file>
 
@@ -425,7 +468,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -605,11 +648,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -677,6 +729,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3455,8 +3521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D39057C-680C-4843-89F6-29B9284CAFAA}">
   <dimension ref="A1:V74"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7:P47"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5950,8 +6016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B29ADA29-60E2-5C49-A453-E54C505FD3C8}">
   <dimension ref="A1:AP74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AE7" sqref="AE7:AF47"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9631,6 +9697,10 @@
     <row r="74" spans="4:4" ht="16.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="AA4:AB4"/>
+    <mergeCell ref="AC4:AD4"/>
+    <mergeCell ref="AE4:AF4"/>
+    <mergeCell ref="AG4:AH4"/>
     <mergeCell ref="A1:AP1"/>
     <mergeCell ref="A2:AP2"/>
     <mergeCell ref="G4:H4"/>
@@ -9647,10 +9717,6 @@
     <mergeCell ref="AO4:AP4"/>
     <mergeCell ref="W4:X4"/>
     <mergeCell ref="Y4:Z4"/>
-    <mergeCell ref="AA4:AB4"/>
-    <mergeCell ref="AC4:AD4"/>
-    <mergeCell ref="AE4:AF4"/>
-    <mergeCell ref="AG4:AH4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -9661,8 +9727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E88AD3D-CF93-0A4B-A3CC-3A8B28D063CB}">
   <dimension ref="A1:AT49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A47"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13599,6 +13665,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="AS4:AT4"/>
+    <mergeCell ref="AG4:AH4"/>
+    <mergeCell ref="AK4:AL4"/>
+    <mergeCell ref="AM4:AN4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AQ4:AR4"/>
     <mergeCell ref="A1:AP1"/>
     <mergeCell ref="A2:AP2"/>
     <mergeCell ref="AI4:AJ4"/>
@@ -13615,12 +13687,6 @@
     <mergeCell ref="AA4:AB4"/>
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AE4:AF4"/>
-    <mergeCell ref="AS4:AT4"/>
-    <mergeCell ref="AG4:AH4"/>
-    <mergeCell ref="AK4:AL4"/>
-    <mergeCell ref="AM4:AN4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AQ4:AR4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -13632,7 +13698,7 @@
   <dimension ref="A1:AP49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13688,7 +13754,7 @@
     </row>
     <row r="2" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A2" s="38" t="s">
-        <v>54</v>
+        <v>112</v>
       </c>
       <c r="B2" s="38"/>
       <c r="C2" s="38"/>
@@ -14917,10 +14983,4046 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B35352C0-29D1-1D43-893D-0D73A9F2CD47}">
+  <dimension ref="A1:AV49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="37.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" customWidth="1"/>
+    <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="48" max="16384" width="10.83203125" style="43"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A1" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="38"/>
+      <c r="V1" s="38"/>
+      <c r="W1" s="38"/>
+      <c r="X1" s="38"/>
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="38"/>
+      <c r="AA1" s="38"/>
+      <c r="AB1" s="38"/>
+      <c r="AC1" s="38"/>
+      <c r="AD1" s="38"/>
+      <c r="AE1" s="38"/>
+      <c r="AF1" s="38"/>
+      <c r="AG1" s="38"/>
+      <c r="AH1" s="38"/>
+      <c r="AI1" s="38"/>
+      <c r="AJ1" s="38"/>
+      <c r="AK1" s="38"/>
+      <c r="AL1" s="38"/>
+      <c r="AM1" s="38"/>
+      <c r="AN1" s="38"/>
+      <c r="AO1" s="38"/>
+      <c r="AP1" s="38"/>
+      <c r="AQ1" s="38"/>
+      <c r="AR1" s="38"/>
+      <c r="AS1" s="38"/>
+      <c r="AT1" s="38"/>
+      <c r="AU1" s="38"/>
+      <c r="AV1" s="38"/>
+    </row>
+    <row r="2" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A2" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="38"/>
+      <c r="V2" s="38"/>
+      <c r="W2" s="38"/>
+      <c r="X2" s="38"/>
+      <c r="Y2" s="38"/>
+      <c r="Z2" s="38"/>
+      <c r="AA2" s="38"/>
+      <c r="AB2" s="38"/>
+      <c r="AC2" s="38"/>
+      <c r="AD2" s="38"/>
+      <c r="AE2" s="38"/>
+      <c r="AF2" s="38"/>
+      <c r="AG2" s="38"/>
+      <c r="AH2" s="38"/>
+      <c r="AI2" s="38"/>
+      <c r="AJ2" s="38"/>
+      <c r="AK2" s="38"/>
+      <c r="AL2" s="38"/>
+      <c r="AM2" s="38"/>
+      <c r="AN2" s="38"/>
+      <c r="AO2" s="38"/>
+      <c r="AP2" s="38"/>
+      <c r="AQ2" s="38"/>
+      <c r="AR2" s="38"/>
+      <c r="AS2" s="38"/>
+      <c r="AT2" s="38"/>
+      <c r="AU2" s="38"/>
+      <c r="AV2" s="38"/>
+    </row>
+    <row r="3" spans="1:48" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AF3" s="2"/>
+      <c r="AH3" s="2"/>
+      <c r="AJ3" s="2"/>
+      <c r="AL3" s="2"/>
+      <c r="AN3" s="2"/>
+      <c r="AP3" s="2"/>
+      <c r="AR3" s="2"/>
+      <c r="AT3" s="2"/>
+      <c r="AV3" s="41"/>
+    </row>
+    <row r="4" spans="1:48" s="42" customFormat="1" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="L4" s="37"/>
+      <c r="M4" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="N4" s="40"/>
+      <c r="O4" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="P4" s="40"/>
+      <c r="Q4" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="R4" s="37"/>
+      <c r="S4" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="T4" s="37"/>
+      <c r="U4" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="V4" s="37"/>
+      <c r="W4" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="X4" s="37"/>
+      <c r="Y4" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z4" s="37"/>
+      <c r="AA4" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="AB4" s="37"/>
+      <c r="AC4" s="37" t="s">
+        <v>114</v>
+      </c>
+      <c r="AD4" s="37"/>
+      <c r="AE4" s="37" t="s">
+        <v>115</v>
+      </c>
+      <c r="AF4" s="37"/>
+      <c r="AG4" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH4" s="37"/>
+      <c r="AI4" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ4" s="37"/>
+      <c r="AK4" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL4" s="37"/>
+      <c r="AM4" s="37" t="s">
+        <v>119</v>
+      </c>
+      <c r="AN4" s="37"/>
+      <c r="AO4" s="37" t="s">
+        <v>118</v>
+      </c>
+      <c r="AP4" s="37"/>
+      <c r="AQ4" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR4" s="37"/>
+      <c r="AS4" s="37" t="s">
+        <v>116</v>
+      </c>
+      <c r="AT4" s="37"/>
+      <c r="AU4" s="1"/>
+    </row>
+    <row r="5" spans="1:48" s="42" customFormat="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="I5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="4"/>
+      <c r="K5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" s="4"/>
+      <c r="M5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N5" s="4"/>
+      <c r="O5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="R5" s="4"/>
+      <c r="S5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="T5" s="4"/>
+      <c r="U5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="V5" s="4"/>
+      <c r="W5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z5" s="4"/>
+      <c r="AA5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB5" s="4"/>
+      <c r="AC5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="AD5" s="4"/>
+      <c r="AE5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF5" s="4"/>
+      <c r="AG5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="AH5" s="4"/>
+      <c r="AI5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ5" s="4"/>
+      <c r="AK5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="AL5" s="4"/>
+      <c r="AM5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="AN5" s="4"/>
+      <c r="AO5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="AP5" s="4"/>
+      <c r="AQ5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="AR5" s="4"/>
+      <c r="AS5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="AT5" s="4"/>
+      <c r="AU5" s="1"/>
+    </row>
+    <row r="6" spans="1:48" s="42" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="R6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="S6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="T6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="U6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="V6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="W6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="X6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="AH6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="AJ6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="AK6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="AL6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="AM6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="AN6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="AO6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="AP6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="AQ6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="AR6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="AS6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="AT6" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="AU6" s="47"/>
+    </row>
+    <row r="7" spans="1:48" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="11">
+        <v>28802</v>
+      </c>
+      <c r="C7" s="11">
+        <v>14167</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0.4919</v>
+      </c>
+      <c r="E7" s="11">
+        <v>46</v>
+      </c>
+      <c r="F7" s="9">
+        <f t="shared" ref="F7:F47" si="0">SUM(C7-E7)</f>
+        <v>14121</v>
+      </c>
+      <c r="G7" s="11">
+        <v>7055</v>
+      </c>
+      <c r="H7" s="10">
+        <f t="shared" ref="H7:H47" si="1">SUM(G7/F7)</f>
+        <v>0.49961050917073863</v>
+      </c>
+      <c r="I7" s="11">
+        <v>6356</v>
+      </c>
+      <c r="J7" s="10">
+        <f t="shared" ref="J7:J47" si="2">SUM(I7/F7)</f>
+        <v>0.45010976559733729</v>
+      </c>
+      <c r="K7" s="11"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="11">
+        <v>520</v>
+      </c>
+      <c r="R7" s="10">
+        <f t="shared" ref="R7:R47" si="3">SUM(Q7/C7)</f>
+        <v>3.6705018705442224E-2</v>
+      </c>
+      <c r="S7" s="11"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="11"/>
+      <c r="V7" s="10"/>
+      <c r="W7" s="11">
+        <v>152</v>
+      </c>
+      <c r="X7" s="10">
+        <f t="shared" ref="X7:X23" si="4">SUM(W7/C7)</f>
+        <v>1.0729159313898496E-2</v>
+      </c>
+      <c r="Y7" s="11"/>
+      <c r="Z7" s="10"/>
+      <c r="AA7" s="11"/>
+      <c r="AB7" s="10"/>
+      <c r="AC7" s="11"/>
+      <c r="AD7" s="10"/>
+      <c r="AE7" s="11"/>
+      <c r="AF7" s="10"/>
+      <c r="AG7" s="11">
+        <v>38</v>
+      </c>
+      <c r="AH7" s="10"/>
+      <c r="AI7" s="11"/>
+      <c r="AJ7" s="10"/>
+      <c r="AK7" s="11"/>
+      <c r="AL7" s="10"/>
+      <c r="AM7" s="11"/>
+      <c r="AN7" s="10"/>
+      <c r="AO7" s="11"/>
+      <c r="AP7" s="10"/>
+      <c r="AQ7" s="11"/>
+      <c r="AR7" s="10"/>
+      <c r="AS7" s="11"/>
+      <c r="AT7" s="46"/>
+      <c r="AU7" s="48"/>
+    </row>
+    <row r="8" spans="1:48" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="11">
+        <v>28953</v>
+      </c>
+      <c r="C8" s="11">
+        <v>15350</v>
+      </c>
+      <c r="D8" s="10">
+        <v>0.5302</v>
+      </c>
+      <c r="E8" s="11">
+        <v>62</v>
+      </c>
+      <c r="F8" s="9">
+        <f>SUM(C8-E8)</f>
+        <v>15288</v>
+      </c>
+      <c r="G8" s="11">
+        <v>9858</v>
+      </c>
+      <c r="H8" s="10">
+        <f>SUM(G8/F8)</f>
+        <v>0.64481946624803765</v>
+      </c>
+      <c r="I8" s="11">
+        <v>4443</v>
+      </c>
+      <c r="J8" s="10">
+        <f>SUM(I8/F8)</f>
+        <v>0.29062009419152274</v>
+      </c>
+      <c r="K8" s="11"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="11">
+        <v>987</v>
+      </c>
+      <c r="R8" s="10">
+        <f>SUM(Q8/C8)</f>
+        <v>6.4299674267100981E-2</v>
+      </c>
+      <c r="S8" s="11"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="11"/>
+      <c r="V8" s="10"/>
+      <c r="W8" s="11"/>
+      <c r="X8" s="10"/>
+      <c r="Y8" s="11"/>
+      <c r="Z8" s="10"/>
+      <c r="AA8" s="11"/>
+      <c r="AB8" s="10"/>
+      <c r="AC8" s="11"/>
+      <c r="AD8" s="10"/>
+      <c r="AE8" s="11"/>
+      <c r="AF8" s="10"/>
+      <c r="AG8" s="11"/>
+      <c r="AH8" s="10"/>
+      <c r="AI8" s="11"/>
+      <c r="AJ8" s="10"/>
+      <c r="AK8" s="11"/>
+      <c r="AL8" s="10"/>
+      <c r="AM8" s="11"/>
+      <c r="AN8" s="10"/>
+      <c r="AO8" s="11"/>
+      <c r="AP8" s="10"/>
+      <c r="AQ8" s="11"/>
+      <c r="AR8" s="10"/>
+      <c r="AS8" s="11"/>
+      <c r="AT8" s="46"/>
+      <c r="AU8" s="48"/>
+    </row>
+    <row r="9" spans="1:48" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="11">
+        <v>25183</v>
+      </c>
+      <c r="C9" s="11">
+        <v>14164</v>
+      </c>
+      <c r="D9" s="10">
+        <v>0.56240000000000001</v>
+      </c>
+      <c r="E9" s="11">
+        <v>36</v>
+      </c>
+      <c r="F9" s="9">
+        <f t="shared" si="0"/>
+        <v>14128</v>
+      </c>
+      <c r="G9" s="11">
+        <v>4742</v>
+      </c>
+      <c r="H9" s="10">
+        <f t="shared" si="1"/>
+        <v>0.33564552661381652</v>
+      </c>
+      <c r="I9" s="11">
+        <v>8887</v>
+      </c>
+      <c r="J9" s="10">
+        <f t="shared" si="2"/>
+        <v>0.62903454133635339</v>
+      </c>
+      <c r="K9" s="11"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="11">
+        <v>365</v>
+      </c>
+      <c r="R9" s="10">
+        <f t="shared" si="3"/>
+        <v>2.5769556622423043E-2</v>
+      </c>
+      <c r="S9" s="11"/>
+      <c r="T9" s="10"/>
+      <c r="U9" s="11"/>
+      <c r="V9" s="10"/>
+      <c r="W9" s="11">
+        <v>97</v>
+      </c>
+      <c r="X9" s="10">
+        <f t="shared" si="4"/>
+        <v>6.8483479243151655E-3</v>
+      </c>
+      <c r="Y9" s="11">
+        <v>37</v>
+      </c>
+      <c r="Z9" s="10">
+        <f t="shared" ref="Z9:Z35" si="5">SUM(Y9/C9)</f>
+        <v>2.6122564247387744E-3</v>
+      </c>
+      <c r="AA9" s="11"/>
+      <c r="AB9" s="10"/>
+      <c r="AC9" s="11"/>
+      <c r="AD9" s="10"/>
+      <c r="AE9" s="11"/>
+      <c r="AF9" s="10"/>
+      <c r="AG9" s="11"/>
+      <c r="AH9" s="10"/>
+      <c r="AI9" s="11"/>
+      <c r="AJ9" s="10"/>
+      <c r="AK9" s="11"/>
+      <c r="AL9" s="10"/>
+      <c r="AM9" s="11"/>
+      <c r="AN9" s="10"/>
+      <c r="AO9" s="11"/>
+      <c r="AP9" s="10"/>
+      <c r="AQ9" s="11"/>
+      <c r="AR9" s="10"/>
+      <c r="AS9" s="11"/>
+      <c r="AT9" s="46"/>
+      <c r="AU9" s="48"/>
+    </row>
+    <row r="10" spans="1:48" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="11">
+        <v>31460</v>
+      </c>
+      <c r="C10" s="11">
+        <v>18477</v>
+      </c>
+      <c r="D10" s="10">
+        <v>0.58730000000000004</v>
+      </c>
+      <c r="E10" s="11">
+        <v>46</v>
+      </c>
+      <c r="F10" s="9">
+        <f t="shared" si="0"/>
+        <v>18431</v>
+      </c>
+      <c r="G10" s="11">
+        <v>4854</v>
+      </c>
+      <c r="H10" s="10">
+        <f t="shared" si="1"/>
+        <v>0.2633606423959633</v>
+      </c>
+      <c r="I10" s="11">
+        <v>12663</v>
+      </c>
+      <c r="J10" s="10">
+        <f t="shared" si="2"/>
+        <v>0.68704899354348647</v>
+      </c>
+      <c r="K10" s="11"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="11">
+        <v>914</v>
+      </c>
+      <c r="R10" s="10">
+        <f t="shared" si="3"/>
+        <v>4.9466904800562865E-2</v>
+      </c>
+      <c r="S10" s="11"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="11"/>
+      <c r="V10" s="10"/>
+      <c r="W10" s="11"/>
+      <c r="X10" s="10"/>
+      <c r="Y10" s="11"/>
+      <c r="Z10" s="10"/>
+      <c r="AA10" s="11"/>
+      <c r="AB10" s="10"/>
+      <c r="AC10" s="11"/>
+      <c r="AD10" s="10"/>
+      <c r="AE10" s="11"/>
+      <c r="AF10" s="10"/>
+      <c r="AG10" s="11"/>
+      <c r="AH10" s="10"/>
+      <c r="AI10" s="11"/>
+      <c r="AJ10" s="10"/>
+      <c r="AK10" s="11"/>
+      <c r="AL10" s="10"/>
+      <c r="AM10" s="11"/>
+      <c r="AN10" s="10"/>
+      <c r="AO10" s="11"/>
+      <c r="AP10" s="10"/>
+      <c r="AQ10" s="11"/>
+      <c r="AR10" s="10"/>
+      <c r="AS10" s="11"/>
+      <c r="AT10" s="46"/>
+      <c r="AU10" s="48"/>
+    </row>
+    <row r="11" spans="1:48" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="11">
+        <v>30208</v>
+      </c>
+      <c r="C11" s="11">
+        <v>17315</v>
+      </c>
+      <c r="D11" s="10">
+        <v>0.57320000000000004</v>
+      </c>
+      <c r="E11" s="11">
+        <v>40</v>
+      </c>
+      <c r="F11" s="9">
+        <f t="shared" si="0"/>
+        <v>17275</v>
+      </c>
+      <c r="G11" s="11">
+        <v>2757</v>
+      </c>
+      <c r="H11" s="10">
+        <f t="shared" si="1"/>
+        <v>0.15959479015918959</v>
+      </c>
+      <c r="I11" s="11">
+        <v>13957</v>
+      </c>
+      <c r="J11" s="10">
+        <f t="shared" si="2"/>
+        <v>0.80793053545586102</v>
+      </c>
+      <c r="K11" s="11"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="11">
+        <v>561</v>
+      </c>
+      <c r="R11" s="10">
+        <f t="shared" si="3"/>
+        <v>3.2399653479641931E-2</v>
+      </c>
+      <c r="S11" s="11"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="11"/>
+      <c r="V11" s="10"/>
+      <c r="W11" s="11"/>
+      <c r="X11" s="10"/>
+      <c r="Y11" s="11"/>
+      <c r="Z11" s="10"/>
+      <c r="AA11" s="11"/>
+      <c r="AB11" s="10"/>
+      <c r="AC11" s="11"/>
+      <c r="AD11" s="10"/>
+      <c r="AE11" s="11"/>
+      <c r="AF11" s="10"/>
+      <c r="AG11" s="11"/>
+      <c r="AH11" s="10"/>
+      <c r="AI11" s="11"/>
+      <c r="AJ11" s="10"/>
+      <c r="AK11" s="11"/>
+      <c r="AL11" s="10"/>
+      <c r="AM11" s="11"/>
+      <c r="AN11" s="10"/>
+      <c r="AO11" s="11"/>
+      <c r="AP11" s="10"/>
+      <c r="AQ11" s="11"/>
+      <c r="AR11" s="10"/>
+      <c r="AS11" s="11"/>
+      <c r="AT11" s="46"/>
+      <c r="AU11" s="48"/>
+    </row>
+    <row r="12" spans="1:48" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="11">
+        <v>27728</v>
+      </c>
+      <c r="C12" s="11">
+        <v>16110</v>
+      </c>
+      <c r="D12" s="10">
+        <v>0.58099999999999996</v>
+      </c>
+      <c r="E12" s="11">
+        <v>37</v>
+      </c>
+      <c r="F12" s="9">
+        <f t="shared" si="0"/>
+        <v>16073</v>
+      </c>
+      <c r="G12" s="11">
+        <v>5317</v>
+      </c>
+      <c r="H12" s="10">
+        <f t="shared" si="1"/>
+        <v>0.3308032103527655</v>
+      </c>
+      <c r="I12" s="11">
+        <v>10097</v>
+      </c>
+      <c r="J12" s="10">
+        <f t="shared" si="2"/>
+        <v>0.62819635413426245</v>
+      </c>
+      <c r="K12" s="11"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="11">
+        <v>487</v>
+      </c>
+      <c r="R12" s="10">
+        <f t="shared" si="3"/>
+        <v>3.0229671011793916E-2</v>
+      </c>
+      <c r="S12" s="11"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="11"/>
+      <c r="V12" s="10"/>
+      <c r="W12" s="11">
+        <v>125</v>
+      </c>
+      <c r="X12" s="10">
+        <f t="shared" si="4"/>
+        <v>7.7591558038485409E-3</v>
+      </c>
+      <c r="Y12" s="11"/>
+      <c r="Z12" s="10"/>
+      <c r="AA12" s="11"/>
+      <c r="AB12" s="10"/>
+      <c r="AC12" s="11"/>
+      <c r="AD12" s="10"/>
+      <c r="AE12" s="11"/>
+      <c r="AF12" s="10"/>
+      <c r="AG12" s="11"/>
+      <c r="AH12" s="10"/>
+      <c r="AI12" s="11"/>
+      <c r="AJ12" s="10"/>
+      <c r="AK12" s="11"/>
+      <c r="AL12" s="10"/>
+      <c r="AM12" s="11"/>
+      <c r="AN12" s="10"/>
+      <c r="AO12" s="11"/>
+      <c r="AP12" s="10"/>
+      <c r="AQ12" s="11"/>
+      <c r="AR12" s="10"/>
+      <c r="AS12" s="11">
+        <v>47</v>
+      </c>
+      <c r="AT12" s="10">
+        <f>SUM(AS12/C12)</f>
+        <v>2.9174425822470515E-3</v>
+      </c>
+      <c r="AU12" s="48"/>
+    </row>
+    <row r="13" spans="1:48" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="11">
+        <v>29043</v>
+      </c>
+      <c r="C13" s="11">
+        <v>18046</v>
+      </c>
+      <c r="D13" s="10">
+        <v>0.62139999999999995</v>
+      </c>
+      <c r="E13" s="11">
+        <v>44</v>
+      </c>
+      <c r="F13" s="9">
+        <f t="shared" si="0"/>
+        <v>18002</v>
+      </c>
+      <c r="G13" s="11">
+        <v>1390</v>
+      </c>
+      <c r="H13" s="10">
+        <f t="shared" si="1"/>
+        <v>7.7213642928563489E-2</v>
+      </c>
+      <c r="I13" s="11">
+        <v>16013</v>
+      </c>
+      <c r="J13" s="10">
+        <f t="shared" si="2"/>
+        <v>0.88951227641373176</v>
+      </c>
+      <c r="K13" s="11"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="11">
+        <v>599</v>
+      </c>
+      <c r="R13" s="10">
+        <f t="shared" si="3"/>
+        <v>3.3192951346558794E-2</v>
+      </c>
+      <c r="S13" s="11"/>
+      <c r="T13" s="10"/>
+      <c r="U13" s="11"/>
+      <c r="V13" s="10"/>
+      <c r="W13" s="11"/>
+      <c r="X13" s="10"/>
+      <c r="Y13" s="11"/>
+      <c r="Z13" s="10"/>
+      <c r="AA13" s="11"/>
+      <c r="AB13" s="10"/>
+      <c r="AC13" s="11"/>
+      <c r="AD13" s="10"/>
+      <c r="AE13" s="11"/>
+      <c r="AF13" s="10"/>
+      <c r="AG13" s="11"/>
+      <c r="AH13" s="10"/>
+      <c r="AI13" s="11"/>
+      <c r="AJ13" s="10"/>
+      <c r="AK13" s="11"/>
+      <c r="AL13" s="10"/>
+      <c r="AM13" s="11"/>
+      <c r="AN13" s="10"/>
+      <c r="AO13" s="11"/>
+      <c r="AP13" s="10"/>
+      <c r="AQ13" s="11"/>
+      <c r="AR13" s="10"/>
+      <c r="AS13" s="11"/>
+      <c r="AT13" s="46"/>
+      <c r="AU13" s="48"/>
+    </row>
+    <row r="14" spans="1:48" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="11">
+        <v>30681</v>
+      </c>
+      <c r="C14" s="11">
+        <v>18064</v>
+      </c>
+      <c r="D14" s="10">
+        <v>0.58879999999999999</v>
+      </c>
+      <c r="E14" s="11">
+        <v>42</v>
+      </c>
+      <c r="F14" s="9">
+        <f t="shared" si="0"/>
+        <v>18022</v>
+      </c>
+      <c r="G14" s="11">
+        <v>3094</v>
+      </c>
+      <c r="H14" s="10">
+        <f t="shared" si="1"/>
+        <v>0.17167905892797691</v>
+      </c>
+      <c r="I14" s="11">
+        <v>13201</v>
+      </c>
+      <c r="J14" s="10">
+        <f t="shared" si="2"/>
+        <v>0.7324936189102208</v>
+      </c>
+      <c r="K14" s="11"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="11">
+        <v>1727</v>
+      </c>
+      <c r="R14" s="10">
+        <f t="shared" si="3"/>
+        <v>9.5604517271922054E-2</v>
+      </c>
+      <c r="S14" s="11"/>
+      <c r="T14" s="10"/>
+      <c r="U14" s="11"/>
+      <c r="V14" s="10"/>
+      <c r="W14" s="11"/>
+      <c r="X14" s="10"/>
+      <c r="Y14" s="11"/>
+      <c r="Z14" s="10"/>
+      <c r="AA14" s="11"/>
+      <c r="AB14" s="10"/>
+      <c r="AC14" s="11"/>
+      <c r="AD14" s="10"/>
+      <c r="AE14" s="11"/>
+      <c r="AF14" s="10"/>
+      <c r="AG14" s="11"/>
+      <c r="AH14" s="10"/>
+      <c r="AI14" s="11"/>
+      <c r="AJ14" s="10"/>
+      <c r="AK14" s="11"/>
+      <c r="AL14" s="10"/>
+      <c r="AM14" s="11"/>
+      <c r="AN14" s="10"/>
+      <c r="AO14" s="11"/>
+      <c r="AP14" s="10"/>
+      <c r="AQ14" s="11"/>
+      <c r="AR14" s="10"/>
+      <c r="AS14" s="11"/>
+      <c r="AT14" s="46"/>
+      <c r="AU14" s="48"/>
+    </row>
+    <row r="15" spans="1:48" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="11">
+        <v>30975</v>
+      </c>
+      <c r="C15" s="11">
+        <v>17881</v>
+      </c>
+      <c r="D15" s="10">
+        <v>0.57730000000000004</v>
+      </c>
+      <c r="E15" s="11">
+        <v>41</v>
+      </c>
+      <c r="F15" s="9">
+        <f t="shared" si="0"/>
+        <v>17840</v>
+      </c>
+      <c r="G15" s="11">
+        <v>3763</v>
+      </c>
+      <c r="H15" s="10">
+        <f t="shared" si="1"/>
+        <v>0.2109304932735426</v>
+      </c>
+      <c r="I15" s="11">
+        <v>13122</v>
+      </c>
+      <c r="J15" s="10">
+        <f t="shared" si="2"/>
+        <v>0.73553811659192825</v>
+      </c>
+      <c r="K15" s="11"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="11">
+        <v>955</v>
+      </c>
+      <c r="R15" s="10">
+        <f t="shared" si="3"/>
+        <v>5.3408646048878697E-2</v>
+      </c>
+      <c r="S15" s="11"/>
+      <c r="T15" s="10"/>
+      <c r="U15" s="11"/>
+      <c r="V15" s="10"/>
+      <c r="W15" s="11"/>
+      <c r="X15" s="10"/>
+      <c r="Y15" s="11"/>
+      <c r="Z15" s="10"/>
+      <c r="AA15" s="11"/>
+      <c r="AB15" s="10"/>
+      <c r="AC15" s="11"/>
+      <c r="AD15" s="10"/>
+      <c r="AE15" s="11"/>
+      <c r="AF15" s="10"/>
+      <c r="AG15" s="11"/>
+      <c r="AH15" s="10"/>
+      <c r="AI15" s="11"/>
+      <c r="AJ15" s="10"/>
+      <c r="AK15" s="11"/>
+      <c r="AL15" s="10"/>
+      <c r="AM15" s="11"/>
+      <c r="AN15" s="10"/>
+      <c r="AO15" s="11"/>
+      <c r="AP15" s="10"/>
+      <c r="AQ15" s="11"/>
+      <c r="AR15" s="10"/>
+      <c r="AS15" s="11"/>
+      <c r="AT15" s="46"/>
+      <c r="AU15" s="48"/>
+    </row>
+    <row r="16" spans="1:48" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="11">
+        <v>30776</v>
+      </c>
+      <c r="C16" s="11">
+        <v>18447</v>
+      </c>
+      <c r="D16" s="10">
+        <v>0.59940000000000004</v>
+      </c>
+      <c r="E16" s="11">
+        <v>57</v>
+      </c>
+      <c r="F16" s="9">
+        <f t="shared" si="0"/>
+        <v>18390</v>
+      </c>
+      <c r="G16" s="11">
+        <v>5393</v>
+      </c>
+      <c r="H16" s="10">
+        <f t="shared" si="1"/>
+        <v>0.29325720500271885</v>
+      </c>
+      <c r="I16" s="11">
+        <v>12559</v>
+      </c>
+      <c r="J16" s="10">
+        <f t="shared" si="2"/>
+        <v>0.68292550299075583</v>
+      </c>
+      <c r="K16" s="11"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="11">
+        <v>438</v>
+      </c>
+      <c r="R16" s="10">
+        <f t="shared" si="3"/>
+        <v>2.3743698162302814E-2</v>
+      </c>
+      <c r="S16" s="11"/>
+      <c r="T16" s="10"/>
+      <c r="U16" s="11"/>
+      <c r="V16" s="10"/>
+      <c r="W16" s="11"/>
+      <c r="X16" s="10"/>
+      <c r="Y16" s="11"/>
+      <c r="Z16" s="10"/>
+      <c r="AA16" s="11"/>
+      <c r="AB16" s="10"/>
+      <c r="AC16" s="11"/>
+      <c r="AD16" s="10"/>
+      <c r="AE16" s="11"/>
+      <c r="AF16" s="10"/>
+      <c r="AG16" s="11"/>
+      <c r="AH16" s="10"/>
+      <c r="AI16" s="11"/>
+      <c r="AJ16" s="10"/>
+      <c r="AK16" s="11"/>
+      <c r="AL16" s="10"/>
+      <c r="AM16" s="11"/>
+      <c r="AN16" s="10"/>
+      <c r="AO16" s="11"/>
+      <c r="AP16" s="10"/>
+      <c r="AQ16" s="11"/>
+      <c r="AR16" s="10"/>
+      <c r="AS16" s="11"/>
+      <c r="AT16" s="46"/>
+      <c r="AU16" s="48"/>
+    </row>
+    <row r="17" spans="1:47" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="11">
+        <v>29515</v>
+      </c>
+      <c r="C17" s="11">
+        <v>16000</v>
+      </c>
+      <c r="D17" s="10">
+        <v>0.54210000000000003</v>
+      </c>
+      <c r="E17" s="11">
+        <v>48</v>
+      </c>
+      <c r="F17" s="9">
+        <f>SUM(C17-E17)</f>
+        <v>15952</v>
+      </c>
+      <c r="G17" s="11">
+        <v>7690</v>
+      </c>
+      <c r="H17" s="10">
+        <f>SUM(G17/F17)</f>
+        <v>0.48207121364092276</v>
+      </c>
+      <c r="I17" s="11">
+        <v>7428</v>
+      </c>
+      <c r="J17" s="10">
+        <f>SUM(I17/F17)</f>
+        <v>0.46564694082246738</v>
+      </c>
+      <c r="K17" s="11"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="11">
+        <v>834</v>
+      </c>
+      <c r="R17" s="10">
+        <f>SUM(Q17/C17)</f>
+        <v>5.2124999999999998E-2</v>
+      </c>
+      <c r="S17" s="11"/>
+      <c r="T17" s="10"/>
+      <c r="U17" s="11"/>
+      <c r="V17" s="10"/>
+      <c r="W17" s="11"/>
+      <c r="X17" s="10"/>
+      <c r="Y17" s="11"/>
+      <c r="Z17" s="10"/>
+      <c r="AA17" s="11"/>
+      <c r="AB17" s="10"/>
+      <c r="AC17" s="11"/>
+      <c r="AD17" s="10"/>
+      <c r="AE17" s="11"/>
+      <c r="AF17" s="10"/>
+      <c r="AG17" s="11"/>
+      <c r="AH17" s="10"/>
+      <c r="AI17" s="11"/>
+      <c r="AJ17" s="10"/>
+      <c r="AK17" s="11"/>
+      <c r="AL17" s="10"/>
+      <c r="AM17" s="11"/>
+      <c r="AN17" s="10"/>
+      <c r="AO17" s="11"/>
+      <c r="AP17" s="10"/>
+      <c r="AQ17" s="11"/>
+      <c r="AR17" s="10"/>
+      <c r="AS17" s="11"/>
+      <c r="AT17" s="46"/>
+      <c r="AU17" s="48"/>
+    </row>
+    <row r="18" spans="1:47" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="11">
+        <v>29623</v>
+      </c>
+      <c r="C18" s="11">
+        <v>13149</v>
+      </c>
+      <c r="D18" s="10">
+        <v>0.44390000000000002</v>
+      </c>
+      <c r="E18" s="11">
+        <v>55</v>
+      </c>
+      <c r="F18" s="9">
+        <f t="shared" si="0"/>
+        <v>13094</v>
+      </c>
+      <c r="G18" s="11">
+        <v>7409</v>
+      </c>
+      <c r="H18" s="10">
+        <f t="shared" si="1"/>
+        <v>0.56583167863143424</v>
+      </c>
+      <c r="I18" s="11">
+        <v>4600</v>
+      </c>
+      <c r="J18" s="10">
+        <f t="shared" si="2"/>
+        <v>0.35130594165266532</v>
+      </c>
+      <c r="K18" s="11"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S18" s="11"/>
+      <c r="T18" s="10"/>
+      <c r="U18" s="11"/>
+      <c r="V18" s="10"/>
+      <c r="W18" s="11">
+        <v>1085</v>
+      </c>
+      <c r="X18" s="10">
+        <f t="shared" si="4"/>
+        <v>8.2515780667731381E-2</v>
+      </c>
+      <c r="Y18" s="11"/>
+      <c r="Z18" s="10"/>
+      <c r="AA18" s="11"/>
+      <c r="AB18" s="10"/>
+      <c r="AC18" s="11"/>
+      <c r="AD18" s="10"/>
+      <c r="AE18" s="11"/>
+      <c r="AF18" s="10"/>
+      <c r="AG18" s="11"/>
+      <c r="AH18" s="10"/>
+      <c r="AI18" s="11"/>
+      <c r="AJ18" s="10"/>
+      <c r="AK18" s="11"/>
+      <c r="AL18" s="10"/>
+      <c r="AM18" s="11"/>
+      <c r="AN18" s="10"/>
+      <c r="AO18" s="11"/>
+      <c r="AP18" s="10"/>
+      <c r="AQ18" s="11"/>
+      <c r="AR18" s="10"/>
+      <c r="AS18" s="11"/>
+      <c r="AT18" s="46"/>
+      <c r="AU18" s="48"/>
+    </row>
+    <row r="19" spans="1:47" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="11">
+        <v>29869</v>
+      </c>
+      <c r="C19" s="11">
+        <v>12612</v>
+      </c>
+      <c r="D19" s="10">
+        <v>0.42220000000000002</v>
+      </c>
+      <c r="E19" s="11">
+        <v>49</v>
+      </c>
+      <c r="F19" s="9">
+        <f t="shared" si="0"/>
+        <v>12563</v>
+      </c>
+      <c r="G19" s="11">
+        <v>7064</v>
+      </c>
+      <c r="H19" s="10">
+        <f t="shared" si="1"/>
+        <v>0.56228607816604315</v>
+      </c>
+      <c r="I19" s="11">
+        <v>3525</v>
+      </c>
+      <c r="J19" s="10">
+        <f t="shared" si="2"/>
+        <v>0.28058584732945951</v>
+      </c>
+      <c r="K19" s="11"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="11">
+        <v>708</v>
+      </c>
+      <c r="R19" s="10">
+        <f t="shared" si="3"/>
+        <v>5.6137012369172214E-2</v>
+      </c>
+      <c r="S19" s="11">
+        <v>556</v>
+      </c>
+      <c r="T19" s="10">
+        <f>SUM(S19/C19)</f>
+        <v>4.4084998414208688E-2</v>
+      </c>
+      <c r="U19" s="11"/>
+      <c r="V19" s="10"/>
+      <c r="W19" s="11">
+        <v>565</v>
+      </c>
+      <c r="X19" s="10">
+        <f t="shared" si="4"/>
+        <v>4.4798604503647317E-2</v>
+      </c>
+      <c r="Y19" s="11">
+        <v>145</v>
+      </c>
+      <c r="Z19" s="10">
+        <f t="shared" si="5"/>
+        <v>1.149698699651126E-2</v>
+      </c>
+      <c r="AA19" s="11"/>
+      <c r="AB19" s="10"/>
+      <c r="AC19" s="11"/>
+      <c r="AD19" s="10"/>
+      <c r="AE19" s="11"/>
+      <c r="AF19" s="10"/>
+      <c r="AG19" s="11"/>
+      <c r="AH19" s="10"/>
+      <c r="AI19" s="11"/>
+      <c r="AJ19" s="10"/>
+      <c r="AK19" s="11"/>
+      <c r="AL19" s="10"/>
+      <c r="AM19" s="11"/>
+      <c r="AN19" s="10"/>
+      <c r="AO19" s="11"/>
+      <c r="AP19" s="10"/>
+      <c r="AQ19" s="11"/>
+      <c r="AR19" s="10"/>
+      <c r="AS19" s="11"/>
+      <c r="AT19" s="46"/>
+      <c r="AU19" s="48"/>
+    </row>
+    <row r="20" spans="1:47" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" s="11">
+        <v>29967</v>
+      </c>
+      <c r="C20" s="11">
+        <v>12358</v>
+      </c>
+      <c r="D20" s="10">
+        <v>0.41239999999999999</v>
+      </c>
+      <c r="E20" s="11">
+        <v>62</v>
+      </c>
+      <c r="F20" s="9">
+        <f t="shared" si="0"/>
+        <v>12296</v>
+      </c>
+      <c r="G20" s="11">
+        <v>7703</v>
+      </c>
+      <c r="H20" s="10">
+        <f t="shared" si="1"/>
+        <v>0.62646389069616137</v>
+      </c>
+      <c r="I20" s="11">
+        <v>3257</v>
+      </c>
+      <c r="J20" s="10">
+        <f t="shared" si="2"/>
+        <v>0.2648828887443071</v>
+      </c>
+      <c r="K20" s="11"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S20" s="11"/>
+      <c r="T20" s="10"/>
+      <c r="U20" s="11"/>
+      <c r="V20" s="10"/>
+      <c r="W20" s="11">
+        <v>1336</v>
+      </c>
+      <c r="X20" s="10">
+        <f t="shared" si="4"/>
+        <v>0.10810810810810811</v>
+      </c>
+      <c r="Y20" s="11"/>
+      <c r="Z20" s="10"/>
+      <c r="AA20" s="11"/>
+      <c r="AB20" s="10"/>
+      <c r="AC20" s="11"/>
+      <c r="AD20" s="10"/>
+      <c r="AE20" s="11"/>
+      <c r="AF20" s="10"/>
+      <c r="AG20" s="11"/>
+      <c r="AH20" s="10"/>
+      <c r="AI20" s="11"/>
+      <c r="AJ20" s="10"/>
+      <c r="AK20" s="11"/>
+      <c r="AL20" s="10"/>
+      <c r="AM20" s="11"/>
+      <c r="AN20" s="10"/>
+      <c r="AO20" s="11"/>
+      <c r="AP20" s="10"/>
+      <c r="AQ20" s="11"/>
+      <c r="AR20" s="10"/>
+      <c r="AS20" s="11"/>
+      <c r="AT20" s="46"/>
+      <c r="AU20" s="48"/>
+    </row>
+    <row r="21" spans="1:47" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" s="11">
+        <v>27471</v>
+      </c>
+      <c r="C21" s="11">
+        <v>16422</v>
+      </c>
+      <c r="D21" s="10">
+        <v>0.5978</v>
+      </c>
+      <c r="E21" s="11">
+        <v>33</v>
+      </c>
+      <c r="F21" s="9">
+        <f t="shared" si="0"/>
+        <v>16389</v>
+      </c>
+      <c r="G21" s="11">
+        <v>4454</v>
+      </c>
+      <c r="H21" s="10">
+        <f t="shared" si="1"/>
+        <v>0.27176764903288791</v>
+      </c>
+      <c r="I21" s="11">
+        <v>11396</v>
+      </c>
+      <c r="J21" s="10">
+        <f t="shared" si="2"/>
+        <v>0.69534443834279092</v>
+      </c>
+      <c r="K21" s="11"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="11">
+        <v>539</v>
+      </c>
+      <c r="R21" s="10">
+        <f t="shared" si="3"/>
+        <v>3.2821824381926684E-2</v>
+      </c>
+      <c r="S21" s="11"/>
+      <c r="T21" s="10"/>
+      <c r="U21" s="11"/>
+      <c r="V21" s="10"/>
+      <c r="W21" s="11"/>
+      <c r="X21" s="10"/>
+      <c r="Y21" s="11"/>
+      <c r="Z21" s="10"/>
+      <c r="AA21" s="11"/>
+      <c r="AB21" s="10"/>
+      <c r="AC21" s="11"/>
+      <c r="AD21" s="10"/>
+      <c r="AE21" s="11"/>
+      <c r="AF21" s="10"/>
+      <c r="AG21" s="11"/>
+      <c r="AH21" s="10"/>
+      <c r="AI21" s="11"/>
+      <c r="AJ21" s="10"/>
+      <c r="AK21" s="11"/>
+      <c r="AL21" s="10"/>
+      <c r="AM21" s="11"/>
+      <c r="AN21" s="10"/>
+      <c r="AO21" s="11"/>
+      <c r="AP21" s="10"/>
+      <c r="AQ21" s="11"/>
+      <c r="AR21" s="10"/>
+      <c r="AS21" s="11"/>
+      <c r="AT21" s="46"/>
+      <c r="AU21" s="48"/>
+    </row>
+    <row r="22" spans="1:47" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="11">
+        <v>26616</v>
+      </c>
+      <c r="C22" s="11">
+        <v>13824</v>
+      </c>
+      <c r="D22" s="10">
+        <v>0.51939999999999997</v>
+      </c>
+      <c r="E22" s="11">
+        <v>71</v>
+      </c>
+      <c r="F22" s="9">
+        <f t="shared" si="0"/>
+        <v>13753</v>
+      </c>
+      <c r="G22" s="11">
+        <v>6262</v>
+      </c>
+      <c r="H22" s="10">
+        <f t="shared" si="1"/>
+        <v>0.45531883952592161</v>
+      </c>
+      <c r="I22" s="11">
+        <v>7001</v>
+      </c>
+      <c r="J22" s="10">
+        <f t="shared" si="2"/>
+        <v>0.50905257034828766</v>
+      </c>
+      <c r="K22" s="11"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="11">
+        <v>413</v>
+      </c>
+      <c r="R22" s="10">
+        <f t="shared" si="3"/>
+        <v>2.9875578703703703E-2</v>
+      </c>
+      <c r="S22" s="11"/>
+      <c r="T22" s="10"/>
+      <c r="U22" s="11"/>
+      <c r="V22" s="10"/>
+      <c r="W22" s="11"/>
+      <c r="X22" s="10"/>
+      <c r="Y22" s="11">
+        <v>53</v>
+      </c>
+      <c r="Z22" s="10">
+        <f t="shared" si="5"/>
+        <v>3.8339120370370371E-3</v>
+      </c>
+      <c r="AA22" s="11"/>
+      <c r="AB22" s="10"/>
+      <c r="AC22" s="11">
+        <v>24</v>
+      </c>
+      <c r="AD22" s="10">
+        <f>SUM(AC22/C22)</f>
+        <v>1.736111111111111E-3</v>
+      </c>
+      <c r="AE22" s="11"/>
+      <c r="AF22" s="10"/>
+      <c r="AG22" s="11"/>
+      <c r="AH22" s="10"/>
+      <c r="AI22" s="11"/>
+      <c r="AJ22" s="10"/>
+      <c r="AK22" s="11"/>
+      <c r="AL22" s="10"/>
+      <c r="AM22" s="11"/>
+      <c r="AN22" s="10"/>
+      <c r="AO22" s="11"/>
+      <c r="AP22" s="10"/>
+      <c r="AQ22" s="11"/>
+      <c r="AR22" s="10"/>
+      <c r="AS22" s="11"/>
+      <c r="AT22" s="46"/>
+      <c r="AU22" s="48"/>
+    </row>
+    <row r="23" spans="1:47" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="11">
+        <v>29061</v>
+      </c>
+      <c r="C23" s="11">
+        <v>16960</v>
+      </c>
+      <c r="D23" s="10">
+        <v>0.58360000000000001</v>
+      </c>
+      <c r="E23" s="11">
+        <v>54</v>
+      </c>
+      <c r="F23" s="9">
+        <f t="shared" si="0"/>
+        <v>16906</v>
+      </c>
+      <c r="G23" s="11">
+        <v>6712</v>
+      </c>
+      <c r="H23" s="10">
+        <f t="shared" si="1"/>
+        <v>0.3970188098899799</v>
+      </c>
+      <c r="I23" s="11">
+        <v>9585</v>
+      </c>
+      <c r="J23" s="10">
+        <f t="shared" si="2"/>
+        <v>0.56695847628061047</v>
+      </c>
+      <c r="K23" s="11"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="11"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="11">
+        <v>502</v>
+      </c>
+      <c r="R23" s="10">
+        <f t="shared" si="3"/>
+        <v>2.9599056603773585E-2</v>
+      </c>
+      <c r="S23" s="11"/>
+      <c r="T23" s="10"/>
+      <c r="U23" s="11"/>
+      <c r="V23" s="10"/>
+      <c r="W23" s="11">
+        <v>107</v>
+      </c>
+      <c r="X23" s="10">
+        <f t="shared" si="4"/>
+        <v>6.3089622641509437E-3</v>
+      </c>
+      <c r="Y23" s="11"/>
+      <c r="Z23" s="10"/>
+      <c r="AA23" s="11"/>
+      <c r="AB23" s="10"/>
+      <c r="AC23" s="11"/>
+      <c r="AD23" s="10"/>
+      <c r="AE23" s="11"/>
+      <c r="AF23" s="10"/>
+      <c r="AG23" s="11"/>
+      <c r="AH23" s="10"/>
+      <c r="AI23" s="11"/>
+      <c r="AJ23" s="10"/>
+      <c r="AK23" s="11"/>
+      <c r="AL23" s="10"/>
+      <c r="AM23" s="11"/>
+      <c r="AN23" s="10"/>
+      <c r="AO23" s="11"/>
+      <c r="AP23" s="10"/>
+      <c r="AQ23" s="11"/>
+      <c r="AR23" s="10"/>
+      <c r="AS23" s="11"/>
+      <c r="AT23" s="46"/>
+      <c r="AU23" s="48"/>
+    </row>
+    <row r="24" spans="1:47" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" s="11">
+        <v>25231</v>
+      </c>
+      <c r="C24" s="11">
+        <v>9781</v>
+      </c>
+      <c r="D24" s="10">
+        <v>0.38769999999999999</v>
+      </c>
+      <c r="E24" s="11">
+        <v>22</v>
+      </c>
+      <c r="F24" s="9">
+        <f t="shared" si="0"/>
+        <v>9759</v>
+      </c>
+      <c r="G24" s="11">
+        <v>5837</v>
+      </c>
+      <c r="H24" s="10">
+        <f t="shared" si="1"/>
+        <v>0.59811456091812687</v>
+      </c>
+      <c r="I24" s="11">
+        <v>3270</v>
+      </c>
+      <c r="J24" s="10">
+        <f t="shared" si="2"/>
+        <v>0.3350753150937596</v>
+      </c>
+      <c r="K24" s="11"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="11"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="11">
+        <v>577</v>
+      </c>
+      <c r="R24" s="10">
+        <f t="shared" si="3"/>
+        <v>5.8991923116245785E-2</v>
+      </c>
+      <c r="S24" s="11"/>
+      <c r="T24" s="10"/>
+      <c r="U24" s="11"/>
+      <c r="V24" s="10"/>
+      <c r="W24" s="11"/>
+      <c r="X24" s="10"/>
+      <c r="Y24" s="11">
+        <v>75</v>
+      </c>
+      <c r="Z24" s="10">
+        <f t="shared" si="5"/>
+        <v>7.6679276147633164E-3</v>
+      </c>
+      <c r="AA24" s="11"/>
+      <c r="AB24" s="10"/>
+      <c r="AC24" s="11"/>
+      <c r="AD24" s="10"/>
+      <c r="AE24" s="11"/>
+      <c r="AF24" s="10"/>
+      <c r="AG24" s="11"/>
+      <c r="AH24" s="10"/>
+      <c r="AI24" s="11"/>
+      <c r="AJ24" s="10"/>
+      <c r="AK24" s="11"/>
+      <c r="AL24" s="10"/>
+      <c r="AM24" s="11"/>
+      <c r="AN24" s="10"/>
+      <c r="AO24" s="11"/>
+      <c r="AP24" s="10"/>
+      <c r="AQ24" s="11"/>
+      <c r="AR24" s="10"/>
+      <c r="AS24" s="11"/>
+      <c r="AT24" s="46"/>
+      <c r="AU24" s="48"/>
+    </row>
+    <row r="25" spans="1:47" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25" s="11">
+        <v>25147</v>
+      </c>
+      <c r="C25" s="11">
+        <v>8852</v>
+      </c>
+      <c r="D25" s="10">
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="E25" s="11">
+        <v>36</v>
+      </c>
+      <c r="F25" s="9">
+        <f t="shared" si="0"/>
+        <v>8816</v>
+      </c>
+      <c r="G25" s="11">
+        <v>6096</v>
+      </c>
+      <c r="H25" s="10">
+        <f t="shared" si="1"/>
+        <v>0.69147005444646104</v>
+      </c>
+      <c r="I25" s="11">
+        <v>2291</v>
+      </c>
+      <c r="J25" s="10">
+        <f t="shared" si="2"/>
+        <v>0.25986842105263158</v>
+      </c>
+      <c r="K25" s="11"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="11"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="11">
+        <v>429</v>
+      </c>
+      <c r="R25" s="10">
+        <f t="shared" si="3"/>
+        <v>4.8463624039765021E-2</v>
+      </c>
+      <c r="S25" s="11"/>
+      <c r="T25" s="10"/>
+      <c r="U25" s="11"/>
+      <c r="V25" s="10"/>
+      <c r="W25" s="11"/>
+      <c r="X25" s="10"/>
+      <c r="Y25" s="11"/>
+      <c r="Z25" s="10"/>
+      <c r="AA25" s="11"/>
+      <c r="AB25" s="10"/>
+      <c r="AC25" s="11"/>
+      <c r="AD25" s="10"/>
+      <c r="AE25" s="11"/>
+      <c r="AF25" s="10"/>
+      <c r="AG25" s="11"/>
+      <c r="AH25" s="10"/>
+      <c r="AI25" s="11"/>
+      <c r="AJ25" s="10"/>
+      <c r="AK25" s="11"/>
+      <c r="AL25" s="10"/>
+      <c r="AM25" s="11"/>
+      <c r="AN25" s="10"/>
+      <c r="AO25" s="11"/>
+      <c r="AP25" s="10"/>
+      <c r="AQ25" s="11"/>
+      <c r="AR25" s="10"/>
+      <c r="AS25" s="11"/>
+      <c r="AT25" s="46"/>
+      <c r="AU25" s="48"/>
+    </row>
+    <row r="26" spans="1:47" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26" s="11">
+        <v>28493</v>
+      </c>
+      <c r="C26" s="11">
+        <v>16381</v>
+      </c>
+      <c r="D26" s="10">
+        <v>0.57489999999999997</v>
+      </c>
+      <c r="E26" s="11">
+        <v>37</v>
+      </c>
+      <c r="F26" s="9">
+        <f>SUM(C26-E26)</f>
+        <v>16344</v>
+      </c>
+      <c r="G26" s="11">
+        <v>7961</v>
+      </c>
+      <c r="H26" s="10">
+        <f>SUM(G26/F26)</f>
+        <v>0.48709006363191387</v>
+      </c>
+      <c r="I26" s="11">
+        <v>7699</v>
+      </c>
+      <c r="J26" s="10">
+        <f>SUM(I26/F26)</f>
+        <v>0.47105971610376896</v>
+      </c>
+      <c r="K26" s="11"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="11"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="11">
+        <v>538</v>
+      </c>
+      <c r="R26" s="10">
+        <f>SUM(Q26/C26)</f>
+        <v>3.2842927782186677E-2</v>
+      </c>
+      <c r="S26" s="11"/>
+      <c r="T26" s="10"/>
+      <c r="U26" s="11"/>
+      <c r="V26" s="10"/>
+      <c r="W26" s="11">
+        <v>146</v>
+      </c>
+      <c r="X26" s="10">
+        <f>SUM(W26/C26)</f>
+        <v>8.9127647884744525E-3</v>
+      </c>
+      <c r="Y26" s="11"/>
+      <c r="Z26" s="10"/>
+      <c r="AA26" s="11"/>
+      <c r="AB26" s="10"/>
+      <c r="AC26" s="11"/>
+      <c r="AD26" s="10"/>
+      <c r="AE26" s="11"/>
+      <c r="AF26" s="10"/>
+      <c r="AG26" s="11"/>
+      <c r="AH26" s="10"/>
+      <c r="AI26" s="11"/>
+      <c r="AJ26" s="10"/>
+      <c r="AK26" s="11"/>
+      <c r="AL26" s="10"/>
+      <c r="AM26" s="11"/>
+      <c r="AN26" s="10"/>
+      <c r="AO26" s="11"/>
+      <c r="AP26" s="10"/>
+      <c r="AQ26" s="11"/>
+      <c r="AR26" s="10"/>
+      <c r="AS26" s="11"/>
+      <c r="AT26" s="46"/>
+      <c r="AU26" s="48"/>
+    </row>
+    <row r="27" spans="1:47" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" s="11">
+        <v>29346</v>
+      </c>
+      <c r="C27" s="11">
+        <v>16030</v>
+      </c>
+      <c r="D27" s="10">
+        <v>0.54620000000000002</v>
+      </c>
+      <c r="E27" s="11">
+        <v>61</v>
+      </c>
+      <c r="F27" s="9">
+        <f t="shared" si="0"/>
+        <v>15969</v>
+      </c>
+      <c r="G27" s="11">
+        <v>4381</v>
+      </c>
+      <c r="H27" s="10">
+        <f t="shared" si="1"/>
+        <v>0.27434404158056236</v>
+      </c>
+      <c r="I27" s="11">
+        <v>11241</v>
+      </c>
+      <c r="J27" s="10">
+        <f t="shared" si="2"/>
+        <v>0.70392635731730224</v>
+      </c>
+      <c r="K27" s="11"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="11"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="11"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="11">
+        <v>347</v>
+      </c>
+      <c r="R27" s="10">
+        <f t="shared" si="3"/>
+        <v>2.164691203992514E-2</v>
+      </c>
+      <c r="S27" s="11"/>
+      <c r="T27" s="10"/>
+      <c r="U27" s="11"/>
+      <c r="V27" s="10"/>
+      <c r="W27" s="11"/>
+      <c r="X27" s="10"/>
+      <c r="Y27" s="11"/>
+      <c r="Z27" s="10"/>
+      <c r="AA27" s="11"/>
+      <c r="AB27" s="10"/>
+      <c r="AC27" s="11"/>
+      <c r="AD27" s="10"/>
+      <c r="AE27" s="11"/>
+      <c r="AF27" s="10"/>
+      <c r="AG27" s="11"/>
+      <c r="AH27" s="10"/>
+      <c r="AI27" s="11"/>
+      <c r="AJ27" s="10"/>
+      <c r="AK27" s="11"/>
+      <c r="AL27" s="10"/>
+      <c r="AM27" s="11"/>
+      <c r="AN27" s="10"/>
+      <c r="AO27" s="11"/>
+      <c r="AP27" s="10"/>
+      <c r="AQ27" s="11"/>
+      <c r="AR27" s="10"/>
+      <c r="AS27" s="11"/>
+      <c r="AT27" s="46"/>
+      <c r="AU27" s="48"/>
+    </row>
+    <row r="28" spans="1:47" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28" s="11">
+        <v>29744</v>
+      </c>
+      <c r="C28" s="11">
+        <v>19448</v>
+      </c>
+      <c r="D28" s="10">
+        <v>0.65380000000000005</v>
+      </c>
+      <c r="E28" s="11">
+        <v>101</v>
+      </c>
+      <c r="F28" s="9">
+        <f t="shared" si="0"/>
+        <v>19347</v>
+      </c>
+      <c r="G28" s="11">
+        <v>7983</v>
+      </c>
+      <c r="H28" s="10">
+        <f t="shared" si="1"/>
+        <v>0.41262211195534193</v>
+      </c>
+      <c r="I28" s="11">
+        <v>11083</v>
+      </c>
+      <c r="J28" s="10">
+        <f t="shared" si="2"/>
+        <v>0.57285367240399032</v>
+      </c>
+      <c r="K28" s="11"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="11"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="11">
+        <v>281</v>
+      </c>
+      <c r="R28" s="10">
+        <f t="shared" si="3"/>
+        <v>1.4448786507610037E-2</v>
+      </c>
+      <c r="S28" s="11"/>
+      <c r="T28" s="10"/>
+      <c r="U28" s="11"/>
+      <c r="V28" s="10"/>
+      <c r="W28" s="11"/>
+      <c r="X28" s="10"/>
+      <c r="Y28" s="11"/>
+      <c r="Z28" s="10"/>
+      <c r="AA28" s="11"/>
+      <c r="AB28" s="10"/>
+      <c r="AC28" s="11"/>
+      <c r="AD28" s="10"/>
+      <c r="AE28" s="11"/>
+      <c r="AF28" s="10"/>
+      <c r="AG28" s="11"/>
+      <c r="AH28" s="10"/>
+      <c r="AI28" s="11"/>
+      <c r="AJ28" s="10"/>
+      <c r="AK28" s="11"/>
+      <c r="AL28" s="10"/>
+      <c r="AM28" s="11"/>
+      <c r="AN28" s="10"/>
+      <c r="AO28" s="11"/>
+      <c r="AP28" s="10"/>
+      <c r="AQ28" s="11"/>
+      <c r="AR28" s="10"/>
+      <c r="AS28" s="11"/>
+      <c r="AT28" s="46"/>
+      <c r="AU28" s="48"/>
+    </row>
+    <row r="29" spans="1:47" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" s="11">
+        <v>27150</v>
+      </c>
+      <c r="C29" s="11">
+        <v>15799</v>
+      </c>
+      <c r="D29" s="10">
+        <v>0.58189999999999997</v>
+      </c>
+      <c r="E29" s="11">
+        <v>38</v>
+      </c>
+      <c r="F29" s="9">
+        <f t="shared" si="0"/>
+        <v>15761</v>
+      </c>
+      <c r="G29" s="11">
+        <v>1650</v>
+      </c>
+      <c r="H29" s="10">
+        <f t="shared" si="1"/>
+        <v>0.10468878878243766</v>
+      </c>
+      <c r="I29" s="11">
+        <v>13649</v>
+      </c>
+      <c r="J29" s="10">
+        <f t="shared" si="2"/>
+        <v>0.86599835035847983</v>
+      </c>
+      <c r="K29" s="11"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="11"/>
+      <c r="N29" s="10"/>
+      <c r="O29" s="11"/>
+      <c r="P29" s="10"/>
+      <c r="Q29" s="11">
+        <v>462</v>
+      </c>
+      <c r="R29" s="10">
+        <f t="shared" si="3"/>
+        <v>2.9242357111209569E-2</v>
+      </c>
+      <c r="S29" s="11"/>
+      <c r="T29" s="10"/>
+      <c r="U29" s="11"/>
+      <c r="V29" s="10"/>
+      <c r="W29" s="11"/>
+      <c r="X29" s="10"/>
+      <c r="Y29" s="11"/>
+      <c r="Z29" s="10"/>
+      <c r="AA29" s="11"/>
+      <c r="AB29" s="10"/>
+      <c r="AC29" s="11"/>
+      <c r="AD29" s="10"/>
+      <c r="AE29" s="11"/>
+      <c r="AF29" s="10"/>
+      <c r="AG29" s="11"/>
+      <c r="AH29" s="10"/>
+      <c r="AI29" s="11"/>
+      <c r="AJ29" s="10"/>
+      <c r="AK29" s="11"/>
+      <c r="AL29" s="10"/>
+      <c r="AM29" s="11"/>
+      <c r="AN29" s="10"/>
+      <c r="AO29" s="11"/>
+      <c r="AP29" s="10"/>
+      <c r="AQ29" s="11"/>
+      <c r="AR29" s="10"/>
+      <c r="AS29" s="11"/>
+      <c r="AT29" s="46"/>
+      <c r="AU29" s="48"/>
+    </row>
+    <row r="30" spans="1:47" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" s="11">
+        <v>28092</v>
+      </c>
+      <c r="C30" s="11">
+        <v>16742</v>
+      </c>
+      <c r="D30" s="10">
+        <v>0.59599999999999997</v>
+      </c>
+      <c r="E30" s="11">
+        <v>58</v>
+      </c>
+      <c r="F30" s="9">
+        <f t="shared" si="0"/>
+        <v>16684</v>
+      </c>
+      <c r="G30" s="11">
+        <v>2264</v>
+      </c>
+      <c r="H30" s="10">
+        <f t="shared" si="1"/>
+        <v>0.13569887317190121</v>
+      </c>
+      <c r="I30" s="11">
+        <v>13649</v>
+      </c>
+      <c r="J30" s="10">
+        <f t="shared" si="2"/>
+        <v>0.81808918724526491</v>
+      </c>
+      <c r="K30" s="11"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="10"/>
+      <c r="O30" s="11"/>
+      <c r="P30" s="10"/>
+      <c r="Q30" s="11">
+        <v>771</v>
+      </c>
+      <c r="R30" s="10">
+        <f t="shared" si="3"/>
+        <v>4.6051845657627523E-2</v>
+      </c>
+      <c r="S30" s="11"/>
+      <c r="T30" s="10"/>
+      <c r="U30" s="11"/>
+      <c r="V30" s="10"/>
+      <c r="W30" s="11"/>
+      <c r="X30" s="10"/>
+      <c r="Y30" s="11"/>
+      <c r="Z30" s="10"/>
+      <c r="AA30" s="11"/>
+      <c r="AB30" s="10"/>
+      <c r="AC30" s="11"/>
+      <c r="AD30" s="10"/>
+      <c r="AE30" s="11"/>
+      <c r="AF30" s="10"/>
+      <c r="AG30" s="11"/>
+      <c r="AH30" s="10"/>
+      <c r="AI30" s="11"/>
+      <c r="AJ30" s="10"/>
+      <c r="AK30" s="11"/>
+      <c r="AL30" s="10"/>
+      <c r="AM30" s="11"/>
+      <c r="AN30" s="10"/>
+      <c r="AO30" s="11"/>
+      <c r="AP30" s="10"/>
+      <c r="AQ30" s="11"/>
+      <c r="AR30" s="10"/>
+      <c r="AS30" s="11"/>
+      <c r="AT30" s="46"/>
+      <c r="AU30" s="48"/>
+    </row>
+    <row r="31" spans="1:47" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" s="11">
+        <v>25429</v>
+      </c>
+      <c r="C31" s="11">
+        <v>14734</v>
+      </c>
+      <c r="D31" s="10">
+        <v>0.57940000000000003</v>
+      </c>
+      <c r="E31" s="11">
+        <v>52</v>
+      </c>
+      <c r="F31" s="9">
+        <f t="shared" si="0"/>
+        <v>14682</v>
+      </c>
+      <c r="G31" s="11">
+        <v>2349</v>
+      </c>
+      <c r="H31" s="10">
+        <f t="shared" si="1"/>
+        <v>0.159991826726604</v>
+      </c>
+      <c r="I31" s="11">
+        <v>11882</v>
+      </c>
+      <c r="J31" s="10">
+        <f t="shared" si="2"/>
+        <v>0.80929028742678111</v>
+      </c>
+      <c r="K31" s="11"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="11"/>
+      <c r="N31" s="10"/>
+      <c r="O31" s="11"/>
+      <c r="P31" s="10"/>
+      <c r="Q31" s="11">
+        <v>451</v>
+      </c>
+      <c r="R31" s="10">
+        <f t="shared" si="3"/>
+        <v>3.060947468440342E-2</v>
+      </c>
+      <c r="S31" s="11"/>
+      <c r="T31" s="10"/>
+      <c r="U31" s="11"/>
+      <c r="V31" s="10"/>
+      <c r="W31" s="11"/>
+      <c r="X31" s="10"/>
+      <c r="Y31" s="11"/>
+      <c r="Z31" s="10"/>
+      <c r="AA31" s="11"/>
+      <c r="AB31" s="10"/>
+      <c r="AC31" s="11"/>
+      <c r="AD31" s="10"/>
+      <c r="AE31" s="11"/>
+      <c r="AF31" s="10"/>
+      <c r="AG31" s="11"/>
+      <c r="AH31" s="10"/>
+      <c r="AI31" s="11"/>
+      <c r="AJ31" s="10"/>
+      <c r="AK31" s="11"/>
+      <c r="AL31" s="10"/>
+      <c r="AM31" s="11"/>
+      <c r="AN31" s="10"/>
+      <c r="AO31" s="11"/>
+      <c r="AP31" s="10"/>
+      <c r="AQ31" s="11"/>
+      <c r="AR31" s="10"/>
+      <c r="AS31" s="11"/>
+      <c r="AT31" s="46"/>
+      <c r="AU31" s="48"/>
+    </row>
+    <row r="32" spans="1:47" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32" s="11">
+        <v>26470</v>
+      </c>
+      <c r="C32" s="11">
+        <v>14151</v>
+      </c>
+      <c r="D32" s="10">
+        <v>0.53459999999999996</v>
+      </c>
+      <c r="E32" s="11">
+        <v>65</v>
+      </c>
+      <c r="F32" s="9">
+        <f t="shared" si="0"/>
+        <v>14086</v>
+      </c>
+      <c r="G32" s="11">
+        <v>6509</v>
+      </c>
+      <c r="H32" s="10">
+        <f t="shared" si="1"/>
+        <v>0.46209001845804343</v>
+      </c>
+      <c r="I32" s="11">
+        <v>7293</v>
+      </c>
+      <c r="J32" s="10">
+        <f t="shared" si="2"/>
+        <v>0.51774811869941784</v>
+      </c>
+      <c r="K32" s="11"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="11"/>
+      <c r="N32" s="10"/>
+      <c r="O32" s="11"/>
+      <c r="P32" s="10"/>
+      <c r="Q32" s="11"/>
+      <c r="R32" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S32" s="11"/>
+      <c r="T32" s="10"/>
+      <c r="U32" s="11"/>
+      <c r="V32" s="10"/>
+      <c r="W32" s="11">
+        <v>203</v>
+      </c>
+      <c r="X32" s="10">
+        <f t="shared" ref="X32:X34" si="6">SUM(W32/C32)</f>
+        <v>1.4345275952229524E-2</v>
+      </c>
+      <c r="Y32" s="11">
+        <v>81</v>
+      </c>
+      <c r="Z32" s="10">
+        <f t="shared" si="5"/>
+        <v>5.7239771040915833E-3</v>
+      </c>
+      <c r="AA32" s="11"/>
+      <c r="AB32" s="10"/>
+      <c r="AC32" s="11"/>
+      <c r="AD32" s="10"/>
+      <c r="AE32" s="11"/>
+      <c r="AF32" s="10"/>
+      <c r="AG32" s="11"/>
+      <c r="AH32" s="10"/>
+      <c r="AI32" s="11"/>
+      <c r="AJ32" s="10"/>
+      <c r="AK32" s="11"/>
+      <c r="AL32" s="10"/>
+      <c r="AM32" s="11"/>
+      <c r="AN32" s="10"/>
+      <c r="AO32" s="11"/>
+      <c r="AP32" s="10"/>
+      <c r="AQ32" s="11"/>
+      <c r="AR32" s="10"/>
+      <c r="AS32" s="11"/>
+      <c r="AT32" s="46"/>
+      <c r="AU32" s="48"/>
+    </row>
+    <row r="33" spans="1:47" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B33" s="11">
+        <v>26078</v>
+      </c>
+      <c r="C33" s="11">
+        <v>15467</v>
+      </c>
+      <c r="D33" s="10">
+        <v>0.59309999999999996</v>
+      </c>
+      <c r="E33" s="11">
+        <v>34</v>
+      </c>
+      <c r="F33" s="9">
+        <f>SUM(C33-E33)</f>
+        <v>15433</v>
+      </c>
+      <c r="G33" s="11">
+        <v>4934</v>
+      </c>
+      <c r="H33" s="10">
+        <f>SUM(G33/F33)</f>
+        <v>0.31970452925549148</v>
+      </c>
+      <c r="I33" s="11">
+        <v>9969</v>
+      </c>
+      <c r="J33" s="10">
+        <f>SUM(I33/F33)</f>
+        <v>0.64595347631698308</v>
+      </c>
+      <c r="K33" s="11"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="11"/>
+      <c r="N33" s="10"/>
+      <c r="O33" s="11"/>
+      <c r="P33" s="10"/>
+      <c r="Q33" s="11">
+        <v>530</v>
+      </c>
+      <c r="R33" s="10">
+        <f>SUM(Q33/C33)</f>
+        <v>3.4266502877093166E-2</v>
+      </c>
+      <c r="S33" s="11"/>
+      <c r="T33" s="10"/>
+      <c r="U33" s="11"/>
+      <c r="V33" s="10"/>
+      <c r="W33" s="11"/>
+      <c r="X33" s="10"/>
+      <c r="Y33" s="11"/>
+      <c r="Z33" s="10"/>
+      <c r="AA33" s="11"/>
+      <c r="AB33" s="10"/>
+      <c r="AC33" s="11"/>
+      <c r="AD33" s="10"/>
+      <c r="AE33" s="11"/>
+      <c r="AF33" s="10"/>
+      <c r="AG33" s="11"/>
+      <c r="AH33" s="10"/>
+      <c r="AI33" s="11"/>
+      <c r="AJ33" s="10"/>
+      <c r="AK33" s="11"/>
+      <c r="AL33" s="10"/>
+      <c r="AM33" s="11"/>
+      <c r="AN33" s="10"/>
+      <c r="AO33" s="11"/>
+      <c r="AP33" s="10"/>
+      <c r="AQ33" s="11"/>
+      <c r="AR33" s="10"/>
+      <c r="AS33" s="11"/>
+      <c r="AT33" s="46"/>
+      <c r="AU33" s="48"/>
+    </row>
+    <row r="34" spans="1:47" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B34" s="11">
+        <v>25670</v>
+      </c>
+      <c r="C34" s="11">
+        <v>10809</v>
+      </c>
+      <c r="D34" s="10">
+        <v>0.42109999999999997</v>
+      </c>
+      <c r="E34" s="11">
+        <v>48</v>
+      </c>
+      <c r="F34" s="9">
+        <f t="shared" si="0"/>
+        <v>10761</v>
+      </c>
+      <c r="G34" s="11">
+        <v>7243</v>
+      </c>
+      <c r="H34" s="10">
+        <f t="shared" si="1"/>
+        <v>0.67307871015704857</v>
+      </c>
+      <c r="I34" s="11">
+        <v>2597</v>
+      </c>
+      <c r="J34" s="10">
+        <f t="shared" si="2"/>
+        <v>0.24133444847133165</v>
+      </c>
+      <c r="K34" s="11"/>
+      <c r="L34" s="10"/>
+      <c r="M34" s="11"/>
+      <c r="N34" s="10"/>
+      <c r="O34" s="11"/>
+      <c r="P34" s="10"/>
+      <c r="Q34" s="11"/>
+      <c r="R34" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S34" s="11"/>
+      <c r="T34" s="10"/>
+      <c r="U34" s="11"/>
+      <c r="V34" s="10"/>
+      <c r="W34" s="11">
+        <v>443</v>
+      </c>
+      <c r="X34" s="10">
+        <f t="shared" si="6"/>
+        <v>4.0984364881117584E-2</v>
+      </c>
+      <c r="Y34" s="11"/>
+      <c r="Z34" s="10"/>
+      <c r="AA34" s="11"/>
+      <c r="AB34" s="10"/>
+      <c r="AC34" s="11"/>
+      <c r="AD34" s="10"/>
+      <c r="AE34" s="11"/>
+      <c r="AF34" s="10"/>
+      <c r="AG34" s="11"/>
+      <c r="AH34" s="10"/>
+      <c r="AI34" s="11"/>
+      <c r="AJ34" s="10"/>
+      <c r="AK34" s="11"/>
+      <c r="AL34" s="10"/>
+      <c r="AM34" s="11"/>
+      <c r="AN34" s="10"/>
+      <c r="AO34" s="11"/>
+      <c r="AP34" s="10"/>
+      <c r="AQ34" s="11">
+        <v>478</v>
+      </c>
+      <c r="AR34" s="10">
+        <f>SUM(AQ34/C34)</f>
+        <v>4.4222407253214913E-2</v>
+      </c>
+      <c r="AS34" s="11"/>
+      <c r="AT34" s="46"/>
+      <c r="AU34" s="48"/>
+    </row>
+    <row r="35" spans="1:47" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B35" s="11">
+        <v>25534</v>
+      </c>
+      <c r="C35" s="11">
+        <v>9215</v>
+      </c>
+      <c r="D35" s="10">
+        <v>0.3609</v>
+      </c>
+      <c r="E35" s="11">
+        <v>35</v>
+      </c>
+      <c r="F35" s="9">
+        <f t="shared" si="0"/>
+        <v>9180</v>
+      </c>
+      <c r="G35" s="11">
+        <v>5523</v>
+      </c>
+      <c r="H35" s="10">
+        <f t="shared" si="1"/>
+        <v>0.60163398692810455</v>
+      </c>
+      <c r="I35" s="11">
+        <v>2218</v>
+      </c>
+      <c r="J35" s="10">
+        <f t="shared" si="2"/>
+        <v>0.24161220043572984</v>
+      </c>
+      <c r="K35" s="11"/>
+      <c r="L35" s="10"/>
+      <c r="M35" s="11"/>
+      <c r="N35" s="10"/>
+      <c r="O35" s="11"/>
+      <c r="P35" s="10"/>
+      <c r="Q35" s="11">
+        <v>670</v>
+      </c>
+      <c r="R35" s="10">
+        <f t="shared" si="3"/>
+        <v>7.2707542051003798E-2</v>
+      </c>
+      <c r="S35" s="11"/>
+      <c r="T35" s="10"/>
+      <c r="U35" s="11"/>
+      <c r="V35" s="10"/>
+      <c r="W35" s="11">
+        <v>352</v>
+      </c>
+      <c r="X35" s="10">
+        <f>SUM(W35/C35)</f>
+        <v>3.8198589256646771E-2</v>
+      </c>
+      <c r="Y35" s="11">
+        <v>149</v>
+      </c>
+      <c r="Z35" s="10">
+        <f t="shared" si="5"/>
+        <v>1.6169289202387412E-2</v>
+      </c>
+      <c r="AA35" s="11"/>
+      <c r="AB35" s="10"/>
+      <c r="AC35" s="11"/>
+      <c r="AD35" s="10"/>
+      <c r="AE35" s="11"/>
+      <c r="AF35" s="10"/>
+      <c r="AG35" s="11"/>
+      <c r="AH35" s="10"/>
+      <c r="AI35" s="11">
+        <v>268</v>
+      </c>
+      <c r="AJ35" s="10">
+        <f>SUM(AI35/C35)</f>
+        <v>2.9083016820401521E-2</v>
+      </c>
+      <c r="AK35" s="11"/>
+      <c r="AL35" s="10"/>
+      <c r="AM35" s="11"/>
+      <c r="AN35" s="10"/>
+      <c r="AO35" s="11"/>
+      <c r="AP35" s="10"/>
+      <c r="AQ35" s="11"/>
+      <c r="AR35" s="10"/>
+      <c r="AS35" s="11"/>
+      <c r="AT35" s="46"/>
+      <c r="AU35" s="48"/>
+    </row>
+    <row r="36" spans="1:47" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B36" s="11">
+        <v>27774</v>
+      </c>
+      <c r="C36" s="11">
+        <v>15751</v>
+      </c>
+      <c r="D36" s="10">
+        <v>0.56710000000000005</v>
+      </c>
+      <c r="E36" s="11">
+        <v>49</v>
+      </c>
+      <c r="F36" s="9">
+        <f t="shared" si="0"/>
+        <v>15702</v>
+      </c>
+      <c r="G36" s="11">
+        <v>3340</v>
+      </c>
+      <c r="H36" s="10">
+        <f t="shared" si="1"/>
+        <v>0.2127117564641447</v>
+      </c>
+      <c r="I36" s="11">
+        <v>11852</v>
+      </c>
+      <c r="J36" s="10">
+        <f t="shared" si="2"/>
+        <v>0.75480830467456372</v>
+      </c>
+      <c r="K36" s="11"/>
+      <c r="L36" s="10"/>
+      <c r="M36" s="11"/>
+      <c r="N36" s="10"/>
+      <c r="O36" s="11"/>
+      <c r="P36" s="10"/>
+      <c r="Q36" s="11">
+        <v>510</v>
+      </c>
+      <c r="R36" s="10">
+        <f t="shared" si="3"/>
+        <v>3.2378896577995045E-2</v>
+      </c>
+      <c r="S36" s="11"/>
+      <c r="T36" s="10"/>
+      <c r="U36" s="11"/>
+      <c r="V36" s="10"/>
+      <c r="W36" s="11"/>
+      <c r="X36" s="10"/>
+      <c r="Y36" s="11"/>
+      <c r="Z36" s="10"/>
+      <c r="AA36" s="11"/>
+      <c r="AB36" s="10"/>
+      <c r="AC36" s="11"/>
+      <c r="AD36" s="10"/>
+      <c r="AE36" s="11"/>
+      <c r="AF36" s="10"/>
+      <c r="AG36" s="11"/>
+      <c r="AH36" s="10"/>
+      <c r="AI36" s="11"/>
+      <c r="AJ36" s="10"/>
+      <c r="AK36" s="11"/>
+      <c r="AL36" s="10"/>
+      <c r="AM36" s="11"/>
+      <c r="AN36" s="10"/>
+      <c r="AO36" s="11"/>
+      <c r="AP36" s="10"/>
+      <c r="AQ36" s="11"/>
+      <c r="AR36" s="10"/>
+      <c r="AS36" s="11"/>
+      <c r="AT36" s="46"/>
+      <c r="AU36" s="48"/>
+    </row>
+    <row r="37" spans="1:47" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="B37" s="11">
+        <v>25667</v>
+      </c>
+      <c r="C37" s="11">
+        <v>13909</v>
+      </c>
+      <c r="D37" s="10">
+        <v>0.54190000000000005</v>
+      </c>
+      <c r="E37" s="11">
+        <v>36</v>
+      </c>
+      <c r="F37" s="9">
+        <f t="shared" si="0"/>
+        <v>13873</v>
+      </c>
+      <c r="G37" s="11">
+        <v>7026</v>
+      </c>
+      <c r="H37" s="10">
+        <f t="shared" si="1"/>
+        <v>0.50645138037915371</v>
+      </c>
+      <c r="I37" s="11">
+        <v>6357</v>
+      </c>
+      <c r="J37" s="10">
+        <f t="shared" si="2"/>
+        <v>0.45822821307575867</v>
+      </c>
+      <c r="K37" s="11"/>
+      <c r="L37" s="10"/>
+      <c r="M37" s="11"/>
+      <c r="N37" s="10"/>
+      <c r="O37" s="11"/>
+      <c r="P37" s="10"/>
+      <c r="Q37" s="11">
+        <v>490</v>
+      </c>
+      <c r="R37" s="10">
+        <f t="shared" si="3"/>
+        <v>3.5228988424760944E-2</v>
+      </c>
+      <c r="S37" s="11"/>
+      <c r="T37" s="10"/>
+      <c r="U37" s="11"/>
+      <c r="V37" s="10"/>
+      <c r="W37" s="11"/>
+      <c r="X37" s="10"/>
+      <c r="Y37" s="11"/>
+      <c r="Z37" s="10"/>
+      <c r="AA37" s="11"/>
+      <c r="AB37" s="10"/>
+      <c r="AC37" s="11"/>
+      <c r="AD37" s="10"/>
+      <c r="AE37" s="11"/>
+      <c r="AF37" s="10"/>
+      <c r="AG37" s="11"/>
+      <c r="AH37" s="10"/>
+      <c r="AI37" s="11"/>
+      <c r="AJ37" s="10"/>
+      <c r="AK37" s="11"/>
+      <c r="AL37" s="10"/>
+      <c r="AM37" s="11"/>
+      <c r="AN37" s="10"/>
+      <c r="AO37" s="11"/>
+      <c r="AP37" s="10"/>
+      <c r="AQ37" s="11"/>
+      <c r="AR37" s="10"/>
+      <c r="AS37" s="11"/>
+      <c r="AT37" s="46"/>
+      <c r="AU37" s="48"/>
+    </row>
+    <row r="38" spans="1:47" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B38" s="11">
+        <v>25378</v>
+      </c>
+      <c r="C38" s="11">
+        <v>14583</v>
+      </c>
+      <c r="D38" s="10">
+        <v>0.5746</v>
+      </c>
+      <c r="E38" s="11">
+        <v>65</v>
+      </c>
+      <c r="F38" s="9">
+        <f t="shared" si="0"/>
+        <v>14518</v>
+      </c>
+      <c r="G38" s="11">
+        <v>6638</v>
+      </c>
+      <c r="H38" s="10">
+        <f t="shared" si="1"/>
+        <v>0.45722551315608212</v>
+      </c>
+      <c r="I38" s="11">
+        <v>7341</v>
+      </c>
+      <c r="J38" s="10">
+        <f t="shared" si="2"/>
+        <v>0.50564816090370579</v>
+      </c>
+      <c r="K38" s="11"/>
+      <c r="L38" s="10"/>
+      <c r="M38" s="11"/>
+      <c r="N38" s="10"/>
+      <c r="O38" s="11"/>
+      <c r="P38" s="10"/>
+      <c r="Q38" s="11">
+        <v>450</v>
+      </c>
+      <c r="R38" s="10">
+        <f t="shared" si="3"/>
+        <v>3.0857848179386957E-2</v>
+      </c>
+      <c r="S38" s="11"/>
+      <c r="T38" s="10"/>
+      <c r="U38" s="11"/>
+      <c r="V38" s="10"/>
+      <c r="W38" s="11">
+        <v>44</v>
+      </c>
+      <c r="X38" s="10">
+        <f t="shared" ref="X38:X47" si="7">SUM(W38/C38)</f>
+        <v>3.0172118219845027E-3</v>
+      </c>
+      <c r="Y38" s="11">
+        <v>28</v>
+      </c>
+      <c r="Z38" s="10">
+        <f>SUM(Y38/C38)</f>
+        <v>1.9200438867174106E-3</v>
+      </c>
+      <c r="AA38" s="11"/>
+      <c r="AB38" s="10"/>
+      <c r="AC38" s="11"/>
+      <c r="AD38" s="10"/>
+      <c r="AE38" s="11"/>
+      <c r="AF38" s="10"/>
+      <c r="AG38" s="11">
+        <v>17</v>
+      </c>
+      <c r="AH38" s="10">
+        <f>SUM(AG38/C38)</f>
+        <v>1.1657409312212852E-3</v>
+      </c>
+      <c r="AI38" s="11"/>
+      <c r="AJ38" s="10"/>
+      <c r="AK38" s="11"/>
+      <c r="AL38" s="10"/>
+      <c r="AM38" s="11"/>
+      <c r="AN38" s="10"/>
+      <c r="AO38" s="11"/>
+      <c r="AP38" s="10"/>
+      <c r="AQ38" s="11"/>
+      <c r="AR38" s="10"/>
+      <c r="AS38" s="11"/>
+      <c r="AT38" s="46"/>
+      <c r="AU38" s="48"/>
+    </row>
+    <row r="39" spans="1:47" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B39" s="11">
+        <v>29096</v>
+      </c>
+      <c r="C39" s="11">
+        <v>16740</v>
+      </c>
+      <c r="D39" s="10">
+        <v>0.57530000000000003</v>
+      </c>
+      <c r="E39" s="11">
+        <v>54</v>
+      </c>
+      <c r="F39" s="9">
+        <f t="shared" si="0"/>
+        <v>16686</v>
+      </c>
+      <c r="G39" s="11">
+        <v>2412</v>
+      </c>
+      <c r="H39" s="10">
+        <f t="shared" si="1"/>
+        <v>0.14455231930960086</v>
+      </c>
+      <c r="I39" s="11">
+        <v>13900</v>
+      </c>
+      <c r="J39" s="10">
+        <f t="shared" si="2"/>
+        <v>0.83303368093012109</v>
+      </c>
+      <c r="K39" s="11"/>
+      <c r="L39" s="10"/>
+      <c r="M39" s="11"/>
+      <c r="N39" s="10"/>
+      <c r="O39" s="11"/>
+      <c r="P39" s="10"/>
+      <c r="Q39" s="11">
+        <v>374</v>
+      </c>
+      <c r="R39" s="10">
+        <f t="shared" si="3"/>
+        <v>2.2341696535244922E-2</v>
+      </c>
+      <c r="S39" s="11"/>
+      <c r="T39" s="10"/>
+      <c r="U39" s="11"/>
+      <c r="V39" s="10"/>
+      <c r="W39" s="11"/>
+      <c r="X39" s="10"/>
+      <c r="Y39" s="11"/>
+      <c r="Z39" s="10"/>
+      <c r="AA39" s="11"/>
+      <c r="AB39" s="10"/>
+      <c r="AC39" s="11"/>
+      <c r="AD39" s="10"/>
+      <c r="AE39" s="11"/>
+      <c r="AF39" s="10"/>
+      <c r="AG39" s="11"/>
+      <c r="AH39" s="10"/>
+      <c r="AI39" s="11"/>
+      <c r="AJ39" s="10"/>
+      <c r="AK39" s="11"/>
+      <c r="AL39" s="10"/>
+      <c r="AM39" s="11"/>
+      <c r="AN39" s="10"/>
+      <c r="AO39" s="11"/>
+      <c r="AP39" s="10"/>
+      <c r="AQ39" s="11"/>
+      <c r="AR39" s="10"/>
+      <c r="AS39" s="11"/>
+      <c r="AT39" s="46"/>
+      <c r="AU39" s="48"/>
+    </row>
+    <row r="40" spans="1:47" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B40" s="11">
+        <v>30113</v>
+      </c>
+      <c r="C40" s="11">
+        <v>13502</v>
+      </c>
+      <c r="D40" s="10">
+        <v>0.44840000000000002</v>
+      </c>
+      <c r="E40" s="11">
+        <v>53</v>
+      </c>
+      <c r="F40" s="9">
+        <f t="shared" si="0"/>
+        <v>13449</v>
+      </c>
+      <c r="G40" s="11">
+        <v>7472</v>
+      </c>
+      <c r="H40" s="10">
+        <f t="shared" si="1"/>
+        <v>0.55558034054576544</v>
+      </c>
+      <c r="I40" s="11">
+        <v>4263</v>
+      </c>
+      <c r="J40" s="10">
+        <f t="shared" si="2"/>
+        <v>0.31697523979478026</v>
+      </c>
+      <c r="K40" s="11"/>
+      <c r="L40" s="10"/>
+      <c r="M40" s="11"/>
+      <c r="N40" s="10"/>
+      <c r="O40" s="11"/>
+      <c r="P40" s="10"/>
+      <c r="Q40" s="11">
+        <v>1242</v>
+      </c>
+      <c r="R40" s="10">
+        <f t="shared" si="3"/>
+        <v>9.1986372389275664E-2</v>
+      </c>
+      <c r="S40" s="11"/>
+      <c r="T40" s="10"/>
+      <c r="U40" s="11"/>
+      <c r="V40" s="10"/>
+      <c r="W40" s="11">
+        <v>472</v>
+      </c>
+      <c r="X40" s="10">
+        <f t="shared" si="7"/>
+        <v>3.4957784031995259E-2</v>
+      </c>
+      <c r="Y40" s="11"/>
+      <c r="Z40" s="10"/>
+      <c r="AA40" s="11"/>
+      <c r="AB40" s="10"/>
+      <c r="AC40" s="11"/>
+      <c r="AD40" s="10"/>
+      <c r="AE40" s="11"/>
+      <c r="AF40" s="10"/>
+      <c r="AG40" s="11"/>
+      <c r="AH40" s="10"/>
+      <c r="AI40" s="11"/>
+      <c r="AJ40" s="10"/>
+      <c r="AK40" s="11"/>
+      <c r="AL40" s="10"/>
+      <c r="AM40" s="11"/>
+      <c r="AN40" s="10"/>
+      <c r="AO40" s="11"/>
+      <c r="AP40" s="10"/>
+      <c r="AQ40" s="11"/>
+      <c r="AR40" s="10"/>
+      <c r="AS40" s="11"/>
+      <c r="AT40" s="46"/>
+      <c r="AU40" s="48"/>
+    </row>
+    <row r="41" spans="1:47" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B41" s="11">
+        <v>28397</v>
+      </c>
+      <c r="C41" s="11">
+        <v>17209</v>
+      </c>
+      <c r="D41" s="10">
+        <v>0.60599999999999998</v>
+      </c>
+      <c r="E41" s="11">
+        <v>41</v>
+      </c>
+      <c r="F41" s="9">
+        <f t="shared" si="0"/>
+        <v>17168</v>
+      </c>
+      <c r="G41" s="11">
+        <v>3865</v>
+      </c>
+      <c r="H41" s="10">
+        <f t="shared" si="1"/>
+        <v>0.22512814538676607</v>
+      </c>
+      <c r="I41" s="11">
+        <v>12664</v>
+      </c>
+      <c r="J41" s="10">
+        <f t="shared" si="2"/>
+        <v>0.73765144454799625</v>
+      </c>
+      <c r="K41" s="11"/>
+      <c r="L41" s="10"/>
+      <c r="M41" s="11"/>
+      <c r="N41" s="10"/>
+      <c r="O41" s="11"/>
+      <c r="P41" s="10"/>
+      <c r="Q41" s="11">
+        <v>481</v>
+      </c>
+      <c r="R41" s="10">
+        <f t="shared" si="3"/>
+        <v>2.7950491022139579E-2</v>
+      </c>
+      <c r="S41" s="11"/>
+      <c r="T41" s="10"/>
+      <c r="U41" s="11"/>
+      <c r="V41" s="10"/>
+      <c r="W41" s="11">
+        <v>129</v>
+      </c>
+      <c r="X41" s="10">
+        <f t="shared" si="7"/>
+        <v>7.4960776337962692E-3</v>
+      </c>
+      <c r="Y41" s="11"/>
+      <c r="Z41" s="10"/>
+      <c r="AA41" s="11"/>
+      <c r="AB41" s="10"/>
+      <c r="AC41" s="11"/>
+      <c r="AD41" s="10"/>
+      <c r="AE41" s="11"/>
+      <c r="AF41" s="10"/>
+      <c r="AG41" s="11"/>
+      <c r="AH41" s="10"/>
+      <c r="AI41" s="11"/>
+      <c r="AJ41" s="10"/>
+      <c r="AK41" s="11">
+        <v>29</v>
+      </c>
+      <c r="AL41" s="10">
+        <f>SUM(AK41/C41)</f>
+        <v>1.6851647393805566E-3</v>
+      </c>
+      <c r="AM41" s="11"/>
+      <c r="AN41" s="10"/>
+      <c r="AO41" s="11"/>
+      <c r="AP41" s="10"/>
+      <c r="AQ41" s="11"/>
+      <c r="AR41" s="10"/>
+      <c r="AS41" s="11"/>
+      <c r="AT41" s="46"/>
+      <c r="AU41" s="48"/>
+    </row>
+    <row r="42" spans="1:47" ht="19" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B42" s="11">
+        <v>28873</v>
+      </c>
+      <c r="C42" s="11">
+        <v>17339</v>
+      </c>
+      <c r="D42" s="10">
+        <v>0.60050000000000003</v>
+      </c>
+      <c r="E42" s="11">
+        <v>48</v>
+      </c>
+      <c r="F42" s="9">
+        <f>SUM(C42-E42)</f>
+        <v>17291</v>
+      </c>
+      <c r="G42" s="11">
+        <v>6672</v>
+      </c>
+      <c r="H42" s="10">
+        <f>SUM(G42/F42)</f>
+        <v>0.38586547915100339</v>
+      </c>
+      <c r="I42" s="11">
+        <v>9908</v>
+      </c>
+      <c r="J42" s="10">
+        <f>SUM(I42/F42)</f>
+        <v>0.57301486322364237</v>
+      </c>
+      <c r="K42" s="11"/>
+      <c r="L42" s="10"/>
+      <c r="M42" s="11"/>
+      <c r="N42" s="10"/>
+      <c r="O42" s="11"/>
+      <c r="P42" s="10"/>
+      <c r="Q42" s="11">
+        <v>350</v>
+      </c>
+      <c r="R42" s="10">
+        <f>SUM(Q42/C42)</f>
+        <v>2.0185708518368994E-2</v>
+      </c>
+      <c r="S42" s="11"/>
+      <c r="T42" s="10"/>
+      <c r="U42" s="11"/>
+      <c r="V42" s="10"/>
+      <c r="W42" s="11">
+        <v>334</v>
+      </c>
+      <c r="X42" s="10">
+        <f>SUM(W42/C42)</f>
+        <v>1.9262933271814983E-2</v>
+      </c>
+      <c r="Y42" s="11"/>
+      <c r="Z42" s="10"/>
+      <c r="AA42" s="11"/>
+      <c r="AB42" s="10"/>
+      <c r="AC42" s="11"/>
+      <c r="AD42" s="10"/>
+      <c r="AE42" s="11"/>
+      <c r="AF42" s="10"/>
+      <c r="AG42" s="11"/>
+      <c r="AH42" s="10"/>
+      <c r="AI42" s="11"/>
+      <c r="AJ42" s="10"/>
+      <c r="AK42" s="11">
+        <v>27</v>
+      </c>
+      <c r="AL42" s="10"/>
+      <c r="AM42" s="11"/>
+      <c r="AN42" s="10"/>
+      <c r="AO42" s="11"/>
+      <c r="AP42" s="10"/>
+      <c r="AQ42" s="11"/>
+      <c r="AR42" s="10"/>
+      <c r="AS42" s="11"/>
+      <c r="AT42" s="46"/>
+      <c r="AU42" s="48"/>
+    </row>
+    <row r="43" spans="1:47" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B43" s="11">
+        <v>28876</v>
+      </c>
+      <c r="C43" s="11">
+        <v>15765</v>
+      </c>
+      <c r="D43" s="10">
+        <v>0.54600000000000004</v>
+      </c>
+      <c r="E43" s="11">
+        <v>46</v>
+      </c>
+      <c r="F43" s="9">
+        <f t="shared" si="0"/>
+        <v>15719</v>
+      </c>
+      <c r="G43" s="11">
+        <v>3436</v>
+      </c>
+      <c r="H43" s="10">
+        <f t="shared" si="1"/>
+        <v>0.21858896876391629</v>
+      </c>
+      <c r="I43" s="11">
+        <v>11615</v>
+      </c>
+      <c r="J43" s="10">
+        <f t="shared" si="2"/>
+        <v>0.7389146892295948</v>
+      </c>
+      <c r="K43" s="11"/>
+      <c r="L43" s="10"/>
+      <c r="M43" s="11"/>
+      <c r="N43" s="10"/>
+      <c r="O43" s="11"/>
+      <c r="P43" s="10"/>
+      <c r="Q43" s="11">
+        <v>668</v>
+      </c>
+      <c r="R43" s="10">
+        <f t="shared" si="3"/>
+        <v>4.2372343799555977E-2</v>
+      </c>
+      <c r="S43" s="11"/>
+      <c r="T43" s="10"/>
+      <c r="U43" s="11"/>
+      <c r="V43" s="10"/>
+      <c r="W43" s="11"/>
+      <c r="X43" s="10"/>
+      <c r="Y43" s="11"/>
+      <c r="Z43" s="10"/>
+      <c r="AA43" s="11"/>
+      <c r="AB43" s="10"/>
+      <c r="AC43" s="11"/>
+      <c r="AD43" s="10"/>
+      <c r="AE43" s="11"/>
+      <c r="AF43" s="10"/>
+      <c r="AG43" s="11"/>
+      <c r="AH43" s="10"/>
+      <c r="AI43" s="11"/>
+      <c r="AJ43" s="10"/>
+      <c r="AK43" s="11"/>
+      <c r="AL43" s="10"/>
+      <c r="AM43" s="11"/>
+      <c r="AN43" s="10"/>
+      <c r="AO43" s="11"/>
+      <c r="AP43" s="10"/>
+      <c r="AQ43" s="11"/>
+      <c r="AR43" s="10"/>
+      <c r="AS43" s="11"/>
+      <c r="AT43" s="46"/>
+      <c r="AU43" s="48"/>
+    </row>
+    <row r="44" spans="1:47" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B44" s="11">
+        <v>23853</v>
+      </c>
+      <c r="C44" s="11">
+        <v>12542</v>
+      </c>
+      <c r="D44" s="10">
+        <v>0.52580000000000005</v>
+      </c>
+      <c r="E44" s="11">
+        <v>33</v>
+      </c>
+      <c r="F44" s="9">
+        <f t="shared" si="0"/>
+        <v>12509</v>
+      </c>
+      <c r="G44" s="11">
+        <v>4396</v>
+      </c>
+      <c r="H44" s="10">
+        <f t="shared" si="1"/>
+        <v>0.35142697257974259</v>
+      </c>
+      <c r="I44" s="11">
+        <v>7144</v>
+      </c>
+      <c r="J44" s="10">
+        <f t="shared" si="2"/>
+        <v>0.57110880166280276</v>
+      </c>
+      <c r="K44" s="11"/>
+      <c r="L44" s="10"/>
+      <c r="M44" s="11"/>
+      <c r="N44" s="10"/>
+      <c r="O44" s="11"/>
+      <c r="P44" s="10"/>
+      <c r="Q44" s="11">
+        <v>99</v>
+      </c>
+      <c r="R44" s="10">
+        <f t="shared" si="3"/>
+        <v>7.8934779142082606E-3</v>
+      </c>
+      <c r="S44" s="11"/>
+      <c r="T44" s="10"/>
+      <c r="U44" s="11">
+        <v>788</v>
+      </c>
+      <c r="V44" s="10">
+        <f>SUM(U44/C44)</f>
+        <v>6.2828894913092015E-2</v>
+      </c>
+      <c r="W44" s="11"/>
+      <c r="X44" s="10"/>
+      <c r="Y44" s="11"/>
+      <c r="Z44" s="10"/>
+      <c r="AA44" s="11"/>
+      <c r="AB44" s="10"/>
+      <c r="AC44" s="11"/>
+      <c r="AD44" s="10"/>
+      <c r="AE44" s="11">
+        <v>82</v>
+      </c>
+      <c r="AF44" s="10">
+        <f>SUM(AE44/C44)</f>
+        <v>6.5380322117684578E-3</v>
+      </c>
+      <c r="AG44" s="11"/>
+      <c r="AH44" s="10"/>
+      <c r="AI44" s="11"/>
+      <c r="AJ44" s="10"/>
+      <c r="AK44" s="11"/>
+      <c r="AL44" s="10"/>
+      <c r="AM44" s="11"/>
+      <c r="AN44" s="10"/>
+      <c r="AO44" s="11"/>
+      <c r="AP44" s="10"/>
+      <c r="AQ44" s="11"/>
+      <c r="AR44" s="10"/>
+      <c r="AS44" s="11"/>
+      <c r="AT44" s="46"/>
+      <c r="AU44" s="48"/>
+    </row>
+    <row r="45" spans="1:47" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B45" s="11">
+        <v>28863</v>
+      </c>
+      <c r="C45" s="11">
+        <v>14379</v>
+      </c>
+      <c r="D45" s="10">
+        <v>0.49819999999999998</v>
+      </c>
+      <c r="E45" s="11">
+        <v>55</v>
+      </c>
+      <c r="F45" s="9">
+        <f t="shared" si="0"/>
+        <v>14324</v>
+      </c>
+      <c r="G45" s="11">
+        <v>6604</v>
+      </c>
+      <c r="H45" s="10">
+        <f t="shared" si="1"/>
+        <v>0.4610444010053058</v>
+      </c>
+      <c r="I45" s="11">
+        <v>6713</v>
+      </c>
+      <c r="J45" s="10">
+        <f t="shared" si="2"/>
+        <v>0.46865400726054174</v>
+      </c>
+      <c r="K45" s="11"/>
+      <c r="L45" s="10"/>
+      <c r="M45" s="11"/>
+      <c r="N45" s="10"/>
+      <c r="O45" s="11"/>
+      <c r="P45" s="10"/>
+      <c r="Q45" s="11">
+        <v>154</v>
+      </c>
+      <c r="R45" s="10">
+        <f t="shared" si="3"/>
+        <v>1.0710063286737603E-2</v>
+      </c>
+      <c r="S45" s="11"/>
+      <c r="T45" s="10"/>
+      <c r="U45" s="11">
+        <v>608</v>
+      </c>
+      <c r="V45" s="10">
+        <f>SUM(U45/C45)</f>
+        <v>4.2283886222964043E-2</v>
+      </c>
+      <c r="W45" s="11"/>
+      <c r="X45" s="10"/>
+      <c r="Y45" s="11">
+        <v>87</v>
+      </c>
+      <c r="Z45" s="10">
+        <f t="shared" ref="Z45" si="8">SUM(Y45/C45)</f>
+        <v>6.0504902983517629E-3</v>
+      </c>
+      <c r="AA45" s="11">
+        <v>22</v>
+      </c>
+      <c r="AB45" s="10">
+        <f>SUM(AA45/C45)</f>
+        <v>1.5300090409625148E-3</v>
+      </c>
+      <c r="AC45" s="11"/>
+      <c r="AD45" s="10"/>
+      <c r="AE45" s="11">
+        <v>61</v>
+      </c>
+      <c r="AF45" s="10">
+        <f>SUM(AE45/C45)</f>
+        <v>4.242297795396064E-3</v>
+      </c>
+      <c r="AG45" s="11"/>
+      <c r="AH45" s="10"/>
+      <c r="AI45" s="11"/>
+      <c r="AJ45" s="10"/>
+      <c r="AK45" s="11"/>
+      <c r="AL45" s="10"/>
+      <c r="AM45" s="11">
+        <v>37</v>
+      </c>
+      <c r="AN45" s="10">
+        <f>SUM(AM45/C45)</f>
+        <v>2.5731970234369565E-3</v>
+      </c>
+      <c r="AO45" s="11">
+        <v>38</v>
+      </c>
+      <c r="AP45" s="10">
+        <f>SUM(AO45/C45)</f>
+        <v>2.6427428889352527E-3</v>
+      </c>
+      <c r="AQ45" s="11"/>
+      <c r="AR45" s="10"/>
+      <c r="AS45" s="11"/>
+      <c r="AT45" s="46"/>
+      <c r="AU45" s="48"/>
+    </row>
+    <row r="46" spans="1:47" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B46" s="11">
+        <v>31186</v>
+      </c>
+      <c r="C46" s="11">
+        <v>17691</v>
+      </c>
+      <c r="D46" s="10">
+        <v>0.56730000000000003</v>
+      </c>
+      <c r="E46" s="11">
+        <v>72</v>
+      </c>
+      <c r="F46" s="9">
+        <f t="shared" si="0"/>
+        <v>17619</v>
+      </c>
+      <c r="G46" s="11">
+        <v>7363</v>
+      </c>
+      <c r="H46" s="10">
+        <f t="shared" si="1"/>
+        <v>0.41790112946251207</v>
+      </c>
+      <c r="I46" s="11">
+        <v>9728</v>
+      </c>
+      <c r="J46" s="10">
+        <f t="shared" si="2"/>
+        <v>0.55213122197627562</v>
+      </c>
+      <c r="K46" s="11"/>
+      <c r="L46" s="10"/>
+      <c r="M46" s="11"/>
+      <c r="N46" s="10"/>
+      <c r="O46" s="11"/>
+      <c r="P46" s="10"/>
+      <c r="Q46" s="11">
+        <v>385</v>
+      </c>
+      <c r="R46" s="10">
+        <f t="shared" si="3"/>
+        <v>2.176247809620711E-2</v>
+      </c>
+      <c r="S46" s="11"/>
+      <c r="T46" s="10"/>
+      <c r="U46" s="11"/>
+      <c r="V46" s="10"/>
+      <c r="W46" s="11">
+        <v>143</v>
+      </c>
+      <c r="X46" s="10">
+        <f t="shared" si="7"/>
+        <v>8.0832061500197838E-3</v>
+      </c>
+      <c r="Y46" s="11"/>
+      <c r="Z46" s="10"/>
+      <c r="AA46" s="11"/>
+      <c r="AB46" s="10"/>
+      <c r="AC46" s="11"/>
+      <c r="AD46" s="10"/>
+      <c r="AE46" s="11"/>
+      <c r="AF46" s="10"/>
+      <c r="AG46" s="11"/>
+      <c r="AH46" s="10"/>
+      <c r="AI46" s="11"/>
+      <c r="AJ46" s="10"/>
+      <c r="AK46" s="11"/>
+      <c r="AL46" s="10"/>
+      <c r="AM46" s="11"/>
+      <c r="AN46" s="10"/>
+      <c r="AO46" s="11"/>
+      <c r="AP46" s="10"/>
+      <c r="AQ46" s="11"/>
+      <c r="AR46" s="10"/>
+      <c r="AS46" s="11"/>
+      <c r="AT46" s="46"/>
+      <c r="AU46" s="48"/>
+    </row>
+    <row r="47" spans="1:47" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B47" s="11">
+        <v>27485</v>
+      </c>
+      <c r="C47" s="11">
+        <v>16016</v>
+      </c>
+      <c r="D47" s="10">
+        <v>0.5827</v>
+      </c>
+      <c r="E47" s="11">
+        <v>39</v>
+      </c>
+      <c r="F47" s="9">
+        <f t="shared" si="0"/>
+        <v>15977</v>
+      </c>
+      <c r="G47" s="11">
+        <v>6943</v>
+      </c>
+      <c r="H47" s="10">
+        <f t="shared" si="1"/>
+        <v>0.43456218313826123</v>
+      </c>
+      <c r="I47" s="11">
+        <v>8466</v>
+      </c>
+      <c r="J47" s="10">
+        <f t="shared" si="2"/>
+        <v>0.52988671214871375</v>
+      </c>
+      <c r="K47" s="11"/>
+      <c r="L47" s="10"/>
+      <c r="M47" s="11"/>
+      <c r="N47" s="10"/>
+      <c r="O47" s="11"/>
+      <c r="P47" s="10"/>
+      <c r="Q47" s="11">
+        <v>413</v>
+      </c>
+      <c r="R47" s="10">
+        <f t="shared" si="3"/>
+        <v>2.5786713286713288E-2</v>
+      </c>
+      <c r="S47" s="11"/>
+      <c r="T47" s="10"/>
+      <c r="U47" s="11"/>
+      <c r="V47" s="10"/>
+      <c r="W47" s="11">
+        <v>127</v>
+      </c>
+      <c r="X47" s="10">
+        <f t="shared" si="7"/>
+        <v>7.9295704295704299E-3</v>
+      </c>
+      <c r="Y47" s="11"/>
+      <c r="Z47" s="10"/>
+      <c r="AA47" s="11"/>
+      <c r="AB47" s="10"/>
+      <c r="AC47" s="11"/>
+      <c r="AD47" s="10"/>
+      <c r="AE47" s="11"/>
+      <c r="AF47" s="10"/>
+      <c r="AG47" s="11"/>
+      <c r="AH47" s="10"/>
+      <c r="AI47" s="11"/>
+      <c r="AJ47" s="10"/>
+      <c r="AK47" s="11">
+        <v>28</v>
+      </c>
+      <c r="AL47" s="10"/>
+      <c r="AM47" s="11"/>
+      <c r="AN47" s="10"/>
+      <c r="AO47" s="11"/>
+      <c r="AP47" s="10"/>
+      <c r="AQ47" s="11"/>
+      <c r="AR47" s="10"/>
+      <c r="AS47" s="11"/>
+      <c r="AT47" s="46"/>
+      <c r="AU47" s="48"/>
+    </row>
+    <row r="48" spans="1:47" s="44" customFormat="1" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B48" s="34">
+        <f>SUM(B7:B47)</f>
+        <v>1153876</v>
+      </c>
+      <c r="C48" s="31">
+        <f>SUM(C7:C47)</f>
+        <v>622181</v>
+      </c>
+      <c r="D48" s="15">
+        <f>SUM(C48/B48)</f>
+        <v>0.53920958577871447</v>
+      </c>
+      <c r="E48" s="16">
+        <f>SUM(E7:E47)</f>
+        <v>2001</v>
+      </c>
+      <c r="F48" s="16">
+        <f>SUM(F7:F47)</f>
+        <v>620180</v>
+      </c>
+      <c r="G48" s="16">
+        <f>SUM(G7:G47)</f>
+        <v>224414</v>
+      </c>
+      <c r="H48" s="15">
+        <f>AVERAGE(H7:H47)</f>
+        <v>0.38144485024416963</v>
+      </c>
+      <c r="I48" s="16">
+        <f>SUM(I7:I47)</f>
+        <v>364882</v>
+      </c>
+      <c r="J48" s="15">
+        <f>AVERAGE(J7:J47)</f>
+        <v>0.56561101934243863</v>
+      </c>
+      <c r="K48" s="16">
+        <f>SUM(K7:K47)</f>
+        <v>0</v>
+      </c>
+      <c r="L48" s="15"/>
+      <c r="M48" s="16">
+        <f>SUM(M7:M47)</f>
+        <v>0</v>
+      </c>
+      <c r="N48" s="15"/>
+      <c r="O48" s="16">
+        <f>SUM(O7:O47)</f>
+        <v>0</v>
+      </c>
+      <c r="P48" s="15"/>
+      <c r="Q48" s="16">
+        <f>SUM(Q7:Q47)</f>
+        <v>21221</v>
+      </c>
+      <c r="R48" s="15">
+        <f>AVERAGE(R7:R47)</f>
+        <v>3.4246481406655323E-2</v>
+      </c>
+      <c r="S48" s="16">
+        <f>SUM(S7:S47)</f>
+        <v>556</v>
+      </c>
+      <c r="T48" s="15">
+        <f>AVERAGE(T7:T47)</f>
+        <v>4.4084998414208688E-2</v>
+      </c>
+      <c r="U48" s="16">
+        <f>SUM(U7:U47)</f>
+        <v>1396</v>
+      </c>
+      <c r="V48" s="15">
+        <f>AVERAGE(V7:V47)</f>
+        <v>5.2556390568028029E-2</v>
+      </c>
+      <c r="W48" s="16">
+        <f>SUM(W7:W47)</f>
+        <v>5860</v>
+      </c>
+      <c r="X48" s="15">
+        <f>AVERAGE(X7:X47)</f>
+        <v>2.6485640988432327E-2</v>
+      </c>
+      <c r="Y48" s="16">
+        <f>SUM(Y7:Y47)</f>
+        <v>655</v>
+      </c>
+      <c r="Z48" s="15">
+        <f>AVERAGE(Z7:Z47)</f>
+        <v>6.9343604455748198E-3</v>
+      </c>
+      <c r="AA48" s="16">
+        <f>SUM(AA7:AA47)</f>
+        <v>22</v>
+      </c>
+      <c r="AB48" s="15">
+        <f>AVERAGE(AB7:AB47)</f>
+        <v>1.5300090409625148E-3</v>
+      </c>
+      <c r="AC48" s="16">
+        <f>SUM(AC7:AC47)</f>
+        <v>24</v>
+      </c>
+      <c r="AD48" s="15">
+        <f>AVERAGE(AD7:AD47)</f>
+        <v>1.736111111111111E-3</v>
+      </c>
+      <c r="AE48" s="16">
+        <f>SUM(AE7:AE47)</f>
+        <v>143</v>
+      </c>
+      <c r="AF48" s="15">
+        <f>AVERAGE(AF7:AF47)</f>
+        <v>5.3901650035822609E-3</v>
+      </c>
+      <c r="AG48" s="16">
+        <f>SUM(AG7:AG47)</f>
+        <v>55</v>
+      </c>
+      <c r="AH48" s="15">
+        <f>AVERAGE(AH7:AH47)</f>
+        <v>1.1657409312212852E-3</v>
+      </c>
+      <c r="AI48" s="16">
+        <f>SUM(AI7:AI47)</f>
+        <v>268</v>
+      </c>
+      <c r="AJ48" s="15">
+        <f>AVERAGE(AJ7:AJ47)</f>
+        <v>2.9083016820401521E-2</v>
+      </c>
+      <c r="AK48" s="16">
+        <f>SUM(AK7:AK47)</f>
+        <v>84</v>
+      </c>
+      <c r="AL48" s="15">
+        <f>AVERAGE(AL7:AL47)</f>
+        <v>1.6851647393805566E-3</v>
+      </c>
+      <c r="AM48" s="16">
+        <f>SUM(AM7:AM47)</f>
+        <v>37</v>
+      </c>
+      <c r="AN48" s="15">
+        <f>AVERAGE(AN7:AN47)</f>
+        <v>2.5731970234369565E-3</v>
+      </c>
+      <c r="AO48" s="16">
+        <f>SUM(AO7:AO47)</f>
+        <v>38</v>
+      </c>
+      <c r="AP48" s="15">
+        <f>AVERAGE(AP7:AP47)</f>
+        <v>2.6427428889352527E-3</v>
+      </c>
+      <c r="AQ48" s="16">
+        <f>SUM(AQ7:AQ47)</f>
+        <v>478</v>
+      </c>
+      <c r="AR48" s="15">
+        <f>AVERAGE(AR7:AR47)</f>
+        <v>4.4222407253214913E-2</v>
+      </c>
+      <c r="AS48" s="16">
+        <f>SUM(AS7:AS47)</f>
+        <v>47</v>
+      </c>
+      <c r="AT48" s="15">
+        <f>AVERAGE(AT7:AT47)</f>
+        <v>2.9174425822470515E-3</v>
+      </c>
+      <c r="AU48" s="17"/>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B49" s="33"/>
+    </row>
+  </sheetData>
+  <mergeCells count="22">
+    <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AK4:AL4"/>
+    <mergeCell ref="AM4:AN4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AQ4:AR4"/>
+    <mergeCell ref="AS4:AT4"/>
+    <mergeCell ref="Y4:Z4"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="AA4:AB4"/>
+    <mergeCell ref="AC4:AD4"/>
+    <mergeCell ref="AE4:AF4"/>
+    <mergeCell ref="AG4:AH4"/>
+    <mergeCell ref="A1:AV1"/>
+    <mergeCell ref="A2:AV2"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="W4:X4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80A4F573-B339-FF41-B352-70D57E35F1E4}">
   <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>

</xml_diff>